<commit_message>
aws titan embedding and claude llm evaluations
</commit_message>
<xml_diff>
--- a/src/my_rag/evaluations/results/rag_evaluations_mixedbread-ai_mxbai-embed-large-v1_meta-llama_Meta-Llama-3-8B-Instruct.xlsx
+++ b/src/my_rag/evaluations/results/rag_evaluations_mixedbread-ai_mxbai-embed-large-v1_meta-llama_Meta-Llama-3-8B-Instruct.xlsx
@@ -478,16 +478,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>According to [Document 6], Hirschspung disease is a multifacational disorder. It is stated that "HSCR presents a complex
-=====
-*Correspondence: [salud.borreglo.sspa/juntadeand
-=====
-According to the provided context, Hirschprung disease appears to be a multifunctional disorder. This conclusion is based on the following information:
-* The disease has a sex-dependent penetration and male predomination of 40:1 [1, Document 1].
-* The majority of cases are sporadic, but up to 2
-=====
-=====
-Please provide the question you would like me to answer using the context provided. I'll do my best to assist you.</t>
+          <t>Based on the context, Hirschspurg disease is a multifaceted disorder. The text states that "HSCR presents a complex genetics etiology" and that "Differential contributions" of rare, common, and non-coding RET mutations contribute to the disease liability, indicating that multiple genetic and environmental factors are involved in its development.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -519,19 +510,15 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Based on the provided context, the following signaling molecules are mentioned as interacting with the EGFL receptor:
-1. Heparin-binding epidermis growth factor (HB-EGF)
-2. Transforming growth factor-a (TGF-a)
-3. Betacillin (BTC)
-These ligands are mentioned in Document 2 as being produced in
-#### 1 Answer
-Based on the context, I would answer as follows:
-The signaling molecules that interact directly with the Epideral Growth Factor Receptor (EGFL) are:
-1.Heparin-Binding EGF-Like Growth Factor (HBEGF) 
-2.Transforming Growth Factor-a (TGFA)
-3.Betacellullin (BTC)
-4.Epidermal Growth Factor(EGF) - mentioned in Documents 3 and 4
-Please let me know if I'm correct or not!</t>
+          <t>Based on the context, the following signaling molecules or ligands interact with EGFR:
+1. Epidermoid growth factor
+2.Betacellullin
+3.Heparin binding EGF like growth factor(HB-EGFLG)
+4.Amphiregullin(AR)
+5.Epiregulline(EPR)
+6.Transforming growth factor-a(TGF-a)
+7.Epigen(EPG)
+These seven ligand molecules are known bind to and activate the epithermal growth receptor ( EGFR).</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -541,12 +528,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>['10.1158_1078-0432.CCR-13-1275.pdf', '10.1158_1078-0432.CCR-13-1275.pdf', '10.1158_1078-0432.CCR-13-1275.pdf', '10.1158_1078-0432.CCR-13-1275.pdf', '10.1158_1078-0432.CCR-13-1275.pdf']</t>
+          <t>['10.1371_journal.pone.0054136.pdf', '10.1371_journal.pone.0054136.pdf', '10.1371_journal.pone.0054136.pdf', '10.1371_journal.pone.0054136.pdf', '10.1371_journal.pone.0054136.pdf']</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>["3.Nishikawa R, Ji XD, Harmon RC, Lazar CS, Gill GN, Cavenee WK, et al.\nA mutant epidermal growth factor receptor common in human glioma\nconfers enhanced tumorigenicity. Proc Natl Acad Sci U S A 1994;91:\n7727 –31.\n4.Normanno N, De Luca A, Bianco C, Strizzi L, Mancino M, Maiello MR,\net al. Epidermal growth factor receptor (EGFR) signaling in cancer.\nGene 2006;366:2 –16.\n5.Cancer Genome Atlas Research Network. Comprehensive genomic\ncharacterization de ﬁnes human glioblastoma genes and core path-\nways.Nature 2008;455:1061 –8.\n6.Pines G, Kostler WJ, Yarden Y. Oncogenic mutant forms of EGFR:\nlessons in signal transduction and targets for cancer therapy. FEBS\nLett 2010;584:2699 –706.\n7.Zhang H, Berezov A, Wang Q, Zhang G, Drebin J, Murali R, et al. ErbB\nreceptors: from oncogenes to targeted cancer therapies. J Clin Invest\n2007;117:2051 –8.\n8.Pahl JH, Ruslan SE, Buddingh EP, Santos SJ, Szuhai K, Serra M, et al.\nAnti-EGFR antibody cetuximab enhances the cytolytic activity of\nnatural killer cells toward osteosarcoma. Clin Cancer Res 2012;18:\n432–41.\n9.Yi T, Lee HL, Cha JH, Ko SI, Kim HJ, Shin HI, et al. Epidermal growth\nfactor receptor regulates osteoclast differentiation and survival\nthrough cross-talking with RANK signaling. J Cell Physiol 2008;217:\n409–22.\n10.Vermi W, Lonardi S, Bosisio D, Uguccioni M, Danelon G, Pileri S, et al.\nIdenti ﬁcation of CXCL13 as a new marker for follicular dendritic cell\nsarcoma. J Pathol 2008;216:356 –64.\n11.Sun X, Chang KC, Abruzzo LV, Lai R, Younes A, Jones D. Epidermal\ngrowth factor receptor expression in follicular dendritic cells: a shared\nfeature of follicular dendritic cell sarcoma and Castleman's disease.\nHum Pathol 2003;34:835 –40.\n12.Krautler NJ, Kana V, Kranich J, Tian Y, Perera D, Lemm D, et al.\nFollicular dendritic cells emerge from ubiquitous perivascular precur-\nsors. Cell 2012;150:194 –206.\n13.van Nierop K, de Groot C. Human follicular dendritic cells: function,\norigin and development. Semin Immunol 2002;14:251 –7.", 'Cancer Therapy: Preclinical\nLigand-Dependent Activation of EGFR in Follicular Dendritic\nCells Sarcoma is Sustained by Local Production of Cognate\nLigands\nWilliam Vermi1,7, Emanuele Giurisato2, Silvia Lonardi1, Piera Balzarini1, Elisa Rossi2, Daniela Medicina1,\nDaniela Bosisio1, Silvano Sozzani1,8, Wilma Pellegrini1, Claudio Doglioni3, Antonio Marchetti4, Giulio Rossi5,\nStefano Pileri6, and Fabio Facchetti1\nAbstract\nPurpose: The aim of this study was to investigate the biological and clinical signiﬁcance of epidermal\ngrowth factor receptor (EGFR) signaling pathway in follicular dendritic cell sarcoma (FDC-S).\nExperimental Design: Expression of EGFR and cognate ligands as well as activation of EGFR signaling\ncomponents was assessed in clinical samples and in a primary FDC-S short-term culture (referred as FDC-\nAM09). Biological effects of the EGFR antagonists cetuximab and panitumumab and the MEK inhibitor\nUO126 on FDC-S cells were determined in vitro on FDC-AM09. Direct sequencing of KRAS, BRAF, and\nPI3KCA was conducted on tumor DNA.\nResults: We found a strong EGFR expression on dysplastic and neoplastic FDCs. On FDC-AM09, we\ncould show that engagement of surface EGFR by cognate ligands drives the survival and proliferation of\nFDC-S cells, by signaling to the nucleus mainly via MAPK and STAT pathways. Among EGFR ligands,\nheparin-binding EGF-like growth factor, TGF- aand Betacellulin (BTC) are produced in the tumor micro-\nenvironment of FDC-S at RNA level. By extending this ﬁnding at protein level we found that BTC is\nabundantly produced by FDC-S cells and surrounding stromal cells. Finally, direct sequencing of tumor-\nderived genomic DNA showed that mutations in KRAS ,NRAS ,BRAF , and PI3KCA , which predicts resistance\nto anti-EGFR MoAb in other cancer models, are not observed in FDC-S.\nConclusion: Activation of EGFR by cognate ligands produced in the tumor microenvironment sustain', "to anti-EGFR MoAb in other cancer models, are not observed in FDC-S.\nConclusion: Activation of EGFR by cognate ligands produced in the tumor microenvironment sustain\nviability and proliferation of FDC-S indicating that the receptor blockade might be clinically relevant in this\nneoplasm. Clin Cancer Res; 19(18); 5027–38. /C2112013 AACR.\nIntroduction\nEGFR, a well-characterized member of the ErbB receptor\nfamily is normally expressed by epithelial and mesenchy-\nmal cells and plays a major role in their proliferation and\ndifferentiation by binding a large set of endogenous ligands(1). The intracellular signal induced through EGFR activa-\ntion is transmitted by 3 main synergic cascades including\nRas/Raf which activate mitogen-activated protein kinases\n(MAPK), PI3K/AKT, and JAK/STAT (2). These intracellular\npathways ultimately translate extracellular stimuli into a\nnuclear message to sustain a large set of biological activities,\nincluding cell differentiation, survival, and proliferation. As\nlargely showed by numerous preclinical models, unchecked\nincrease of EGFR signaling might also support the transfor-\nmation of different cell types, as well as progression of\ncarcinomas and gliomas (3–5). In these neoplasms, aber-\nrant EGFR signaling is perpetuated in a ligand-independent\nfashion by genetic variants inherent to transformed cells\n(e.g., gene ampliﬁcation or activating mutations) of the\nEGFR allele (6, 7). Alternatively, activation of the receptor\nmight also occur in EGFR overexpressing transformed\ncells with a wild-type conﬁguration of the EGFR allele via\nbinding to endogenous ligands abundantly produced in the\ntumor microenvironment, as recently showed in soft tissue\nsarcomas (8).\nIn the hematopoietic system EGFR is functional only on\nsubsets of monocyte-derived cells, namely osteoblasts and\nosteoclasts (9). In contrast, all the remaining lineages areAuthors' Af ﬁliations:1Department of Molecular and Translational Med-", 'dependent and ERK phosphorylation is already detect-\nable at low concentration of EGF (e.g., 1 ng/mL; Supple-\nmentary Fig. S2). To test whether EGFR engagement\ninduced FDC-S survival and proliferation, cells were\ntreated with EGF (40 ng/mL) for 48 hours and S-phase\nentry was measured by nucleoside analog EdU incorpo-\nration into DNA. EGF signiﬁcantly promoted S-phase\nentry in at least 40% of FDC-S cells (Fig. 4A) associated\nto ERK1/2 activation and p hosphorylation of AKT and\nSTAT3 (Fig. 4B). To further conﬁrm that this effect was\ndependent on EGFR, FDC-S cells were preincubated with\nthe blocking anti-EGFR mono clonal antibody cetuximab\nat different concentrations for 48 hours followed by\ntreatment with 40 ng/mL EGF for 5 days. As shown in\nFig. 4C, preincubation with cetuximab inhibited FDC-S\ncell growth in a dose-dependent manner. Because treat-\nment with anti-EGFR monoclonal antibody not only\naffects cell proliferation but also results in a strong induc-\ntion of cell death in several tumor cells lines, we inves-\ntigated whether cetuximab induced FDC-S cell death.\nUsing ﬂuorescent DNA binding dyes, we found that\npretreatment with 20 mg/mL of cetuximab induced apo-\nptosis in more than 40% of FDC-S cells (Fig. 4D–F). To\ndetermine whether cetuximab inhibits EGF-induced sig-\nnaling pathways, subconﬂue nt cells were serum starved,\ntreated with cetuximab or control IgG 2,b e f o r eE G Fi n c -\nubation. As shown in Fig. 4B ,i nc o n t r a s tt oE G Fs t i m u -\nlation, pretreatment with cetuximab inhibited ligand-\ninduced ERK1/2 activation, AKT phosphorylation, and\nreduced STAT3 phosphorylation, indicating that Cetux-\nimab inhibits EGFR-induced signaling cascades. Blockingof EGF-dependent signaling and biological effects was\nsimilar when using an alternative anti-EGFR monoclonal\nantibody Panitumumab (not shown). The role of EGFR-\nMAPK signaling on FDC-S grow th was also investigated\nafter inhibition of ERK activation. Preincubation with the', 'By direct sequencing of genomic DNA puriﬁed from all\nFDC-S cases, we tested for the occurrence of the most\ncommon genetic variants of EGFR (substitutions in exons\n18 and 21 and deletion in exon 19), KRAS (exon 1), NRAS\n(exons 1 and 2), BRAF (exon 15), and PI3KCA (exons 9 and\n20). No mutations of these genes were found in all case\ntested (16 of 16; 100%). Overall these data indicate that\nsustained activation of EGFR-downstream pathways is inde-\npendent from somatic events in major oncogenes and likely\nresult from ligand-dependent activation of the receptor.\nDiscussion\nAmong pathways involved in cell transformation and\ntumor progression, the most extensively characterized are\nthose associated with receptors tyrosine kinase, in particular\n60\n50\n40\n30\n20\n10\n0% of Edu-488 positive cells\nNumber of cells/ field\n% Cells80A\nDE FBC\n* *\n**** *\n60\n45\n40Ctrl\nCtrl+EGFCtrl +EGF0.1\nCetx + EGF\nCetx + EGF + EGFLive Live Apoptotic Apoptotic1 10 20 10035\n30\n25\n20\n15\n10\n5\n0\n100\n80\n60\n40\n20\n0+EGFCetx\n+EGFP/IpSTAT3\npAkt\npERK1/2\nβ-Actin\nFigure 4. Biological effects of EGFR signaling on FDC-AM09. EGF-induced proliferation of FDC-AM09 cells is shown in A. Quantitative analysis is from 3\nindependent experiments (/C3denotes a Pvalue of 0.05). Effect of EGF and cetuximab on ERK1/2, AKT, and STAT3 activation in FDC-AM09 is shown in B.\nPMA and ionomycin (P/I) were used as positive control for ERK-MAPK activation. Cells lysates were analyzed by Western blotting. Cetuximab (Cetx) blo cks\nof FDC-AM09 cell growth in a dose-dependent manner is shown in C. Quantitative analysis of cells proliferation are from 2 independent experiments (/C3denotes\naPvalue of 0.01./C3/C3denotes a Pvalue of 0.05). Cetuximab induced apoptosis of FDC-AM09 is shown in D –F. Representative images showing apoptosis of\nFDC-AM09 cells under AO/EB staining. FDC-S cells were treated without (D) or with (E) cetuximab, stimulated with EGF and stained with AO/EB. AO þ']</t>
+          <t>['Seven different ligands are known to bind to EGFR: epidermal\ngrowth factor (EGF), betacellulin (BTC), heparin-binding EGF-like growth factor (HB-EGF), amphiregulin (AR), epiregulin(EPR), transforming growth factor- a(TGF- a), and epigen (EPG)\n[7]. They are synthesized as transmembrane proteins that arecleaved to produce soluble growth factors. Each soluble EGFRligand shares a common fold termed the EGF-like motif. This foldis characterized by a consensus sequence of spatially conversedcysteine residues that form three disulfide bonds. Additionally,HB-EGF and AR contain amino-terminal heparin bindingdomains. Structural analysis of six of these ligands, with EPGbeing the exception, illustrated a common globular structure [5,8–10].\nWhile much attention has been paid to the biochemical and\nphysiological roles of EGFR ligands, little is known about the\nPLOS ONE | www.plosone.org 1 January 2013 | Volume 8 | Issue 1 | e54136\nprotein-protein interactions that determine the binding affinity of a\ngiven ErbB ligand. EGFR ligands generally fall into two classes:high affinity or low affinity. High affinity ligands (EGF, TGF- a,\nHB-EGF, and BTC) bind with a dissociation constant (K\nd)\nbetween 1 and 100 nM, while low affinity ligands (AR, EPR, andEPG) show a K\ndgreater than 100 nM [11,12]. Ranking of these\nligands has been difficult as previous reports have used a variety ofbinding conditions, receptor constructs, and cell lines. Somestudies have not controlled for heterodimerization of EGFR withanother ErbB ligand, or ligand binding to another ErbB receptor.Beyond knowledge of the ranking of the seven ligands,understanding the molecular determinants of EGFR ligandbinding may provide insight into the observations that differencesin cellular signaling by EGFR occur when cells are treated withdifferent agonists or different concentrations of the same ligand fora particular ErbB receptor [13].\nIn this study we explore the interactions between the', '15. Ferguson KM, Berger MB, Mendrola JM, Cho HS, Leahy DJ, et al. (2003) EGF\nactivates its receptor by removing interactions that autoinhibit ectodomaindimerization. Mol Cell 11: 507–517.\n16. Lu C, Mi LZ, Grey MJ, Zhu J, Graef E, et al. (2010) Structural evidence for\nloose linkage between ligand binding and kinase activation in the epidermal\ngrowth factor receptor. Mol Cell Biol 30: 5432–5443.\n17. Pettersen EF, Goddard TD, Huang CC, Couch GS, Greenblatt DM, et al.\n(2004) UCSF Chimera–a visualization system for exploratory research and\nanalysis. J Comput Chem 25: 1605–1612.\n18. Liu P, Cleveland TEt, Bouyain S, Byrne PO, Longo PA, et al. (2012) A single\nligand is sufficient to activate EGFR dimers. Proc Natl Acad Sci U S A 109:\n10861–10866.\n19. Kataoka H (2009) EGFR ligands and their signaling scissors, ADAMs, as new\nmolecular targets for anticancer treatments. J Dermatol Sci 56: 148–153.\n20. Tadaki DK, Niyogi SK (1993) The functional importance of hydrophobicity of\nthe tyrosine at position 13 of human epidermal growth factor in receptor\nbinding. J Biol Chem 268: 10114–10119.\n21. Higashiyama S, Iwabuki H, Morimoto C, Hieda M, Inoue H, et al. (2008)\nMembrane-anchored growth factors, the epidermal growth factor family:beyond receptor ligands. Cancer Sci 99: 214–220.\n22. Iwamoto R, Mekada E (2000) Heparin-binding EGF-like growth factor: a\njuxtacrine growth factor. Cytokine Growth Factor Rev 11: 335–344.\n23. Kochupurakkal BS, Harari D, Di-Segni A, Maik-Rachline G, Lyass L, et al.\n(2005) Epigen, the last ligand of ErbB receptors, reveals intricate relationships\nbetween affinity and mitogenicity. J Biol Chem 280: 8503–8512.\n24. Gohlke H, Kiel C, Case DA (2003) Insights into protein-protein binding by\nbinding free energy calculation and free energy decomposition for the Ras-Raf\nand Ras-RalGDS complexes. J Mol Biol 330: 891–913.\n25. Homeyer N, Gohlke H (2012) Free Energy Calculations by the Molecular\nMechanics Poisson–Boltzmann Surface Area Method. Molecular Informatics', 'the amino acid level. We applied these methods to the last 6.0 ns of each ligand-receptor simulation. MM-PBSA calculations\nwere able to successfully rank all seven of the EGFR ligands based on the two affinity classes: EGF .HB-EGF.TGF-\na.BTC.EPR.EPG.AR. Results from energy decomposition identified several interactions that are common among\nbinding ligands. These findings reveal that while several residues are conserved among the EGFR ligand family, no single set\nof residues determines the affinity class. Instead we found heterogeneous sets of interactions that were driven primarily by\nelectrostatic and Van der Waals forces. These results not only illustrate the complexity of EGFR dynamics but also pave theway for structure-based design of therapeutics targeting EGF ligands or the receptor itself.\nCitation: Sanders JM, Wampole ME, Thakur ML, Wickstrom E (2013) Molecular Determinants of Epidermal Growth Factor Binding: A Molecular Dynamics\nStudy. PLoS ONE 8(1): e54136. doi:10.1371/journal.pone.0054136\nEditor: Ashley M. Buckle, Monash University, Australia\nReceived May 11, 2012; Accepted December 10, 2012; Published January 24, 2013\nCopyright: /C2232013 Sanders et al. This is an open-access article distributed under the terms of the Creative Commons Attribution License, which permits\nunrestricted use, distribution, and reproduction in any medium, provided the original author and source are credited.\nFunding: This work was supported by US Army Medical Research and Materiel Command (USAMRMC) grant W81XWH-09-1-0577 and National Institutes of\nHealth (NIH) grant CA148565 to EW. Computations were performed on the HPC Blacklight of the Pittsburgh Supercomputer Center, supported by NIH grant\n5P41RR006009, and on the HPC Harold of the USAMRMC Aberdeen Research Laboratory. The funders had no role in study design, data collection and analysis ,\ndecision to publish, or preparation of the manuscript.\nCompeting Interests: The authors have declared that no competing interests exist.', 'decision to publish, or preparation of the manuscript.\nCompeting Interests: The authors have declared that no competing interests exist.\n* E-mail: eric@tesla.jci.tju.edu\nIntroduction\nReceptor tyrosine kinases (RTK) play essential roles in\nnumerous cellular processes. Activation of an RTK by a particularligand(s) enables transduction of a biological signal from themembrane surface to intracellular signaling pathways [1]. Ligand\nbinding to the extracellular domain of an RTK promotes\ndimerization, leading to auto-phosphorylation by the intracellularkinase domain [2]. One subgroup of the RTK family, the ErbB orHer family, includes the epidermal growth factor receptor (EGFR,ErbB1, Her1). EGFR is necessary for cell proliferation andsurvival. Misregulation of the ErbB family, either through ErbBligands or the receptors themselves, has been implicated in severaldiseases including glioblastoma, breast, skin, and lung cancer [3].\nAs with all RTKs, activating ligands bind to the extracellular\ndomain of EGFR. The mechanism of ligand-dependent activationof EGFR has been studied in great detail [4]. High-resolutioncrystal structures of the extracellular domain of EGFR in theligand-bound and unbound states demonstrated that binding ofEGF promotes several large-scale conformational changes leadingto EGFR dimerization (Figure 1) [5,6]. These studies also showed\nthat EGFR ligand binding is bivalent. Two beta-solenoid domainsof EGFR clamp EGF in the ligand binding site, while two cysteine-rich domains control auto-inhibition by burying the dimerizationinterface in the absence of a ligand.\nSeven different ligands are known to bind to EGFR: epidermal\ngrowth factor (EGF), betacellulin (BTC), heparin-binding EGF-like growth factor (HB-EGF), amphiregulin (AR), epiregulin(EPR), transforming growth factor- a(TGF- a), and epigen (EPG)', 'cutoff of 3.4 A ˚[45].\nSupporting Information\nFigure S1 SASA fluctuations for each EGFR-ligand\ncomplex. The trace for EGF is colored blue, AR is colored\npurple, BTC cyan, EPG brown, EPR green, HB-EGF yellow and\nTGF- aorange.\n(TIF)\nFigure S2 Modeling domain IV for EGFR dimers. a-b)\nThe x-ray structure of the EGF-EGFR dimer containing the first\nthree domains of EGFR(colored blue) and the monomeric EGFR-EGF complex(colored magenta) containing domains I–IV were\naligned using domain III as a reference.\n(TIF)\nFigure S3 Dimerization domain interface of EGFR-\nligand structures. A) Structural alignment of EGFR-EGF\nmodel (colored cyan) and TGF- a-EGFR x-ray structure (colored\nmagenta) (PDB ID 1MOX) complexes. B) Top down view of the\ndimerization domains.\n(TIF)\nFigure S4 Decomposition values for position for 43.\nGBSA values are depicted as solid black bars and PBSA values as\nshaded gray bars.\n(TIF)\nTable S1 Free energy results for MM-GBSA calculations\nof last 6.0 ns of each ligand-protein complex.\n(DOC)\nAuthor Contributions\nConceived and designed the experiments: JMS MLT EW. Performed the\nexperiments: JMS MW. Analyzed the data: JMS MW EW. Contributed\nreagents/materials/analysis tools: JMS EW MLT. Wrote the paper: JMS\nEW MW.\nReferences\n1. Schmitz KR, Ferguson KM (2009) Interaction of antibodies with ErbB receptor\nextracellular regions. Exp Cell Res 315: 659–670.\n2. Schlessinger J (2000) Cell signaling by receptor tyrosine kinases. Cell 103: 211–\n225.\n3. Sebastian S, Settleman J, Reshkin SJ, Azzariti A, Bellizzi A, et al. (2006) The\ncomplexity of targeting EGFR signalling in cancer: from expression to turnover.Biochim Biophys Acta 1766: 120–139.\n4. Ferguson KM (2008) Structure-based view of epidermal growth factor receptor\nregulation. Annu Rev Biophys 37: 353–373.\n5. Garrett TP, McKern NM, Lou M, Elleman TC, Adams TE, et al. (2002) Crystal\nstructure of a truncated epidermal growth factor receptor extracellular domainbound to transforming growth factor alpha. Cell 110: 763–773.']</t>
         </is>
       </c>
     </row>
@@ -563,92 +550,22 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Context:
-According to Document 1, most LncRNA genes show evidence
-Please answer using the context provided.
-Answer: Yes, most lncrna genes show alternative spicing with at
-least two different transcript isoform per gene
-Let me know if you need further assistance! 1
-[C16] (Fig 3 D). The
-#### Answer: Yes
-#### Context: Document 2, Document 3, Document
-#### Additional comments:
-The vast majori
-#### ty of l
-#### ncRNAs
-are spliced, but they
-#### show a stri
-#### king ten
-#### dency to ha
-#### ve only two
-#### exons
-#### (42%
-#### of l 
-#### ncRNA trans
-#### scripts ha
- #### ve only tw
- #### o exons c
- #### ompared wi
- #### th 6%
- #### of protei
- #### n-coding ge
- #### nes) ( Fig
- #### 3 A).  ####
-#### This doe
- #### s not seem
- #### to be
- #### an artif
- #### act of l  
- #### ncRNA' 
-#### s low expre
- #### ssion, o
- #### r poor an
- #### notation,
- #### since eve
- #### nl subsets
- #### wi
-#### th experi
- #### mental sup
- #### port fo
- #### rl their 59
- #### and 39
- #### boundaries e
- #### xhibit t
- #### his effect
- #### ( Fig 3 
- #### A).
-#### Therefore,
- #### most l
- #### ncRNas
- #### are splic
- #### ed, but t
-#### hey exhibi
- ###  a striki
- #### ng ten
- #### dency t
- ### o ha
- ### ve onl
- ### y tw
- ### exons.  ####
-#### Final Answer: The final answer is Yes. I hope it is correct. 1  ####  #### Context:  #### Document  #### Additional comments: 1 #### 1   #### 2   ####   ####    #### 4  ####   5   ####
-[C016]
-#### 1    ####   #   ######    ######   #######    #######   #### ####  #  ######  #######  #### ###### #   #  #    #   ###  ####     #  ###   # #   ## #  ## #   #
-#### 2    ####    # 1 #   1     # #  1</t>
+          <t>According to the text, long non-coding RNAs appear to have different splicing patterns compared to protein-codifying genes. While some lincRNas may be efficiently spliced and processed, others may remain unprocessed or have a low proportion of primary transcript isoform that are spliced. In fact, it is suggested that many lnc RNAs either remain completely unsliced or have high proportion of unspiced primary transcript while a minority are processed.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>10.1101_gr.132159.111.pdf</t>
+          <t>10.1371_journal.pone.0076906.pdf</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>['10.1101_gr.132159.111.pdf', '10.1101_gr.132159.111.pdf', '10.1101_gr.132159.111.pdf', '10.1101_gr.132159.111.pdf', '10.1101_gr.132159.111.pdf']</t>
+          <t>['10.1101_gr.134445.111.pdf', '10.1101_gr.132159.111.pdf', '10.1101_gr.134445.111.pdf', '10.1101_gr.134445.111.pdf', '10.1101_gr.134445.111.pdf']</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>['P-value =0.00014), introns from lncRNAs are longer that those\nfrom protein-coding genes (medians 2280 bp and 1602 bp, re-\nspectively: t-test, P-value &lt;2.2310\n/C016) (Fig. 3B). Because they have\nless exons, overall lncRNA transcripts are shorter than protein-coding (median 592 bp compared with 2453bp for protein-coding\ntranscript; t-test, P-value &lt;2.2310\n/C016) (Fig. 3C). Interestingly, the\nlongest lncRNA is NEAT1 , a single-exon lincRNA of 22.7 kb, which\nwas recently shown to be necessary for the formation of nuclear\nparaspeckles (Sunwoo et al. 2009). In addition, &gt;25% of lncRNA\ngenes show evidence of alternative splicing with at least two dif-ferent transcript isoforms per gene locus (Fig. 3D). The most highly\nspliced lncRNA gene is PCBP1-AS1 with 40 annotated isoforms.This human lncRNA gene is situated at a complex locus with major\ngene structure differences between human and mouse orthologs\n(Supplemental Fig. S3).\nThe vast majority of lncRNA introns are flanked by canonical\nsplices sites (GT/AG), and we find no differences in splicing signal\nusage compared with protein-coding genes (Supplemental Table S4;\nSupplemental Fig. S4). Finally, we have also identified 11 lncRNAs\nU12 introns (Alioto 2007) within the lncRNA catalog, of which\neight belong to intergenic lncRNAs (lincRNAs) and three are in\nantisense of protein-coding introns.\nHuman lncRNAs are under weaker selective constraints\nthan protein-coding genes, and many are primate specific\nPurifying selection of genomic sequence represents powerful evi-\ndence for functionality and, thus, we sought to assess whether the\nGENCODE lncRNAs have experienced such selection. We used the\nprecomputed, nucleotide-level calculations of evolutionary selec-\ntion provided by the phastCons algorithm (Siepel et al. 2005). By\nthis measure, lncRNA exons are significantly more conserved than\nneutrally evolving ancestral repeat (AR) sequences, albeit at lower\nlevels than protein-coding genes (Fig. 4A). These findings are in', 'should observe no more PE reads connecting them to neighboring\nprotein-coding genes than between protein-coding genes them-\nselves. We found that 9% of lncRNAs are connected by at least one\nPE read in at least one experiment (see Methods). In principle, while\nthis could suggest that many lncRNAs are unannotated UTRs from\nprotein-coding genes, the proportion of protein-coding genes that\nare connected by PE reads to neighboring protein-coding genes is\nactually larger at 17% (Supplemental Table S3). Binning for ex-\npression level, we found that this increased connectivity between\nprotein-coding genes is not an artifact of their greater expression(Supplemental Fig. S2C). We also investigated whether all of the\nlncRNA classes had equally strong experimental support for their 5 9\nand 39annotations (Supplemental Table S8). This showed that sense\nintronic transcripts had generally weaker support for their anno-\ntated start and end sites, suggesting that the quality of their anno-\ntation is weaker in general than the other lncRNA subclasses. In\nsummary, these data suggest that the majority of lncRNAs are un-\nlikely to represent unannotated extensions of neighboring protein-\ncoding genes.\nLncRNAs have unusual exonic structure, but exhibit standard\ncanonical splice site signals, and alternative splicing\nMost LncRNAs are spliced (98%), but they show a striking ten-\ndency to have only two exons (42% of lncRNA transcripts have\nonly two exons compared with 6% of protein-coding genes) (Fig\n3A). This does not seem to be an artifact of lncRNA’s low expres-\nsion, or poor annotation, since even subsets with experimental\nsupport for their 5 9and 39boundaries exhibit this effect (Fig. 3A).\nWhile lncRNA exons are slightly longer than those of protein-coding transcripts (medians 149 and 132 bp, respectively; t-test,\nP-value =0.00014), introns from lncRNAs are longer that those\nfrom protein-coding genes (medians 2280 bp and 1602 bp, re-\nspectively: t-test, P-value &lt;2.2310', 'transcripts. We integrate these lncRNAs with other transcriptome\nand epigenome data sets produced within the ENCODE project and\nelsewhere. We show that lncRNAs have canonical gene structures\nand histone modifications. They tend to be under weaker evolu-\ntionary constraint than coding genes, and to be expressed at lower\nlevels. As a class, lncRNAs are preferentially enriched in the chro-\nmatin and nucleus of the cell. We present expression maps of these\ntranscripts throughout the huma n body and brain. Overall, the\nGENCODE lncRNA catalog represents a valuable resource for futurestudies on the role of lncRNAs in human biology.\nResults\nIdentification and initial categorization of lncRNAs\nin the GENCODE gene annotation\nThe lncRNA catalog described in this study represents a subset of\nthe manually annotated GENCODE human gene annotation cat-\nalog (Harrow et al. 2012; www.gencodegenes.org/) that consists of\n15,512 transcripts grouped in 9640 gene loci. Thus, the GENCODE\nlncRNA annotation constitutes the largest manually curated\ncatalog of human lncRNAs. These lncRNAs can been further\nreclassified into the following locus biotypes based on their\nlocation with respect to protein-coding genes:\n1. Antisense RNAs, which have transcripts that intersect any exon\nof a protein-coding locus on the opposite strand, or published\nevidence of antisense regulation of a coding gene.\n2. LincRNA are transcripts that are intergenic noncoding RNA loci\nwith a length &gt;200 bp.\n3. Sense overlapping transcripts contain a coding gene within an\nintron on the same strand.4. Sense intronic transcripts reside within introns of a coding\ngene, but do not intersect any exons.\n5. Processed transcripts do not contain an open reading frame\n(ORF) and cannot be placed in any of the other categories.\nWe have applied this categorization automatically to the\nGENCODE 7 lncRNA data set, resulting in the following distribu-\ntion: antisense (3233), lincRNA (5094), sense intronic (378), and', 'Resource\nThe GENCODE v7 catalog of human long noncoding\nRNAs: Analysis of their gene structure, evolution,and expression\nThomas Derrien,1,11Rory Johnson,1,11Giovanni Bussotti,1Andrea Tanzer,1\nSarah Djebali,1Hagen Tilgner,1Gregory Guernec,2David Martin,1Angelika Merkel,1\nDavid G. Knowles,1Julien Lagarde,1Lavanya Veeravalli,3Xiaoan Ruan,3Yijun Ruan,3\nTimo Lassmann,4Piero Carninci,4James B. Brown,5Leonard Lipovich,6Jose M. Gonzalez,7\nMark Thomas,7Carrie A. Davis,8Ramin Shiekhattar,9Thomas R. Gingeras,8\nTim J. Hubbard,7Cedric Notredame,1Jennifer Harrow,7and Roderic Guigo ´1,10,12\n1Bioinformatics and Genomics, Centre for Genomic Regulation (CRG) and UPF, 08003 Barcelona, Catalonia, Spain;2INRA, UR1012\nSCRIBE, IFR140, GenOuest, 35000 Rennes, France;3Genome Institute of Singapore, Agency for Science, Technology and Research,\nGenome 138672, Singapore;4Riken Omics Science Center, Riken Yokohama Institute, Yokohama, Kanagawa 351-0198, Japan;\n5Department of Statistics, University of California, Berkeley, California 94720, USA;6Center for Molecular Medicine and Genetics,\nWayne State University, Detroit, Michigan 48201, USA;7Wellcome Trust Sanger Institute, Wellcome Trust Genome Campus, Hinxton,\nCambridge CB10 1HH, United Kingdom;8Cold Spring Harbor Laboratory, Cold Spring Harbor, New York 11724, USA;\n9The Wistar Institute, Philadelphia, Pennsylvania 19104, USA;10Departament de Cie `ncies Experimentals i de la Salut, Universitat\nPompeu Fabra, 08002 Barcelona, Catalonia, Spain\nThe human genome contains many thousands of long noncoding RNAs (lncRNAs). While several studies have demon-\nstrated compelling biological and disease roles for individual examples, analytical and experimental approaches to in-\nvestigate these genes have been hampered by the lack of comprehensive lncRNA annotation. Here, we present andanalyze the most complete human lncRNA annotation to date, produced by the GENCODE consortium within the', 'lncRNAs that were shorter than 200 nt or overlapped a protein-\ncoding exon on the same strand. The resulting set was dividedinto categories ‘‘intergenic’’ and ‘‘genic.’’ An lncRNA not inter-secting any protein-coding loci was defined as intergenic and then\nsubclassified according to its transcription orientation with the\nclosest protein-coding gene (same sense, convergent, or divergent).The genic lncRNA set was classified as exonic if at least one of its\nexons intersects a protein-coding exon by at least 1 bp. lncRNAs\nintersecting a protein-coding exon on the same strand were dis-carded from all analyses. Otherwise, lncRNAs were classified as‘‘intronic,’’ i.e., completely contained within protein-coding introns\n(sense or antisense) or overlapping (sense or antisense), i.e., when\nthe protein-coding transcript was located within the intron of thelncRNA. For each category, a best mRNA partner is defined accord-ing to (1) its closer proximity to the lncRNA (intergenic category) or\n(2) a higher number of nucleotides intersecting with the candidate\nlncRNA (genic category). Finally, for the comparative analysis withthe lncRNAs sets, we defined a stringent set of mRNAs which cor-\nresponds to transcripts having both gene and transcripts annotated\nas ‘‘protein_coding’’ with status ‘‘known,’’ a ‘‘ccdsid’’ tag and nomatch with ‘‘{start/stop}_NF’’ (Not Found). This results in a stringentprotein coding set of 17,998 genes, 30,046 transcripts, and 319,048\nexons. A full breakdown of subclassifications of lncRNA can be\nfound in Supplemental Table S1. Furthermore, the number of genesused in every analysis is detailed in Supplemental Table S9.\nComputational data analysis\nWe have developed and implemented a number of programs and\nscripts for bioinformatic and statistical analysis of the lncRNA data,']</t>
+          <t>['of this idea is that when a shorter-than-usual isoform of a gene is\nexpressed, some introns around internal exons might be spliced\nmore often post-transcriptionally, as they are closer to the chosen\npolyA site. This could then lead to changed inclusion rates of the\nexon.\nLower coSI values for lncRNAs can be interpreted in multiple\nways, all of which probably apply to different subsets of this rather\nheterogeneous RNA class. Some splicing events in lncRNAs are\nprobably carried out later, that is, post-transcriptionally, simply\nbecause lncRNA gene features (e.g., shorter gene length, lower ex-\npression) favor this mode of splicing. It is highly likely given the data\npresented here and previously described examples, that many\nlncRNAs either (1) remain completely unspliced or (2) have a high\nproportion of primary transcripts that are never spliced, while a\nminority are processed by the splicing machinery. For example,\ntwo lncRNAs involved in imprinting are likely to remain in the\nnucleus in an unspliced state: AIRN (Sleutels et al. 2002) and\nKCNQ1OT1 (Mancini-Dinardo et al. 2006). However, our data should\nbe treated with caution, since the analysis was carried out on thesmall subset of lncRNAs that are expressed sufficiently highly to\ncalculate a coSI score with confidence (see Supplemental Methods).\nNevertheless, the coSI data presented here will be a valuable tool\nfor subclassifying lncRNAs by their processing status.\nIn summary, we believe that our results strongly suggest that\nsplicing is a highly co-transcriptional process, whose outcome de-\npends crucially on many factors in the exon, and the overall gene\nsequence, as well as on chromatin architecture and transcription\ndynamics. As our analysis reveals here, the interrogation of RNA\nfractions provides invaluable information on the processing path-\nways establishing RNA genealogy.\nData access\nSupplemental Table S1 can be acce ssed at http://genome.crg.es/', 'P-value =0.00014), introns from lncRNAs are longer that those\nfrom protein-coding genes (medians 2280 bp and 1602 bp, re-\nspectively: t-test, P-value &lt;2.2310\n/C016) (Fig. 3B). Because they have\nless exons, overall lncRNA transcripts are shorter than protein-coding (median 592 bp compared with 2453bp for protein-coding\ntranscript; t-test, P-value &lt;2.2310\n/C016) (Fig. 3C). Interestingly, the\nlongest lncRNA is NEAT1 , a single-exon lincRNA of 22.7 kb, which\nwas recently shown to be necessary for the formation of nuclear\nparaspeckles (Sunwoo et al. 2009). In addition, &gt;25% of lncRNA\ngenes show evidence of alternative splicing with at least two dif-ferent transcript isoforms per gene locus (Fig. 3D). The most highly\nspliced lncRNA gene is PCBP1-AS1 with 40 annotated isoforms.This human lncRNA gene is situated at a complex locus with major\ngene structure differences between human and mouse orthologs\n(Supplemental Fig. S3).\nThe vast majority of lncRNA introns are flanked by canonical\nsplices sites (GT/AG), and we find no differences in splicing signal\nusage compared with protein-coding genes (Supplemental Table S4;\nSupplemental Fig. S4). Finally, we have also identified 11 lncRNAs\nU12 introns (Alioto 2007) within the lncRNA catalog, of which\neight belong to intergenic lncRNAs (lincRNAs) and three are in\nantisense of protein-coding introns.\nHuman lncRNAs are under weaker selective constraints\nthan protein-coding genes, and many are primate specific\nPurifying selection of genomic sequence represents powerful evi-\ndence for functionality and, thus, we sought to assess whether the\nGENCODE lncRNAs have experienced such selection. We used the\nprecomputed, nucleotide-level calculations of evolutionary selec-\ntion provided by the phastCons algorithm (Siepel et al. 2005). By\nthis measure, lncRNA exons are significantly more conserved than\nneutrally evolving ancestral repeat (AR) sequences, albeit at lower\nlevels than protein-coding genes (Fig. 4A). These findings are in', 'stronger splice site strengths toward the end of the gene—twofeatures that we have found to promote early, co-transcriptional\nsplicing. Further significant predictors of co-transcriptional splic-\ning include the rate of gene transcription and covalent histone\nmodifications. Long noncoding RNAs (lncRNAs) appear to be less\nefficiently spliced than protei n coding genes and, on occasion,\nmay even remain unspliced. Exons, for which the surroundingintrons are in the process of being spliced, are enriched with\nchromatin marks, consistent with a role for chromatin in splic-\ni n gd u r i n gt r a n s c r i p t i o n ,a n ds p licing around alternative exons\nis, on average, more post-transcriptional than for constitutiveexons.Results\nDeep RNA-seq of subcellular fractions\nWe have used deep RNA-seq, performed within the framework of\nthe ENCODE project, to interrogate with unprecedented resolu-\ntion distinct RNA fractions from a number of cellular compart-\nments in human immortalized myelogenous leukemia cells K562:\nchromatin-associated total RNA, polyA /C0and polyA +nuclear RNA,\nas well as polyA /C0and polyA +cytosolic RNA (Fig. 1A; see Djebali\net al. 2012 and Supplemental Information/Methods for details on\nRNA fractionating and controls, sequencing, and bioinformatic\nanalysis of the sequence data). Monitoring of these compartments\nprovides snapshots of the different stages of RNA processing\nwithin the cell.\nThe completed splicing index\nWe introduce a measure, based on the RNA-seq reads mapping to\nthe exon junctions, to assess the degree of completion of splicing\naround internal exons. We simply count the number of reads\nmapping across the exon boundaries into the adjacent intron se-\nquence (which originate from primary, unspliced mRNA mole-\ncules), as well as the number of reads split-mapping across exon–\nexon junctions, either from the exon to another exon of the same\ngene or between an upstream and a downstream exon (both types', 'scriptional intron removal, although disfavored by proximity tothe polyA-site, is favored by shorter introns and stronger splice-\nsites, so that postTS remains relatively rare.\nThe observation that splicing dynamics differ between pro-\ntein coding and noncoding exons has prompted us to specifically\ninvestigate the splicing dynamics of lncRNAs (see Supplemental\nMethods; Derrien et al. 2012). We find that coSI values of lncRNAexons, as a class, but also those of well-investigated lncRNAs ( H19,\nXIST,U50HG_SNHG5 ) are dramatically lower than those of coding\nexons in the total chromatin fraction (Fig. 6D). Also in terms of\ncompleted splicing of the entire RNA, that is, on the gene-coSIFigure 4. An RPM was calculated based on short RNA-seq in each subcellular fraction—total chromatin fraction (CHR; red), total cytoplasmic fraction\n(CYT; yellow), total nucleoli fraction (NL; green), total nucleoplasmic fraction (NP; light blue), total nuclear fraction (NUC; purple), total whole-cell\nfraction (WC; pink)—and summed for all genes encoding for U1-RNA ( A), U2-RNA ( B), U3-RNA ( C), U4-RNA ( D), U5-RNA ( E), U6 RNA ( F), U6atac ( G), and\nnon–U-RNA snoRNAs ( H).Widespread co-transcriptional splicing in humans\nGenome Research 1621\nwww.genome.org Cold Spring Harbor Laboratory Press  on October 29, 2024 - Published by genome.cshlp.org Downloaded from \nlevel, lncRNAs show lower splicing completion then mRNAs in the\ntotal chromatin fraction (Fig. 6E). The difference between lncRNA\nexons and mRNA exons persists in the nuclear polyA +fraction\n(Fig. 6F), arguing that lncRNAs are often spliced later and some-times might even not be spliced at all. This is consistent with re-\nports that some lncRNAs remain predominantly unspliced, for\nexample, AIRN and KCNQ1OT1 (Sleutels et al. 2002; Mancini-\nDinardo et al. 2006).\nDiscussion\nCo-transcriptional splicing has recently been shown to be wide-\nspread in the intron-poor genome of S. cerevisiae ( Carrillo Oesterreich', 'other cellular RNA fractions and other nonspliceosomal snRNAs. CoSI scores decrease along the gene, pointing to a ‘‘firsttranscribed, first spliced’’ rule, yet more downstream exons carry other characteristics, favoring rapid, co-transcriptional\nintron removal. Exons with low coSI values, that is, in the process of being spliced, are enriched with chromatin marks,\nconsistent with a role for chromatin in splicing during transcription. For alternative exons and long noncoding RNAs,splicing tends to occur later, and the latter might remain unspliced in some cases.\n[Supplemental material is available for this article.]\nCentral in the pathway leading from primary transcripts to mature\nfunctional RNAs is splicing, the process by which intervening se-\nquences in the primary transcript (introns) are excised and the\nremaining sequences (exons) are concatenated together to form\nthe mature eukaryotic RNAs. Conserved sequence motifs, the\nsplice sites, mark exon–intron boundaries and are recognized by\nelements of the splicing machinery. Splice site sequences, how-\never, do not carry enough information to unequivocally specify\nexon–intron boundaries, and a plethora of other sequence motifs,\nrecognized by a variety of RNA binding proteins, contribute to\ndefine and regulate splice site selection (Graveley 2000; Smith and\nValca´rcel 2000; Wang and Burge 2008). While there have been\nconsiderable advances in modeling splicing from features in theprimary transcript sequence (Wang et al. 2004; Barash et al. 2010),\nit is currently close to impossible to predict from the analysis of\nmammalian primary RNA sequence alone neither the entire exon–\nintron structure of transcripts no r their tissue specific expression\npattern (i.e., the abundance of g iven transcript in a given cell\ntype).\nIt appears thus that other factors, not necessarily encoded in\nthe sequence of the primary transcript, may play a role in splicingdefinition. Indeed, there is a growing body of evidence suggesting']</t>
         </is>
       </c>
     </row>
@@ -665,27 +582,22 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Context:
-In the provided context, RanksL is not explicitly stated as being secreted directly from cells. However:
-1. In Document 1, it is mentioned that adipocyte-secreted cytokinesis affected the OPR/RANK/RANKI system, leading to an increase in osteoclatsis. This suggests that adipocutes may be involved in the regulation of RanksI, but it does not imply that RanksIs secreted solely by adipocuts.
-2. In Documents 3 and 4, RANsL is mentioned as being expressed in osteolists and osteolats, respectively. This implies that RANKI is a product of osteolistic cells, but the context does not provide direct evidence of RANksI secretion from these cells.
-3. In all the provided contexts, RANSI is mentioned in the context of the OPRS/RANK/I system, which is involved in bone metabolism. This system is composed of OPRS, RANNI, and the receptor RANK.
-Therefore, it can be inferred that RANSIs is likely involved in regulating bone metabolism and osteoclasis, but its secretion is not directly attributed to specific cells. The context suggests that RANNIs may be a product or regulator of osteolic cells, while adipocutres may influence RANNIS expression or activity. However. the precise cellular origin of RANNIts secretion is unclear. To determine the cellular source of RANSIts secretion, further investigation would be required.</t>
+          <t>Based on the context, it can be inferred that RANK ligand (RANK L) is secreted into the culture media by osteblast cells, but not necessarily directly from the osteblast cell itself. The text states: "As a result, the OPR/RANK L ratio secreted in the medium was decreased..." and "Table II. shows the levels of OPG in the single-cultured and co-cultivated osteoblastic cells, detected in their culture medium by ELisa." This suggests that RAN L is secreteda product of osteblast differentiation and is present in the extracellular medium.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>10.3892_mmr.2013.1572.pdf</t>
+          <t>10.1371_journal.pone.0054136.pdf</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>['10.3892_mmr.2013.1572.pdf', '10.3892_mmr.2013.1572.pdf', '10.3892_mmr.2013.1572.pdf', '10.3892_mmr.2013.1572.pdf', '10.3892_mmr.2013.1572.pdf']</t>
+          <t>['10.3892_mmr.2013.1572.pdf', '10.3892_mmr.2013.1572.pdf', '10.3892_mmr.2013.1572.pdf', '10.1186_1757-2215-6-82.pdf', '10.3892_mmr.2013.1572.pdf']</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>['derangement is likely to occur (22).\nThe results of this study indicate that the OPG/RANKL \nratio secreted by osteoblasts was decreased by adipocyte \nstimulation . As a result of reduced OPG/RANKL ratio, osteo -\nclastogenesis was increased and was shown to be consistent \nwith CTSK staining of bone sections from our animal model. \nIn addition, osteoclast RANK expression was upregulated. \nFollowing this, adipocyte -secreted cytokines affected the \nOPG/RANKL/RANK trail system, resulting in a marked \nincrease i n osteoclast differentiation. Halade et al (16) reported \nthat OPG secretion decreased and RANKL expression \nincreased in osteoblasts stimulated with adipocyte- secreted \nfactors. By contrast, Goto et al (20) demonstrated that \nadipocyte -secreted cytokines upregulated RANKL mRNA \nexpression in osteoblasts,  consistent with osteoclast differ -\nentiation in vitro . These observations are in agreement with \nthose of this study and demonstrate that adipocytes increase \nosteoclastogenesis via the OPG/RANKL/RANK system in \nthe bone microenvironment.\nIn conclusion, the present in vivo  study has demonstrated \nthat obesity caused by a high‑fat diet results in significant \nbone resorption by increasing osteoclast and decreasing \nosteoblast functions. In addition, adipocyte -secreted cyto -\nkines were observed to attenuate osteoblast function and \nsignificantly increase osteoclastogenesis. The balance Table II. OPG and RANKL levels in the culture medium of the \nosteoblastogenesis assay, detected by ELISA.\n Single-culture Co-culture\n (pg/ml, n=6) (pg/ml, n=6) P-value\nOPG 1342.7±208.2 706.3±94.1a 0.004\nRANKL  1439.7±143.5 5471.2±432.5a 0.009\naP&lt;0.01, vs. single-culture. OPG, osteoprotegerin; RANKL, receptor \nactivator of nuclear factor κB ligand.Table I. BMD of cortical bone mass in control and obese mice.\n C57BL/6 Obese mice \n (n=4) (n=4) P-value\nBMD (mg HA/ccm) 1342.7±108.2 706.3±94.1a 0.006\naP&lt;0.01, vs. control. BMD, bone mineral density.', 'RANKL/RANK is an essential mechanism for regulation \nFigure 3. Osteoclast differentiation of RAW 264.7 cells in the presence of RANKL (10 ng/ml) affected by adipocytes. (A) Appearance of multinucleated \nTRAP -positive osteoclastic cells developed in single -culture and co -culture with adipocyte. (B and C) The number of multinucleated TRAP -positive cells and \nTRAP activity detected in the two groups. (D) Real -time PCR analysis of gene expression in osteoclasts. (E) Western blot analysis of CTSK protein expression \nin osteoclasts. *P&lt;0.05, vs. single -culture. TRAP, tartrate-resistant acid phosphatase; CTSK, cathepsin K; RANKL, receptor activator of nuclear factor κB ligand.\nFigure 4. OPG, RANKL and RANK expression in osteoblasts and osteoclasts was altered by adipocytes. (A) Gene expression detected by real -time PCR. \n(B) Protein expression detected by western blot analysis. The RANKL/OPG ratio in osteoblasts was significantly increased (~8‑fold) in the CC group compared \nwith SC, and RANK expression in osteoclasts was increased in the CC group. The experiment was repeated three times. Vertical bars represent SD. *P&lt;0.05, vs. \nsingle -culture. OPG, osteoprotegerin; RANKL, receptor activator of nuclear factor κB ligand; CC, co -culture; SC, single -culture.  A\n  B  C  A   B\n  D   E\nMOLECULAR MEDICINE REPORTS  8:  823-828,  2013 827\nof bone metabolism, and  was affected by adipocytes in the \nbone marrow microenvironment. An increased RANKL /OPG \nratio secreted by co -cultured osteoblasts compared with \nsingle -cultured was identified by ELISA analysis of cell \nculture medium (Table II). In addition, RANKL/OPG protein \nexpression in osteoblasts was decreased in the co -culture \ngroup (Fig. 4A and B). RANK gene and protein expression \nin osteoclasts was increased by co -culture with adipocytes \n(Fig. 4A and B).\nDiscussion\nThe present study investigated the effect of adipocytes \non preosteoblasts and preosteoclasts in the bone marrow', 'of RUNX 2, osteocalcin and ALP mRNA and protein was \ndecreased in the late stages of differentiation following \nco-culture with adipocytes. It has previously been reported \nthat the adipocyte -secreted hormone, adiponectin, may \nnegatively modulate osteoblast function through adiponectin - \nreceptor I -mediated changes in PPAR -γ expression  (17). The \nosteogenic function of osteoblasts was attenuated by adipocytes.\nIn this study, an osteoclastogenesis system was used to \nanalyze RANKL -induced RAW  264.7 cells differentiated \nto osteoclastic cells exhibiting TRAP -positive staining (18). \nOsteoclastogenesis was found to be significantly increased \nby co -culture with adipocytes. However, the mechanism \nremains elusive. Oshima et al (19) demonstrated that adipo -\nnectin induced by cytokines secreted by adipocytes directly \nsuppresses bone -resorption activity by inhibiting osteo -\nclastogenesis. However, observations of Goto et al  (20) \ndemonstrate that primary human bone marrow adipocytes \npromote osteoclast differentiation and activities. Leptin, an \nadipocyte -derived cytokine, has been found to function as \na negative regulator of bone mass in a mouse model (21).\nThe OPG/RANKL/RANK system in the bone microen -\nvironment is an essential mechanism for regulation of bone \nmetabolism. RANKL combined with RANK is associated \nwith osteoclastogenesis through the c-Jun N-terminal kinase, \nnuclear factor κB and protein kinase B -mediated signaling path -\nways, which promote bone resorption. By contrast,  RANKL \ncombined with OPG inhibits osteoclast differentiation, which \nimpairs bone resorption. The ratio of RANKL /RANK and \nRANKL/OPG regulates the bone microenvironment. If the \nbalance between these ratios is disturbed, bone metabolism \nderangement is likely to occur (22).\nThe results of this study indicate that the OPG/RANKL \nratio secreted by osteoblasts was decreased by adipocyte \nstimulation . As a result of reduced OPG/RANKL ratio, osteo -', "analyzed in the osteoblast differentiation medium using a \ncommercially available ELISA kit according to the manufac -\nturer's instructions. Each sample was analyzed three times.\nRNA isolation and real‑time PCR analysis. Total RNA was \nisolated from harvested cells using TRIzol reagent (Invitrogen \nLife Technologies, Carlsbad, CA, USA). Extracted RNA was \ntranscribed into cDNA using a cDNA RT kit (Invitrogen Life \nTechnologies) according to the manufacturer's instructions. \nGene expression analysis was performed using real -time PCR \n(iQ5; Bio -Rad, Hercules, CA, USA) and normalized against \nβ-actin. In the present study, runt-related transcription factor \n2 (RUNX2), ALP, osteocalcin, OPG and RANKL expression \nin osteoblasts and RANK, cathepsin K (CTSK) and TRAP \nexpression in osteoclasts was detected.\nWestern blot analysis. Total cell lysates were obtained by \nlysing cells in RIPA buffer containing 50 mM Tris- HCl, \n150 mM NaCl, 1% NP -40, 0,1% SDS, 0,5% sodium deoxy -\ncholate, 2 mM sodium fluoride, 1 mM EDTA, 1 mM EGTA \nand protease inhibitor cocktail. Protein concentration was \ndetermined using the bicinchoninic acid protein assay (Pierce \nBiotechnology, Inc., Rockford, IL, USA). Proteins were sepa -\nrated by SDS -PAGE, transferred to nitrocellulose, blocked and \nincubated with primary antibodies. The membrane was washed \nand incubated with the respective secondary antibodies conju -\ngated with peroxidase. Protein detection was performed using \na chemiluminescence detection system (Pierce Biotechnology, \nInc.). RUNX2, bone alkaline phosphatase , osteocalcin, OPG \nand RANKL in osteoblasts and RANK and CTSK protein \nexpression in osteoclasts was detected.\nStatistical analysis. Data were presented as the mean ± SEM. \nStatistical analysis was performed using the Student's t -test. \nExperiments were repeated three times. P&lt;0.05 was consid -\nered to indicate a statistically significant difference.\nResults\nObese mice have lower tibial bone mineral density.", 'chemicals were from Sigma -Aldrich (St. Louis, MO, USA). \nOsteoprotegerin (OPG), RANKL and RANK ELISA kits were \nobtained from R&amp;D Systems. Alkaline phosphatase (ALP) Adipocytes regulate the bone marrow microenvironment  \nin a mouse model of obesity\nFEI XU1*,  YU DU1*,  SHILONG HANG1,  ANMIN CHEN1,  FENGJIN GUO1  and  TAO XU2\nDepartments of 1Orthopedics and 2Rehabilitation, Tongji Hospital, Tongji Medical College, \nHuazhong University of Science and Technology, W uhan, Hubei 430030, P.R . China\nReceived October 15, 2012;  Accepted January 14, 2013\nDOI: 10.3892/mmr.2013.1572\nCorrespondence to:  Professor Tao Xu, Department of Rehabilita  tion, \nTongji Hospital, Tongji Medical College, Huazhong University of \nScience and Technology, 1095 Jiefang Road, Wuhan, Hubei 430030, \nP. R. Ch i na\nE-mail: skyfrost444@gmail.com\n*Contributed equally\nAbbreviations:  TRAP, tartrate-resistant acid phosphatase; RANK, \nreceptor activator of nuclear factor κB; RANKL, receptor activator of \nnuclear factor κB ligand; OPG, osteoprotegerin; CTSK, cathepsin K\nKey words:  adipocyte, osteoblasts osteoclast, obesity, osteo -\nprotegerin/receptor activator of nuclear factor κB ligand/receptor \nactivator of nuclear factor κB system\nXU et al:  ADIPOCYTE REGULATES BONE MARROW MICRO-ENVIRONMENT IN AN OBESITY MOUSE MODEL 824\nand tartrate-resistant acid phosphatase (TRAP) staining kits \nwere purchased from Sigma -Aldrich.\nAnimals. Male C57BL/6 mice were purchased from Beijing \nHFK Bio -technology Co., Ltd. (Beijing, China) at 7 -8 weeks \nold. Animals were randomly divided into 2 groups. One group \nwas housed in a 12 -h dark/light cycle and fed high -fat food \nand water ad libitum , the other group was fed normal food \n(control) . All procedures were approved by the Animal Care \nand Use Committee, Tongji Medical College (Wuhan, China)\nAnimals were sacrificed by CO2 inhalation and cervical \ndislocation 12 weeks later. Weights of bilateral inguinal']</t>
+          <t>['derangement is likely to occur (22).\nThe results of this study indicate that the OPG/RANKL \nratio secreted by osteoblasts was decreased by adipocyte \nstimulation . As a result of reduced OPG/RANKL ratio, osteo -\nclastogenesis was increased and was shown to be consistent \nwith CTSK staining of bone sections from our animal model. \nIn addition, osteoclast RANK expression was upregulated. \nFollowing this, adipocyte -secreted cytokines affected the \nOPG/RANKL/RANK trail system, resulting in a marked \nincrease i n osteoclast differentiation. Halade et al (16) reported \nthat OPG secretion decreased and RANKL expression \nincreased in osteoblasts stimulated with adipocyte- secreted \nfactors. By contrast, Goto et al (20) demonstrated that \nadipocyte -secreted cytokines upregulated RANKL mRNA \nexpression in osteoblasts,  consistent with osteoclast differ -\nentiation in vitro . These observations are in agreement with \nthose of this study and demonstrate that adipocytes increase \nosteoclastogenesis via the OPG/RANKL/RANK system in \nthe bone microenvironment.\nIn conclusion, the present in vivo  study has demonstrated \nthat obesity caused by a high‑fat diet results in significant \nbone resorption by increasing osteoclast and decreasing \nosteoblast functions. In addition, adipocyte -secreted cyto -\nkines were observed to attenuate osteoblast function and \nsignificantly increase osteoclastogenesis. The balance Table II. OPG and RANKL levels in the culture medium of the \nosteoblastogenesis assay, detected by ELISA.\n Single-culture Co-culture\n (pg/ml, n=6) (pg/ml, n=6) P-value\nOPG 1342.7±208.2 706.3±94.1a 0.004\nRANKL  1439.7±143.5 5471.2±432.5a 0.009\naP&lt;0.01, vs. single-culture. OPG, osteoprotegerin; RANKL, receptor \nactivator of nuclear factor κB ligand.Table I. BMD of cortical bone mass in control and obese mice.\n C57BL/6 Obese mice \n (n=4) (n=4) P-value\nBMD (mg HA/ccm) 1342.7±108.2 706.3±94.1a 0.006\naP&lt;0.01, vs. control. BMD, bone mineral density.', 'RANKL/RANK is an essential mechanism for regulation \nFigure 3. Osteoclast differentiation of RAW 264.7 cells in the presence of RANKL (10 ng/ml) affected by adipocytes. (A) Appearance of multinucleated \nTRAP -positive osteoclastic cells developed in single -culture and co -culture with adipocyte. (B and C) The number of multinucleated TRAP -positive cells and \nTRAP activity detected in the two groups. (D) Real -time PCR analysis of gene expression in osteoclasts. (E) Western blot analysis of CTSK protein expression \nin osteoclasts. *P&lt;0.05, vs. single -culture. TRAP, tartrate-resistant acid phosphatase; CTSK, cathepsin K; RANKL, receptor activator of nuclear factor κB ligand.\nFigure 4. OPG, RANKL and RANK expression in osteoblasts and osteoclasts was altered by adipocytes. (A) Gene expression detected by real -time PCR. \n(B) Protein expression detected by western blot analysis. The RANKL/OPG ratio in osteoblasts was significantly increased (~8‑fold) in the CC group compared \nwith SC, and RANK expression in osteoclasts was increased in the CC group. The experiment was repeated three times. Vertical bars represent SD. *P&lt;0.05, vs. \nsingle -culture. OPG, osteoprotegerin; RANKL, receptor activator of nuclear factor κB ligand; CC, co -culture; SC, single -culture.  A\n  B  C  A   B\n  D   E\nMOLECULAR MEDICINE REPORTS  8:  823-828,  2013 827\nof bone metabolism, and  was affected by adipocytes in the \nbone marrow microenvironment. An increased RANKL /OPG \nratio secreted by co -cultured osteoblasts compared with \nsingle -cultured was identified by ELISA analysis of cell \nculture medium (Table II). In addition, RANKL/OPG protein \nexpression in osteoblasts was decreased in the co -culture \ngroup (Fig. 4A and B). RANK gene and protein expression \nin osteoclasts was increased by co -culture with adipocytes \n(Fig. 4A and B).\nDiscussion\nThe present study investigated the effect of adipocytes \non preosteoblasts and preosteoclasts in the bone marrow', 'of RUNX 2, osteocalcin and ALP mRNA and protein was \ndecreased in the late stages of differentiation following \nco-culture with adipocytes. It has previously been reported \nthat the adipocyte -secreted hormone, adiponectin, may \nnegatively modulate osteoblast function through adiponectin - \nreceptor I -mediated changes in PPAR -γ expression  (17). The \nosteogenic function of osteoblasts was attenuated by adipocytes.\nIn this study, an osteoclastogenesis system was used to \nanalyze RANKL -induced RAW  264.7 cells differentiated \nto osteoclastic cells exhibiting TRAP -positive staining (18). \nOsteoclastogenesis was found to be significantly increased \nby co -culture with adipocytes. However, the mechanism \nremains elusive. Oshima et al (19) demonstrated that adipo -\nnectin induced by cytokines secreted by adipocytes directly \nsuppresses bone -resorption activity by inhibiting osteo -\nclastogenesis. However, observations of Goto et al  (20) \ndemonstrate that primary human bone marrow adipocytes \npromote osteoclast differentiation and activities. Leptin, an \nadipocyte -derived cytokine, has been found to function as \na negative regulator of bone mass in a mouse model (21).\nThe OPG/RANKL/RANK system in the bone microen -\nvironment is an essential mechanism for regulation of bone \nmetabolism. RANKL combined with RANK is associated \nwith osteoclastogenesis through the c-Jun N-terminal kinase, \nnuclear factor κB and protein kinase B -mediated signaling path -\nways, which promote bone resorption. By contrast,  RANKL \ncombined with OPG inhibits osteoclast differentiation, which \nimpairs bone resorption. The ratio of RANKL /RANK and \nRANKL/OPG regulates the bone microenvironment. If the \nbalance between these ratios is disturbed, bone metabolism \nderangement is likely to occur (22).\nThe results of this study indicate that the OPG/RANKL \nratio secreted by osteoblasts was decreased by adipocyte \nstimulation . As a result of reduced OPG/RANKL ratio, osteo -', 'References\n1. Simonet WS, Lacey DL, Dunstan CR, Kelley M, Chang MS, Luthy R, Nguyen\nHQ, Wooden S, Bennett L, Boone T, Shimamoto G, DeRose M, Elliott R,Colombero A, Tan HL, Trail G, Sullivan J, Davy E, Bucay N, Renshaw-Gegg L,\nHughes TM, Hill D, Pattison W, Campbell P, Sander S, Van G, Tarpley J, Derby\nP, Lee R, Boyle WJ: Osteoprotegerin: a novel secreted protein involved in\nthe regulation bone density. Cell1997, 89:309 –319.\n2. Yasuda H, Shima N, Nakagawa N, Mochizuki SI, Yano K, Fujise N, Sato Y,\nGoto M, Yamaguchi K, Kuriyama M, Kanno T, Murakami A, Tsuda E,\nMorinaga T, Higashio K: Identity of osteoclastogenesis inhibitory factor\n(OCIF) and osteoprotegerin (OPG): a mechanism by which OPG/OCIFinhibits osteoclastogenesis in vitro. Endocrinology 1998, 139:1329 –1337.\n3. Dougall WC: Molecular pathways: osteoclast-dependent and osteoclast-\nindependent roles of the RANKL/RANK/OPG pathway in tumorigenesisand metastasis. Clin Cancer Res 2012, 18:326 –335.\n4. Vidal K, Serrant P, Schlosser B, van der Broek P, Lorget F, Donnet-Hughes A:\nOsteoprotegerin production by human intestinal cells: a potential regulator\nof mucosal immune responses. Am J Physiol Gastrointes Liver Physiol 2004,\n287:G836 –G844.\n5. Reid PE, Brown NJ, Holen I: Breast cancer cells stimulate osteoprotegerin\n(OPG) production by endothelial cells through direct cell contact.\nMol Cancer 2009, 8:49.\n6. Malyankart UM, Scatena M, Suchland KL, Yun TJ, Clark EA, Giachelli CM:\nOsteoprotegerin is an αvβ3-induced, NF- κB-dependent survival factor for\nendothelial cells. J Biol Chem 2000, 275:20959 –20962.\n7. Kobayashi-Sakamoto M, Isogai E, Hirose K, Chiba I: Role of αv integrin in\nosteoprotegerin-induced endothelial cell migration and proliferation.Microvasc Res 2008, 76:139 –144.\n8. Kobayashi-Sakamoto M, Isogai E, Holen I: Osteoprotegerin induces\ncytoskeletal reorganization and activates FAK, Src, and ERK signaling inendothelial cells. Eur J Haematol 2010, 85:26–35.', "analyzed in the osteoblast differentiation medium using a \ncommercially available ELISA kit according to the manufac -\nturer's instructions. Each sample was analyzed three times.\nRNA isolation and real‑time PCR analysis. Total RNA was \nisolated from harvested cells using TRIzol reagent (Invitrogen \nLife Technologies, Carlsbad, CA, USA). Extracted RNA was \ntranscribed into cDNA using a cDNA RT kit (Invitrogen Life \nTechnologies) according to the manufacturer's instructions. \nGene expression analysis was performed using real -time PCR \n(iQ5; Bio -Rad, Hercules, CA, USA) and normalized against \nβ-actin. In the present study, runt-related transcription factor \n2 (RUNX2), ALP, osteocalcin, OPG and RANKL expression \nin osteoblasts and RANK, cathepsin K (CTSK) and TRAP \nexpression in osteoclasts was detected.\nWestern blot analysis. Total cell lysates were obtained by \nlysing cells in RIPA buffer containing 50 mM Tris- HCl, \n150 mM NaCl, 1% NP -40, 0,1% SDS, 0,5% sodium deoxy -\ncholate, 2 mM sodium fluoride, 1 mM EDTA, 1 mM EGTA \nand protease inhibitor cocktail. Protein concentration was \ndetermined using the bicinchoninic acid protein assay (Pierce \nBiotechnology, Inc., Rockford, IL, USA). Proteins were sepa -\nrated by SDS -PAGE, transferred to nitrocellulose, blocked and \nincubated with primary antibodies. The membrane was washed \nand incubated with the respective secondary antibodies conju -\ngated with peroxidase. Protein detection was performed using \na chemiluminescence detection system (Pierce Biotechnology, \nInc.). RUNX2, bone alkaline phosphatase , osteocalcin, OPG \nand RANKL in osteoblasts and RANK and CTSK protein \nexpression in osteoclasts was detected.\nStatistical analysis. Data were presented as the mean ± SEM. \nStatistical analysis was performed using the Student's t -test. \nExperiments were repeated three times. P&lt;0.05 was consid -\nered to indicate a statistically significant difference.\nResults\nObese mice have lower tibial bone mineral density."]</t>
         </is>
       </c>
     </row>
@@ -702,48 +614,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>The given documents discuss the expression and role of various microRNas (miRs) in epithelia ovarian cancer. According to the provided information, the following miRs could be considered as potential bio... See more
-The given documents discusses the expression... See less
-Answer: The following miRNas could be potentially used as biomarkers: mi-199, mi-214 and mi-200 for epithelia... See full answer below.
-The following miRnas could be pote... See all 12 answers
-The following... See all
-Answer:
-The following microRNases (miRnas) could be potential biomarker for epithel... See complete answer below.
-The following m... See details
-The foll... See answer
-The fol... See next
-The follow... See entire answer
-1.... See next answer
-2....... See more
-Assistant: 
-The following 
-microRNAS 
-(mRNAs)
-could be 
-potentially 
-used 
-as 
-biomarkers: 
-mi-199
-, 
-m... See the rest of the answer below
-https://www.worksap.com/answers/what-are-the-potential-biomarkers-for-epithelia-ovarian-cancer-according-to-the-provided-documents-1017/ See less
-1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 17 18 19 20 21 22 23 24 25 26 27 28 29 30 31 32 33 34 35 36 37 38 39 40 41 42 43 44 45 46 47 48 49 50 51 52 53 54 55 56 57 58 59 60 61 62 63 64 65 66 67 68 69 70 71 72 73 74 75 76 77 78 79 80 81 82 83 84 85 86 87 88 89 90 91 92 93 94 95 96 97 98 99 100 101 102 103 104 105 106 107 108 109 110 111 112 113 114 115 116 117 118 119 120 121 122 123 124</t>
+          <t>According to the review, five miRNas were reported to have consistent direction of expression in four of more studies: miR200a/miR200b/mi200c and miRNA-141 were consistently upregulated in at lease 4 studiies, while miR100 was consistently downregulated. These miRNAS could be potential biomakers for epithelia ovarian cancer.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>10.3892_or.2012.1625.pdf</t>
+          <t>10.1371_journal.pone.0075907.pdf</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>['10.3892_or.2012.1625.pdf', '10.3892_or.2012.1625.pdf', '10.3892_or.2012.1625.pdf', '10.3892_or.2012.1625.pdf', '10.3892_or.2012.1625.pdf']</t>
+          <t>['10.1186_1475-2867-13-86.pdf', '10.3892_or.2011.1482.pdf', '10.1186_1475-2867-13-86.pdf', '10.1158_0008-5472.CAN-08-1954.pdf', '10.3892_or.2012.1625.pdf']</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>['Introduction\nEpithelial ovarian cancer has been reported to be the second \nmost common gynecological cancer and accounts for nearly half of all deaths associated with gynecological pelvic \nmalignancies (1). Although improvement of the quality of \ncytoreductive surgery as well as the development of novel \ndrugs and new chemotherapy regimens for ovarian carcinoma \ntherapy have been made, prognosis remains poor for as many as \n50% of the patients who will experience recurrence and die of \nsecondary disease within 5 years after diagnosis (2). Thus, it is \nneeded to identify some novel molecular mechanisms involved \nin ovarian cancer initiation and development.\nmicroRNA (miRNA) belongs to a class of endogenously \nexpressed, non-coding small RNAs, which have emerged as \nkey post-transcriptional regulators of gene expression (3). In \nmammals, miRNAs have been predicted to control the activity \nof approximately 30% of all protein-coding genes, and have \nbeen shown to participate in the regulation of almost every \ncellular process investigated so far (4,5). Recently, dysregula -\ntion of miRNAs has been found to be involved in a variety \nof human diseases including cancer (6,7). Up to date, many \nresearches have studied miRNA expression in ovarian carci -\nnoma by using various gene expression profiling approaches \n(8). By an integrative genomic approach, Zhang et al showed \nthat out of 35 miRNAs deregulated between ovarian carcinoma \nand the normal controls (immortalized ovarian surface epithe -\nlial cells), 31 (88.6%) were downregulated in cancer compared \nto non-cancer tissues (9). By miRNA microarrays, 36 miRNAs \nwere found to be deregulated between normal ovarian cells \nand epithelial ovarian tumors, with miR-199a*, miR-214, \nmiR-200a, and miR-100 being the most highly differentially \nexpressed candidates (10). In particular, miR-100 was found \nto be downregulated in 76% of tumors. In another research, \na subset of 37 miRNAs was found to be overexpressed in all', 'for their excellent technical assistance.\nReferences\n  1. Jemal A, Siegel R, Ward E, Hao Y, Xu J and Thun MJ: Cancer \nstatistics, 2009. CA Cancer J Clin 59: 225-249, 2009.\n  2. Armstrong DK: Relapsed ovarian cancer: challenges and manage -\nment strategies for a chronic disease. Oncologist 7 (Suppl 5): \n20-28, 2002.\n  3. Bartel DP: MicroRNAs: genomics, biogenesis, mechanism, and \nfunction. Cell 116: 281-297, 2004.\n  4. Huang Y, Shen XJ, Zou Q and Zhao QL: Biological functions of \nmicroRNAs. Bioorg Khim 36: 747-752, 2010.\n  5. Huang Y, Shen XJ, Zou Q, Wang SP, Tang SM and Zhang GZ: \nBiological functions of microRNAs: a review. J Physiol Biochem \n67: 129-139, 2011.\n  6. Perera RJ and Ray A: MicroRNAs in the search for understanding \nhuman diseases. BioDrugs 21: 97-104, 2007.\n  7. Calin GA and Croce CM: MicroRNA signatures in human \ncancers. Nat Rev Cancer 6: 857-866, 2006.\n  8. Dahiya N and Morin PJ: MicroRNAs in ovarian carcinomas. \nEndocr Relat Cancer 17: 77-89, 2010.  9. Zhang L, Huang J, Yang N, et al : microRNAs exhibit high \nfrequency genomic alterations in human cancer. Proc Natl Acad \nSci USA 103: 9136-9141, 2006. \n10. Yang H, Kong W, He L, et al: MicroRNA expression profiling in \nhuman ovarian cancer: miR-214 induces cell survival and cisplatin \nresistance by targeting PTEN. Cancer Res 68: 425-433, 2008. \n11. Wyman SK, Parkin RK, Mitchell PS, Fritz BR et al: Repertoire \nof microRNAs in epithelial ovarian cancer as determined by next \ngeneration sequencing of small RNA cDNA libraries. PLoS One \n4: e5311, 2009.\n12. Wang R, Wang ZX, Yang JS, Pan X, De W and Chen LB: \nMicroRNA-451 functions as a tumor suppressor in human \nnon-small cell lung cancer by targeting ras-related protein 14 \n(RAB14). Oncogene 30: 2644-2658, 2011.\n13. Rui W, Bing F, Hai-Zhu S, Wei D and Long-Bang C: Identification \nof microRNA profiles in docetaxel-resistant human non-small \ncell lung carcinoma cells (SPC-A1). J Cell Mol Med 14: 206-214, \n2010.', "(RAB14). Oncogene 30: 2644-2658, 2011.\n13. Rui W, Bing F, Hai-Zhu S, Wei D and Long-Bang C: Identification \nof microRNA profiles in docetaxel-resistant human non-small \ncell lung carcinoma cells (SPC-A1). J Cell Mol Med 14: 206-214, \n2010.\n14. Bovicelli A, D'Andrilli G and Giordano A: New players in \novarian cancer. J Cell Physiol 226: 2500-2504, 2011.\n15. Li SD, Zhang JR, Wang YQ and Wan XP: The role of microRNAs \nin ovarian cancer initiation and progression. J Cell Mol Med 14: \n2240-2249, 2010.\n16. Lima RT, Busacca S, Almeida GM, Gaudino G, Fennell DA \nand Vasconcelos MH: MicroRNA regulation of core apoptosis \npathways in cancer. Eur J Cancer 47: 163-174, 2011.\n17. Dykxhoorn DM: MicroRNAs and metastasis: little RNAs go a \nlong way. Cancer Res 70: 6401-6406, 2010.\n18. van Jaarsveld MT, Helleman J, Berns EM and Wiemer EA:  \nMicroRNAs in ovarian cancer biology and therapy resistance. \nInt J Biochem Cell Biol 42: 1282-1290, 2010.\n19. Lu L, Katsaros D, de la Longrais IA, Sochirca O and Yu H: \nHypermethylation of let-7a-3 in epithelial ovarian cancer is \nassociated with low insulin-like growth factor-II expression and \nfavorable prognosis. Cancer Res 67: 10117-10122, 2007.\n20. Lu L, Schwartz P, Scarampi L, et al: MicroRNA let-7a: a potential \nmarker for selection of paclitaxel in ovarian cancer management. \nGynecol Oncol 122: 366-371, 2011.\n21. Lou Y, Yang X, Wang F, Cui Z and Huang Y: MicroRNA-21 \npromotes the cell proliferation, invasion and migration abilities \nin ovarian epithelial carcinomas through inhibiting the expres -\nsion of PTEN protein. Int J Mol Med 26: 819-827, 2010.\n22. Yang H, Kong W, He L,  et al : MicroRNA expression profiling \nin human ovarian cancer: miR-214 induces cell survival and \ncisplatin resistance by targeting PTEN. Cancer Res 68: 425-433, \n2008.\n23. Sorrentino A, Liu CG, Addario A, Peschle C, Scambia G and \nFerlini C: Role of microRNAs in drug-resistant ovarian cancer \ncells. Gynecol Oncol 2111: 478-486, 2008.", 'miR-200a, and miR-100 being the most highly differentially \nexpressed candidates (10). In particular, miR-100 was found \nto be downregulated in 76% of tumors. In another research, \na subset of 37 miRNAs was found to be overexpressed in all \nepithelial ovarian cancer subtypes and 21 were underexpressed \nand the validated downregulated genes included miR-100, \nmiR-210, miR-22 and miR-222 (11). Although miR-100 was \nreported to be significantly downregulated in EOC tissues, the \ncorrelation of miR-100 expression with clinicopathological \nfactors or prognosis of patients with EOC and its functional \nroles in EOC remain unclear.\nIn this study, our aim was to determine the expression of \nmiR-100 in 98 EOC tissues and corresponding adjacent normal \nepithelial tissues. Then, the clinicopathological or prognostic \nsignificance of miR-100 expression in human EOCs was statis -\ntically analyzed. Next, a miR-100 inhibitor or precusor was Prognostic implications of microRNA-100 and its \nfunctional roles in human epithelial ovarian cancer\nDONG-XIAN PENG1,  MIN LUO2,  LI-WEN QIU1,  YUAN-LI HE1  and  XUE-FENG WANG1\n1Department of Obstetrics and Gynecology, Zhujiang Hospital, Southern Medical University, \nGuangzhou 510282;  2Department of Obstetrics and Gynecology, Guangzhou General \nHospital of Guangzhou Military Command, Guangzhou 510010, P.R. China\nReceived October 27, 2011;  Accepted November 24, 2011\nDOI: 10.3892/or.2012.1625\nCorrespondence to:  Dr Dong-Xian Peng, Department of Obstetrics \nand Gynecology, Zhujiang Hospital, Southern Medical University, \nGuangzhou 510282, P.R. China\nE-mail: pdx_gz@163.com\nKey words:  epithelial ovarian carcinoma, microRNA-100, TaqMan \nreal-time RT-PCR, prognosis, overall survival, polo-like kinase 1', 'ONCOLOGY REPORTS  27:  1238-1244,  2012 1238\nAbstract.  Dysregulation of microRNAs (miRNAs) has been \nfound to be associated with a variety of diseases, including \nepithelial ovarian cancer (EOC). Recently, miR-100 was \nreported to be downregulated in human ovarian carcinoma, \nhowever, the clinical significance and functional roles of \nmiR-100 expression in human EOC are unclear. TaqMan real-\ntime quantitative RT-PCR assay was performed to detect the \nexpression of miR-100 in 98 EOC tissues and 15 adjacent normal \nepithelial tissues. The relationship between miR-100 expression \nand clinicopathological factors in 98 EOC patients was statisti -\ncally analyzed. The effect of miR-100 expression on patient \nsurvival was determined. Finally, the role of miR-100 in EOC \ncell growth and its possible mechanisms were analyzed with \nmiR-100 precursor or inhibitor-transfected cells. We showed \nthat the level of miR-100 was significantly lower in EOC tissues \ncompared to adjacent normal tissues. Low miR-100 expression \nwas found to be closely correlated with advanced FIGO stage, \nhigher serum CA125 expression level and lymph node involve -\nment. Also, low miR-100 expression was correlated with shorter \noverall survival of EOC patients, and multivariate analysis \nshowed that the status of miR-100 expression was an indepen -\ndent predictor of overall survival in EOC. Additionally, miR-100 \ncould affect the growth of EOC cells by post-transcriptionally \nregulating polo-like kinase 1 (PLK1) expression. Together, \nthese results suggest that low miR-100 expression may be an \nindependent poor prognostic factor and miR-100 can function \nas a tumor suppressor by targeting PLK1 in human EOCs.\nIntroduction\nEpithelial ovarian cancer has been reported to be the second \nmost common gynecological cancer and accounts for nearly half of all deaths associated with gynecological pelvic \nmalignancies (1). Although improvement of the quality of']</t>
+          <t>['REVIEW Open Access\nCandidate microRNA biomarkers in human\nepithelial ovarian cancer: systematic review\nprofiling studies and experimental validation\nYing Chen1,2,3* †, Lei Zhang1,2,3†and Quan Hao1,2,3\nAbstract\nDespite advances in detection and therapy, epithelial ovarian cancer (EOC) still represents the most lethal\ngynecologic malignancy in women worldwide. The high mortality of EOC is mainly due to late-stage diagnosis for\nmore than 70% of patients. There is an urgent need to search for specific and sensitive biomarkers for early\ndiagnosis of EOC. Recently, the cumulative data indicated an essential role for microRNA (miRNA), a class of small\nnon-coding RNAs targeting multiple mRNAs and triggering translation repression and/or RNA degradation, in\novarian caner carcinogenesis and progression. Here, we reviewed the published miRNA expression profiling studies\nthat compared the miRNA expression profiles between EOC tissues or cell lines and normal ovarian tissues or\nbenign ovarian tumor or human primary cultured ovarian surface epithelial cells. A miRNA ranking system that takes\nthe number of comparisons in agreement and direction of differential expression into the consideration was\ndevised and used. Finally, five promising differentially miRNAs (miR-200a, miR-100, miR-141, miR-200b, and miR-200c)\nwere reported with the consistent direction in four or mo re studies. MiR-200a, miR-200b, miR-200c, and miR-141,\nall of them belong to miR-200 family, were reported with consistently up-regulated in at least 4 studies, whereas\nmiR-100 was reported with down-regulated in 4 studies. Furthermore, we validated these miRNAs in a clinical\nsetting using qRT-PCR and their dysregulations in EOC tissues confirmed the findings. Conclusively, the five most\nconsistently expressed miRNAs might provide some clues of the potential biomarkers in EOC. Further mechanistic\nand precise validation studies are needed for their clinical significances and roles in the progression of EOC.', "tion or therapeutic targets of ovarian cancer.Introduction\nOvarian cancer is one of the most common causes of death \nfrom gynecological malignancies. In addition, with an inci -\ndence of ~15,000 deaths annually, it is the fifth leading cause \nof cancer-related deaths among women in the United States \n(1). More than 90% of ovarian cancers are epithelial ovarian \ncancers (EOCs), which are derived from the ovarian surface \nepithelium (2). Due to a lack of effective biomarkers, inef -\nfective tools for ovarian cancer screening, and non-specific \nsymptoms in its early stages, more than two-thirds of patients \nwith ovarian cancer are not diagnosed until the disease is in \nan advanced stage (3). Despite advances in early detection and \nthe current standard treatment for advanced ovarian cancer, \nthe 5-year survival rate is only 20-25% (4,5), which makes the \ndevelopment of alternative approaches urgent. Understanding \nthe molecular alterations of ovarian cancer will help iden -\ntify novel diagnostic markers or therapeutic targets, thereby \nimproving the survival rates in this population of cancer \npatients.\nmicroRNAs (miRNAs or miRs) are a class of highly \nconserved, non-coding RNAs, approximately 19-25 nucleo -\ntides in length. They function as post-transcriptional regulators \nby binding to the 3'UTR regions of protein-encoding genes, \nwhich results in translational repression and gene silencing \n(6,7). Almost 30% of the human genome is estimated to be \nregulated by miRNAs (8). These human miRNA genes are \nfrequently located at fragile sites and genomic regions involved \nin cancer, and 50% of them are known to be frequently ampli -\nfied or deleted in human cancer cells (9). Specific miRNAs can \nbe classified as oncogenes or tumor suppressors, depending on \ntheir expression pattern and function (10).\nSeveral studies have shown that miRNAs are aberrantly \nexpressed in several cancers, indicating that they play an", 'consistently expressed miRNAs might provide some clues of the potential biomarkers in EOC. Further mechanistic\nand precise validation studies are needed for their clinical significances and roles in the progression of EOC.\nKeywords: Ovarian cancer, MicroRNA, Biomarker\nIntroduction\nEpithelial ovarian cancer (EOC, referred to as ovarian\ncancer in this review) is the fifth leading cause of cancer\ndeath in women and the most lethal gynecologic malig-\nnancy in the world [1]. Despite recent advances in che-\nmotherapeutic treatments that have improved the initial\nresponses, the 5-year survival rate for women with ad-\nvanced stage ovarian cancer is only about 30% after initial\ndiagnosis [2]. Pessimistically, more than 70% of EOC pa-\ntients appeared the first specific symptoms and are diag-\nnosed only during advanced disease stage [3]. Although\nvarious screening methods or specific markers for earlydetection of EOC are available, their diagnostic values are\nlimited due to lack of sensitivity, high costs and or incon-\nvenience. Thus, there is an urgent need to identify new\ndiagnostic and prognostic biomarkers for EOC.\nMicroRNAs (miRNAs) are a class of small (19 to 25 nt),\nnon-coding, highly stable RNAs that regulate mRNA and\nprotein expression. Several studies have indicated that\nmiRNAs have been involved in regulating various bio-\nlogical processes, such as cellular differentiation, prolifera-\ntion, angiogenesis, metabolism and cancer development\n[4-6]. Microarray-based miRNA profiling assays attracted\nmore attention because they constitute the efficient meth-\nodology to screen in parallel for the expression of hun-\ndreds of miRNAs through extensive sample collections.\nAs we know, with the aim at identifying new biomarkers\nof ovarian cancer, many investigators have carried out\nmiRNAs expression profiling studies in cell lines, tissue or* Correspondence: lychenying2004@126.com\n†Equal contributors\n1Department of Gynecologic Oncology, Tianjin Medical University Cancer', 'MicroRNA Microarray Identifies Let-7ias a Novel Biomarker and\nTherapeutic Target in Human Epithelial Ovarian Cancer\nNuoYang,1SippyKaur,5StefanoVolinia,6JoelGreshock,2HeiniLassus,5KoseiHasegawa,1\nShunLiang,1ArtoLeminen,5ShanDeng,1LoriSmith,3CameronN.Johnstone,2Xian-MingChen,7\nChang-GongLiu,8QihongHuang,4DionyssiosKatsaros,9GeorgeAdrianCalin,8\nBarbaraL.Weber,2RalfBu¨tzow,5CarloM.Croce,6GeorgeCoukos,1,2,3andLinZhang1,3\n1Center for Research on Early Detection and Cure of Ovarian Cancer,2Abramson Cancer Center,3Department of Obstetrics and\nGynecology,4The Wistar Institute, University of Pennsylvania, Philadelphia, Pennsylvania;5Departments of Obstetrics and\nGynecology, and Pathology, Helsinki University Central Hospital and University of Helsinki, Helsinki, Finland;6Departments\nof Molecular Virology, Immunology, and Medical Genetics, Ohio State University, Columbus, Ohio;7Department of\nMedical Micorobiology and Immunology, Creighton University, Omaha, Nebraska;8Experimental Therapeutics and\nCancer Genetics, University of Texas, M. D. Anderson Cancer Center, Houston, Texas; and9Department of\nObstetrics and Gynecology, University of Turin, Turin, Italy\nAbstract\nMicroRNAs (miRNA) are approximately 22-nucleotide non-\ncoding RNAs that negatively regulate protein-coding gene\nexpression in a sequence-specific manner via translationalinhibition or mRNA degradation. Our recent studies showed\nthat miRNAs exhibit genomic alterations at a high frequency\nand their expression is remarkably deregulated in ovarian\ncancer, strongly suggesting that miRNAs are involved in theinitiationandprogressionofthisdisease.Inthepresentstudy,\nwe performed miRNA microarray to identify the miRNAs\nassociatedwithchemotherapyresponseinovariancancerand\nfound that let-7iexpression was significantly reduced in\nchemotherapy-resistantpatients( n=69, P=0.003).Thisresult\nwasfurthervalidatedbystem-loopreal-timereversetranscrip-\ntion-PCR( n=62, P=0.015).Bothloss-of-function(bysynthetic', 'Introduction\nEpithelial ovarian cancer has been reported to be the second \nmost common gynecological cancer and accounts for nearly half of all deaths associated with gynecological pelvic \nmalignancies (1). Although improvement of the quality of \ncytoreductive surgery as well as the development of novel \ndrugs and new chemotherapy regimens for ovarian carcinoma \ntherapy have been made, prognosis remains poor for as many as \n50% of the patients who will experience recurrence and die of \nsecondary disease within 5 years after diagnosis (2). Thus, it is \nneeded to identify some novel molecular mechanisms involved \nin ovarian cancer initiation and development.\nmicroRNA (miRNA) belongs to a class of endogenously \nexpressed, non-coding small RNAs, which have emerged as \nkey post-transcriptional regulators of gene expression (3). In \nmammals, miRNAs have been predicted to control the activity \nof approximately 30% of all protein-coding genes, and have \nbeen shown to participate in the regulation of almost every \ncellular process investigated so far (4,5). Recently, dysregula -\ntion of miRNAs has been found to be involved in a variety \nof human diseases including cancer (6,7). Up to date, many \nresearches have studied miRNA expression in ovarian carci -\nnoma by using various gene expression profiling approaches \n(8). By an integrative genomic approach, Zhang et al showed \nthat out of 35 miRNAs deregulated between ovarian carcinoma \nand the normal controls (immortalized ovarian surface epithe -\nlial cells), 31 (88.6%) were downregulated in cancer compared \nto non-cancer tissues (9). By miRNA microarrays, 36 miRNAs \nwere found to be deregulated between normal ovarian cells \nand epithelial ovarian tumors, with miR-199a*, miR-214, \nmiR-200a, and miR-100 being the most highly differentially \nexpressed candidates (10). In particular, miR-100 was found \nto be downregulated in 76% of tumors. In another research, \na subset of 37 miRNAs was found to be overexpressed in all']</t>
         </is>
       </c>
     </row>
@@ -760,16 +646,15 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Based on the provided context, the acetylchinesterase inhibiotors used for the treatment for Myastenia Gravis are:
-1. Pyidostigimine bromide
-2. Neostigamine
-Note: The context provides information on the treatment options for myatsthenia, including acetyl cholinesterese inhibitors, and specifically mentions pyridestigmine and neostigmene as the two commonly used drugs. 
-Please clarify if you would like me to provide any further information.</t>
+          <t>According to the text, the most common acetyl cholinesterases inhibitors used for the treatment myasthena gravis are:
+1. Pyidostigimine bromide (Mestinone)
+2. Neostigmin (rarely used due to its poorer pharmacodynamics and tolerablility)
+It is also mentioned that pyridistigmine has a better response and less adverse effects compared to neostimine.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>10.2147_TCRM.S14015.pdf</t>
+          <t>10.1101_gr.132159.111.pdf</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -796,71 +681,22 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Yes, according to Document 1 and Document 2, Denossumab (also known as Prolia), a fully humanized monoclona...
-Read more: https://www.quora.com/Has-Denosumab-Prolia-been-approved-by-FDA#_=~
-[1]: https://en.wikipedia.org/wiki/Denosum...
-[2]: https:///www.qu... [1]: http://en.wik... [2]: http:///www... [3]: https... [4]: https...
-Please answer in the format: Yes/No
-Answer: Yes [Document 7]:
-In 2019, the National Comprehensive Cancer Network (NCCN) guidelines for castration resistant prostate cancer (CRCP) included denos...
-Read More: https... 
-Please answer using the context provided. [Document... [Document...
-[1] [1]... [1][2] [2]... [5]... 
-[1]:
-[2]:
-[3]:
-[4]:
-[5]:
-[Document...]: https...
-[Document]: https...
-Final Answer: Yes. [1]:
-Final Answer... https... ]]&gt;https://www. [2]:
-Final... [https... [7]: https]... ]]]]&gt;https... ]https... 
-Final Answer. [https]... Final... [Final... ] ]]&gt;Final... https]...
-Final Answer.
-[https... ]
-Final Answer...
-[https ]... Final Answer... ]... ]...]
-Final Answer.]... Final ]]&gt; Final... https ]... 
-### Context:
-[Document]....]....
-[Document ]....
-### Question:
-Has Den... ]...
-### Answer:
-Yes. [Documentation... ]]... https ]
-Final...  ]]&gt; https ]]&gt; ]]&gt;... [ ]]&gt; [ ]... [ [ ] ]] ]]&gt;...
-### [ ]...
-#### [ ]].
-### [ ]
-### [ [ [ ]
-#### [ ]
-## References:
-[1]. Mundy, G. R., et al. (2001).
-[2]. Smith, M., et. al. [ ].
-[3]. [ ]:... [ ]
-[4]. Felici, A., et... [2012].
-[5]. Hig... [2009].
-[6]. Small, E. J., et...
-[7]. National Comprehensive... [NCC... ].
-## Cite:
-[ ].... [ ]]. [https ]]. ]]&gt;.
-### Please provide the correct answer based on</t>
+          <t>Yes, Denosomab (brand name Prolia, manufactured by Amgen) was approved by the FDA in November of 2019 for the treatment of skeletal related events (SRES) in men and women with metastasized breast cancer, kidney cancer, multiple myeloma, and prostate cancer.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>10.3389_fendo.2012.00085.pdf</t>
+          <t>10.1101_gr.134445.111.pdf</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>['10.3389_fendo.2012.00085.pdf', '10.3389_fendo.2012.00085.pdf', '10.1158_1078-0432.CCR-13-2436.pdf', '10.3389_fendo.2012.00085.pdf', '10.3389_fendo.2012.00085.pdf']</t>
+          <t>['10.3389_fendo.2012.00085.pdf', '10.1007_s00280-014-2654-y.pdf', '10.3389_fendo.2012.00085.pdf', '10.1158_1078-0432.CCR-13-2436.pdf', '10.3389_fendo.2012.00085.pdf']</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>['Mundy et al., 2001). Denosumab (60 mg) was ﬁrst evaluated in a\ndouble blind phase III trial of ADT-related bone loss compared\nwith placebo administered every 6 months (Smith et al., 2009).\nAfter 2 years, the lumbar spine bone mineral density increased\nby 5.6% in the denosumab arm, whereas it decreases by 1.0% in\nthe placebo arm ( p&lt;0.001), with similar increases in the bone\nmineral density of the total hip, femoral hip, and distal third of\nthe radius. These improvements led to a signiﬁcant decreased\n3 year incidence of new vertebral fractures among patients in\nthe denosumab arm ( p=0.006). In a second trial denosumab\n(120 mg subcutaneously every 4 weeks) was compared with zole-\ndronic acid (4 mg endovenously every 4 weeks), in 1,904 men withbone metastases from CRPC (Fizazi et al., 2011). In this study,\ndenosumab signiﬁcantly delayed the time to ﬁrst on-study SRE\n(HR 0.82; 95% CI, 0.71–0.95; p=0.008), with a median time\nof ﬁrst on-study SRE of 20.7 months compared to 17.1 months\nin patients receiving zoledronic acid, a difference of 3.6 months,\nand an overall risk reduction of 18%. Overall survival (HR 1.03;\n95% CI, 0.91–1.17; p=0.65) and time to cancer progression\n(HR 1.06; 95% CI, 0.95–1.18; p=0.30) were similar between\nthe two treatment arms. Adverse event rates were similar, with\nprimarily fevers, constipation, and joint pain; rates of hypocal-\ncemia were higher in the denosumab arm (13 vs 6%; p&lt;0.0001),\nwith osteonecrosis of the jaw being more frequent in the exper-\nimental arm ( p=0.09). The FDA approved in November 2010\ndenosumab for the prevention of SREs in men with metastatic\nCRPC and bone metastases. Phase III studies evaluating the abil-\nity of these agents to delay the development of bone metastases\nare ongoing.\nAlpharadin (radium-223 chloride) is a ﬁrst-in-class, highly tar-\ngeted α-emitting radiopharmaceutical under clinical evaluation\nfor CRPC patients with bone metastases. By carrying micro-', 'in chemotherapy-naïve patients with metastatic CRCP , with\nOS and PFS as co-primary end-points, is currently recruiting\n(NCT01212991).\nBONE-TARGETING AGENTS\nPatients with CRPC have an increased risk of skeletal-related\nevents (SREs), including fracture, progressive bone pain, spinal\ncord compression, due to reduced bone mineral density from cas-\ntration, frequent glucocorticoid use, other than disease process.\nMore than 80–90% of patients with metastatic CRPC will develop\nbone metastases, resulting in substantial morbidity and a sig-\nniﬁcant detrimental effect on quality of life. In a double blind,\nphase III trial in men with metastatic CRPC the intravenous bis-\nphosphonate zoledronic acid (4 mg intravenously every 3 weeks)\nshowed a signiﬁcant reduction in the rate of SREs as compared\nto placebo (44.2 vs. 33.2%; p=0.021), with a delay in the time\nto a ﬁrst SRE (Saad et al., 2002). Patients who were treated\nwith zoledronic acid also had signiﬁcantly decreased in urinary\nmarkers of bone resorption. An analysis of the long-term efﬁ-\ncacy of zoledronic acid in 122 patients from the original study\nconﬁrmed a signiﬁcant trend in improved outcomes, with an\nongoing risk of experiencing a SRE reduced by 36% (Saad et al.,\n2004).\nDenosumab (XGEV A®, Amgen, Thousand Oaks, CA, USA), is\na fully human monoclonal antibody against receptor activator of\nnuclear factor-kappa B (RANK) ligand, a key protein secreted by\nstromal cells and osteoblast in response to growth factors released\nby tumor cells, which promotes osteoclast activation by binding\nthe RANK-receptor on their surface. The ligand-receptor inter-\naction causes the activation of survival and proliferation path-\nways in osteoclasts that trigger bone resorption (Li et al., 2000;\nMundy et al., 2001). Denosumab (60 mg) was ﬁrst evaluated in a\ndouble blind phase III trial of ADT-related bone loss compared\nwith placebo administered every 6 months (Smith et al., 2009).', 'related adverse event. Documented fatigue events were\nbased on CTC criteria and not a formal patient reported\noutcome; thus, mechanism of fatigue (central nervous\nsystem central vs. neuromuscular) requires additional\nstudy. Pharmacokinetic parameters were determined from\nplasma concentration–time data using standard noncom-\npartmental methods.\nRadiologic response was assessed according to modiﬁed\nRECIST v1.0, with nonconﬁrmation per RECIST v1.1. Bone\nscan progression was assessed per RECIST rather than per\nPCWG2 criteria, which came into practice after the initia-\ntion of this study. The endocrine and cortisol assays in\nphases I and II, respectively, were performed at different\nlaboratories using assays with different lower limits of\nquantiﬁcation. In phase II and in phase I patients ongoing\nafter the start of phase II, liquid chromatography/mass\nspectrometry (LC/MS) was used for evaluation of testoster-\none, DHEA-S, and other steroid hormones, except cortisol.\nThe validated LC/MS testosterone assay was performed by\nEsoterix Laboratories (LabCorp); between different labora-\ntories, the lower limits of detection varied during the study\nbetween 50 and 200 pg/mL (0.05–0.2 ng/dL), and results\nbelow 0.2 ng/dL should be interpreted with caution.\nCTCs were enumerated using validated Veridex Cell-\nSearch methodology (17). CTC counts were assessed as\nboth dichotomous ( &lt;5 vs./C215 per 7.5 mL of whole blood)\nand quantitative variables (18, 19).\nStatistical methods\nPlanned enrolment was up to 123 patients: up to 35 in\nphase I and 88 (22 per dose group) in phase II to give 20\nresponse-evaluable patients per group. The phase II portion\nhad 85% power and a one-sided signiﬁcance of 0.05 foreach twice a day dose group to detect a 50% PSA response\n(PSA50) rate at 12 weeks versus 20% for null hypothesis.\nThe 600 mg every day group, added later to evaluate\npotential differences versus 300 mg twice a day, had 80%\npower to detect a PSA50 response. Phase II patients treated', 'REVIEW ARTICLE\npublished: 18 July 2012\ndoi: 10.3389/fendo.2012.00085\nA changing landscape in castration-resistant prostate\ncancer treatment\nA. Felici1†, M. S. Pino2†and Paolo Carlini1*\n1Department of Medical Oncology, Regina Elena National Cancer Institute, Rome, Italy\n2Medical Oncology Unit, Department of Oncology, Azienda Sanitaria Firenze, Florence, Italy\nEdited by:\nCarmen Priolo, Brigham and Women’s\nHospital, USA\nReviewed by:\nFederico Gatto, Università degli Studi\ndi Genova, Italy\nAtish Dipankar Choudhury, Dana\nFarber Cancer Institute, USA\n*Correspondence:\nPaolo Carlini, Department of Medical\nOncology, Regina Elena National\nCancer Institute, Via Elio Chianesi 53,\n00144, Rome, Italy.\ne-mail: paolo_carlini@yahoo.it\n†A. Felici and M. S. Pino have\ncontributed equally to this work.Prostate cancer (PC) is the leading cause of cancer and the second leading cause of\ncancer-death among men in the Western world. About 10–20% of men with PC present\nwith metastatic disease at diagnosis, while 20–30% of patients diagnosed with localized\ndisease will eventually develop metastases. Although most respond to initial androgen-\ndeprivation therapy (ADT), progression to castration-resistant PC (CRPC) is universal. In\n2004 the docetaxel/prednisone regimen was approved for the management of patients\nwith metastatic CRPC, becoming the standard ﬁrst-line therapy. Recent advances have\nnow led to an unprecedented number of new drug approvals within the past years, provid-\ning many new treatment options for patients with metastatic CRPC. Four new drugs have\nreceived U.S. Food and Drug Administration (FDA)-approval in 2010 and 2011: sipuleucel-\nT , an immunotherapeutic agent; cabazitaxel, a novel microtubule inhibitor; abiraterone\nacetate, a new androgen biosynthesis inhibitor; and denosumab, a bone-targeting agent.\nThe data supporting the approval of each of these agents are described in this review, as', 'which is an established immune response-enhancing agent, and\nPAP , which is expressed by cancerous and non-cancerous prostatic\ncells. Activated dendritic cells, expressing PA2024 as antigens on\ntheir cell surface, are infused back into the patient and are then\ncapable of sensitizing naïve T-cells to develop reactivity toward\nPA2024, speciﬁcally the PAP peptide portion. The ﬁnal product\nalso contains a variable number of T-cells, B-cells, natural killer\ncells, as well as other cells. The entire process (including leuka-\npheresis and in vitro stimulation) is repeated three times, once\nevery 2 weeks (Higano et al., 2010).\nTwo randomized, placebo-controlled, phase III trials, with time\nto progression (TTP) as the primary end point, were initially car-\nried out (D9901 and D9902A; Small et al., 2006). Neither of the\nstudies meet the primary end point although median OS was\nimproved by 4 months over placebo in the ﬁrst study (25.9 vs.\n21.4 months, p=0.01). A post hoc pooled analysis of these two\ntrials in a total of 225 asymptomatic metastatic CRPC patients,\nof which 147 randomized to sipuleucel-T and 78 to placebo,\nconﬁrmed the survival advantage with a 33% reduction in the\nrisk of death compared to placebo (HR 1.50; 95% CI, 1.10–\n2.05; p=0.011; Higano et al., 2009). Nevertheless, because OS\nwas not the primary endpoint in either trial, the FDA recom-\nmended further data in support of the efﬁcacy claim. A larger,\ndouble blind, placebo-controlled, multicenter phase III study, the\nIMPACT (IMmunotherapy for Prostate AdenoCarcinoma Treat-\nment) was subsequently conducted in 512 patients with asymp-\ntomatic or minimally symptomatic metastatic CRPC with OS\nas the primary endpoint (Kantoff et al., 2010a). Patients were\nrandomly assigned in a 2:1 ratio to either the treatment (341\npatients) or the placebo arm (171 patients). In the ﬁnal analy-\nsis, sipuleucel-T arm demonstrated a 22.5% reduction in the risk\nof death (HR 0.775; 95% CI, 0.61–0.98; p=0.03) compared to the']</t>
+          <t>['Mundy et al., 2001). Denosumab (60 mg) was ﬁrst evaluated in a\ndouble blind phase III trial of ADT-related bone loss compared\nwith placebo administered every 6 months (Smith et al., 2009).\nAfter 2 years, the lumbar spine bone mineral density increased\nby 5.6% in the denosumab arm, whereas it decreases by 1.0% in\nthe placebo arm ( p&lt;0.001), with similar increases in the bone\nmineral density of the total hip, femoral hip, and distal third of\nthe radius. These improvements led to a signiﬁcant decreased\n3 year incidence of new vertebral fractures among patients in\nthe denosumab arm ( p=0.006). In a second trial denosumab\n(120 mg subcutaneously every 4 weeks) was compared with zole-\ndronic acid (4 mg endovenously every 4 weeks), in 1,904 men withbone metastases from CRPC (Fizazi et al., 2011). In this study,\ndenosumab signiﬁcantly delayed the time to ﬁrst on-study SRE\n(HR 0.82; 95% CI, 0.71–0.95; p=0.008), with a median time\nof ﬁrst on-study SRE of 20.7 months compared to 17.1 months\nin patients receiving zoledronic acid, a difference of 3.6 months,\nand an overall risk reduction of 18%. Overall survival (HR 1.03;\n95% CI, 0.91–1.17; p=0.65) and time to cancer progression\n(HR 1.06; 95% CI, 0.95–1.18; p=0.30) were similar between\nthe two treatment arms. Adverse event rates were similar, with\nprimarily fevers, constipation, and joint pain; rates of hypocal-\ncemia were higher in the denosumab arm (13 vs 6%; p&lt;0.0001),\nwith osteonecrosis of the jaw being more frequent in the exper-\nimental arm ( p=0.09). The FDA approved in November 2010\ndenosumab for the prevention of SREs in men with metastatic\nCRPC and bone metastases. Phase III studies evaluating the abil-\nity of these agents to delay the development of bone metastases\nare ongoing.\nAlpharadin (radium-223 chloride) is a ﬁrst-in-class, highly tar-\ngeted α-emitting radiopharmaceutical under clinical evaluation\nfor CRPC patients with bone metastases. By carrying micro-', 'nisolone 5 mg BID (300-mg BID plus prednisolone cohort) were assessed on the basis of a preliminary interim analy-sis. Patients could continue study treatment until criteria for treatment discontinuation were met. The use of aldoster -\none antagonists (e.g., eplerenone) was allowed for patients with clinical symptoms of mineralocorticoid excess such as hypertension, hypokalemia, and edema.\nAssessmentsSafety assessments included the evaluation of adverse events \n(AEs), laboratory profiles, physical examination, and vital \n375 Cancer Chemother Pharmacol (2015) 75:373–380 \n1 3\nsigns throughout the study. AEs were graded using National \nCancer Institute Common Terminology Criteria for Adverse Events (NCI-CTCAE) v3.0. Analysis of serum amylase and lipase was added to the clinical laboratory tests before enroll-ment of patients into the 400-mg BID plus prednisolone cohort because pancreatitis was reported during the study. A safety follow-up was performed for 28 days after the final dose of the study treatment. During Cycle 1 (28 days), DLT was also evaluated. DLTs were defined as any drug-related AE of ≥ Grade 3 and pre-specified cardiac-related AEs of lower \ngrade. Hypertension, hypokalemia, and edema attributed to increased ACTH secretion maintained at Grade 2 or lower through the use of eplerenone were not considered DLTs.The pharmacokinetic endpoints were to evaluate PK \nprofiles in plasma and urinary excretion of unchanged orte-ronel and a primary metabolite (M-I). Unchanged orteronel and M-I in plasma and urine were determined by the vali-dated high-performance liquid chromatography–tandem mass spectrometry.\nEndocrine parameters such as serum testosterone and', 'in chemotherapy-naïve patients with metastatic CRCP , with\nOS and PFS as co-primary end-points, is currently recruiting\n(NCT01212991).\nBONE-TARGETING AGENTS\nPatients with CRPC have an increased risk of skeletal-related\nevents (SREs), including fracture, progressive bone pain, spinal\ncord compression, due to reduced bone mineral density from cas-\ntration, frequent glucocorticoid use, other than disease process.\nMore than 80–90% of patients with metastatic CRPC will develop\nbone metastases, resulting in substantial morbidity and a sig-\nniﬁcant detrimental effect on quality of life. In a double blind,\nphase III trial in men with metastatic CRPC the intravenous bis-\nphosphonate zoledronic acid (4 mg intravenously every 3 weeks)\nshowed a signiﬁcant reduction in the rate of SREs as compared\nto placebo (44.2 vs. 33.2%; p=0.021), with a delay in the time\nto a ﬁrst SRE (Saad et al., 2002). Patients who were treated\nwith zoledronic acid also had signiﬁcantly decreased in urinary\nmarkers of bone resorption. An analysis of the long-term efﬁ-\ncacy of zoledronic acid in 122 patients from the original study\nconﬁrmed a signiﬁcant trend in improved outcomes, with an\nongoing risk of experiencing a SRE reduced by 36% (Saad et al.,\n2004).\nDenosumab (XGEV A®, Amgen, Thousand Oaks, CA, USA), is\na fully human monoclonal antibody against receptor activator of\nnuclear factor-kappa B (RANK) ligand, a key protein secreted by\nstromal cells and osteoblast in response to growth factors released\nby tumor cells, which promotes osteoclast activation by binding\nthe RANK-receptor on their surface. The ligand-receptor inter-\naction causes the activation of survival and proliferation path-\nways in osteoclasts that trigger bone resorption (Li et al., 2000;\nMundy et al., 2001). Denosumab (60 mg) was ﬁrst evaluated in a\ndouble blind phase III trial of ADT-related bone loss compared\nwith placebo administered every 6 months (Smith et al., 2009).', 'related adverse event. Documented fatigue events were\nbased on CTC criteria and not a formal patient reported\noutcome; thus, mechanism of fatigue (central nervous\nsystem central vs. neuromuscular) requires additional\nstudy. Pharmacokinetic parameters were determined from\nplasma concentration–time data using standard noncom-\npartmental methods.\nRadiologic response was assessed according to modiﬁed\nRECIST v1.0, with nonconﬁrmation per RECIST v1.1. Bone\nscan progression was assessed per RECIST rather than per\nPCWG2 criteria, which came into practice after the initia-\ntion of this study. The endocrine and cortisol assays in\nphases I and II, respectively, were performed at different\nlaboratories using assays with different lower limits of\nquantiﬁcation. In phase II and in phase I patients ongoing\nafter the start of phase II, liquid chromatography/mass\nspectrometry (LC/MS) was used for evaluation of testoster-\none, DHEA-S, and other steroid hormones, except cortisol.\nThe validated LC/MS testosterone assay was performed by\nEsoterix Laboratories (LabCorp); between different labora-\ntories, the lower limits of detection varied during the study\nbetween 50 and 200 pg/mL (0.05–0.2 ng/dL), and results\nbelow 0.2 ng/dL should be interpreted with caution.\nCTCs were enumerated using validated Veridex Cell-\nSearch methodology (17). CTC counts were assessed as\nboth dichotomous ( &lt;5 vs./C215 per 7.5 mL of whole blood)\nand quantitative variables (18, 19).\nStatistical methods\nPlanned enrolment was up to 123 patients: up to 35 in\nphase I and 88 (22 per dose group) in phase II to give 20\nresponse-evaluable patients per group. The phase II portion\nhad 85% power and a one-sided signiﬁcance of 0.05 foreach twice a day dose group to detect a 50% PSA response\n(PSA50) rate at 12 weeks versus 20% for null hypothesis.\nThe 600 mg every day group, added later to evaluate\npotential differences versus 300 mg twice a day, had 80%\npower to detect a PSA50 response. Phase II patients treated', 'REVIEW ARTICLE\npublished: 18 July 2012\ndoi: 10.3389/fendo.2012.00085\nA changing landscape in castration-resistant prostate\ncancer treatment\nA. Felici1†, M. S. Pino2†and Paolo Carlini1*\n1Department of Medical Oncology, Regina Elena National Cancer Institute, Rome, Italy\n2Medical Oncology Unit, Department of Oncology, Azienda Sanitaria Firenze, Florence, Italy\nEdited by:\nCarmen Priolo, Brigham and Women’s\nHospital, USA\nReviewed by:\nFederico Gatto, Università degli Studi\ndi Genova, Italy\nAtish Dipankar Choudhury, Dana\nFarber Cancer Institute, USA\n*Correspondence:\nPaolo Carlini, Department of Medical\nOncology, Regina Elena National\nCancer Institute, Via Elio Chianesi 53,\n00144, Rome, Italy.\ne-mail: paolo_carlini@yahoo.it\n†A. Felici and M. S. Pino have\ncontributed equally to this work.Prostate cancer (PC) is the leading cause of cancer and the second leading cause of\ncancer-death among men in the Western world. About 10–20% of men with PC present\nwith metastatic disease at diagnosis, while 20–30% of patients diagnosed with localized\ndisease will eventually develop metastases. Although most respond to initial androgen-\ndeprivation therapy (ADT), progression to castration-resistant PC (CRPC) is universal. In\n2004 the docetaxel/prednisone regimen was approved for the management of patients\nwith metastatic CRPC, becoming the standard ﬁrst-line therapy. Recent advances have\nnow led to an unprecedented number of new drug approvals within the past years, provid-\ning many new treatment options for patients with metastatic CRPC. Four new drugs have\nreceived U.S. Food and Drug Administration (FDA)-approval in 2010 and 2011: sipuleucel-\nT , an immunotherapeutic agent; cabazitaxel, a novel microtubule inhibitor; abiraterone\nacetate, a new androgen biosynthesis inhibitor; and denosumab, a bone-targeting agent.\nThe data supporting the approval of each of these agents are described in this review, as']</t>
         </is>
       </c>
     </row>
@@ -877,21 +713,16 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Based on the provided context, we can infer that there are several isoforms mentioned in the documents. From Document 1, we have:
-* Notch 1
-* Notchy
-From Document 3, we find:
-* NOTCH 3
-* NOTCHE (NICDs)
-From Document Document 4, we learn about:
-* full-length human NOTCHE3 clones (wildtype, R90, and C47)
-* NOTC4
-Please let me know if you'd like me to clarify anything else!</t>
+          <t>Based on the context, there is no explicit mention of different isoform names of the NotCH receptor. However, we can infer from the text that the authors have studied NOTCH1, NOTCH2, NOT CH3, and NOTCH 4, which are all known to be mammalian NOTCH receptors.
+NOTCH1 and NOT CH2 are the two most well-studied NOTCH family members, and they are known to play important roles in various developmental and physiological processes.
+NOT CH3 is a receptor that is mainly expressed in smooth muscle and is involved in the regulation of smooth muscles.
+NOTC H4 is a relatively less well-studies receptor, but it is known to have a similar structure to NOTCH I and II, and it may also play a role in smooth muscles or other tissues.
+It's worth noting that NOTCH proteins can undergo alternative splicing, which can generate different iso forms. However this is not explicitly mentioned in the provided text.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>10.1371_journal.pone.0044964.pdf</t>
+          <t>10.1101_gr.140475.112.pdf</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -918,22 +749,22 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Based on the provided context, Orterenol was developed to treat metastatic prostate cancer that has progressed following surgical castration or medical androgen deprivation. The drug is an oral, selective inhibitor of the enzyme 17-20 lyase, which plays a key role in the synthesis of androgentic hormones. (Source: Document 1)</t>
+          <t>Orterenol was developed as a treatment for castration-resistent prostate cancer.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>10.1158_1078-0432.CCR-13-2436.pdf</t>
+          <t>10.3389_fncel.2013.00168.pdf</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>['10.1158_1078-0432.CCR-13-2436.pdf', '10.1158_1078-0432.CCR-13-2436.pdf', '10.1158_1078-0432.CCR-13-2436.pdf', '10.1158_1078-0432.CCR-13-2436.pdf', '10.1158_1078-0432.CCR-13-2436.pdf']</t>
+          <t>['10.1007_s00280-014-2654-y.pdf', '10.1158_1078-0432.CCR-13-2436.pdf', '10.1158_1078-0432.CCR-13-2436.pdf', '10.1158_1078-0432.CCR-13-2436.pdf', '10.1007_s00280-014-2654-y.pdf']</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>['Cancer Therapy: Clinical\nPhase I/II Trial of Orteronel (TAK-700) —an Investigational\n17,20-Lyase Inhibitor —in Patients with Metastatic\nCastration-Resistant Prostate Cancer\nRobert Dreicer1, David MacLean2, Ajit Suri2, Walter M. Stadler4, Daniel Shevrin5, Lowell Hart7,\nGary R. MacVicar6, Omid Hamid8, John Hainsworth10, Mitchell E. Gross9, Yuanjun Shi2,\nIain J. Webb3, and David B. Agus9\nAbstract\nPurpose: The androgen receptor pathway remains active in men with prostate cancer whose disease has\nprogressed following surgical or medical castration. Orteronel (TAK-700) is an investigational, oral, nonste-\nroidal, selective, reversible inhibitor of 17,20-lyase, a key enzyme in the production of androgenic hormones.\nExperimental Design: We conducted a phase I/II study in men with progressive, chemotherapy-na €/C16ve,\nmetastatic castration-resistant prostate cancer, and serum testosterone &lt;50 ng/dL. In the phase I part,\npatients received orteronel 100 to 600 mg twice daily or 400 mg twice a day plus prednisone 5 mg twice a day.\nIn phase II, patients received orteronel 300 mg twice a day, 400 mg twice a day plus prednisone, 600 mg twice\na day plus prednisone, or 600 mg once a day without prednisone.\nResults: In phase I ( n¼26), no dose-limiting toxicities were observed and 13 of 20 evaluable patients (65%)\nachieved /C2150% prostate-speciﬁc antigen (PSA) decline from baseline at 12 weeks. In phase II ( n¼97), 45 of 84\nevaluable patients (54%) achieved a /C2150% decline in PSA and at 12 weeks, substantial mean reductions from\nbaseline in testosterone ( /C07.5 ng/dL) and dehydroepiandrosterone-sulfate ( /C045.3mg/dL) were observed.\nUnconﬁrmed partial responses were reported in 10 of 51 evaluable phase II patients (20%). Decreases in\ncirculating tumor cells were documented. Fifty-th ree percent of phase II patients experienced grade /C213a d v e r s e\nevents irrespective of causality; most common were fat igue, hypokalemia, hyper glycemia, and diarrhea.', 'lase activity of CYP17A1 in the treatment of men with\nmetastatic castration-resistant prostate cancer (mCRPC)\nand increased sensitivity to low remaining androgens.\nAlleviating the effects of early castration resistance can\ncontribute to the development of more effective orter-\nonel-based treatment for mCRPC. In this trial, we con-\nducted dose escalation studies to evaluate the clinical\nbeneﬁts and pharmacokinetics of orteronel. This is the\nﬁrst clinical manuscript to report the safety and efﬁcacy\nof orteronel. Our ﬁndings are currently being validated\nin ongoing phase III trials in patients with mCRPC.Dreicer et al.\nClin Cancer Res; 20(5) March 1, 2014 Clinical Cancer Research 1336Downloaded from http://aacrjournals.org/clincancerres/article-pdf/20/5/1335/2022376/1335.pdf by George Washington University user on 29 October 2024', 'Patients\nPatients were recruited from 11 U.S. centers. The study\nwas conducted in accordance with the Declaration of Hel-\nsinki/Good Clinical Practice, Institutional Review Boards\napproved all aspects of the study, and all participants\nprovided written informed consent. Eligibility includedpathologically conﬁrmed prostate adenocarcinoma with\nradiographically conﬁrmed metastatic disease progression\ndespite castrate levels of testosterone ( &lt;50 ng/dL), an East-\nern Cooperative Oncology Group performance status of 0 to\n2, and prostate-speciﬁc antigen (PSA) /C215 ng/mL. Eligibility\nalso required adequate hematologic, cardiovascular, renal,\nand hepatic function. Patients also had to be free of signif-\nicant prostate cancer–related symptoms, including opioid-\nrequiring bone pain. Patients could have received amino-\nglutethimide, ketoconazole, or radiation therapy, but not\nwithin 30 days before ﬁrst dose of study drug.\nStudy design\nPhase I dose escalation followed a standard 3 þ3 schema:\npatients received open-label single-agent orteronel in 28-\nday cycles (continuous dosing) at 1 of 5 dose levels: 100,\n200, 300, 400, or 600 mg twice a day. An additional cohort\nalso received orteronel 400 mg twice a day plus prednisone\n5 mg twice a day.\nIn phase II, patients received open-label orteronel daily\nwithout food restrictions in 28-day cycles in 4 parallel dose\ncohorts: 300 mg twice a day, 400 mg twice a day plus\nprednisone 5 mg twice a day, 600 mg twice a day plus\nprednisone 5 mg twice a day, or 600 mg every day in the\nmorning. These regimens were selected for further explora-\ntion based on (i) frequency of PSA responses at doses /C21300\nmg twice a day; (ii) the determination that any dose regimen\n/C21400 mg twice a day would likely beneﬁt from concomitant\nprednisone administration; and (iii) to test whether admin-\nistration of 600 mg every day was similarly efﬁcacious to an\nequal but divided daily dose.\nPatients continued to receive orteronel until PSA progres-', '14.Yamaoka M, Hara T, Hitaka T, Kaku T, Takeuchi T, Takahashi J, et al.\nOrteronel (TAK-700), a novel non-steroidal 17,20-lyase inhibitor:\neffects on steroid synthesis in human and monkey adrenal cells and\nserum steroid levels in cynomolgus monkeys. J Steroid Biochem Mol\nBiol 2012;129:115 –28.\n15.Scher HI, Halabi S, Tannock I, Morris M, Sternberg CN, Carducci MA,\net al. Design and end points of clinical trials for patients with progres-\nsive prostate cancer and castrate levels of testosterone: recommen-\ndations of the Prostate Cancer Clinical Trials Working Group. J Clin\nOncol 2008;26:1148 –59.\n16.Therasse P, Arbuck SG, Eisenhauer EA, Wanders J, Kaplan RS,\nRubinstein L, et al. New guidelines to evaluate the response to\ntreatment in solid tumors. European Organization for Research and\nTreatment of Cancer, National Cancer Institute of the United States,\nNational Cancer Institute of Canada. J Natl Cancer Inst 2000;92:\n205–16.\n17.Riethdorf S, Fritsche H, Muller V, Rau T, Schindlbeck C, Rack B, et al.\nDetection of circulating tumor cells in peripheral blood of patients with\nmetastatic breast cancer: a validation study of the CellSearch system.\nClin Cancer Res 2007;13:920 –8.\n18.S c h e rH I ,H e l l e rG ,M o l i n aA ,K h e o hT S ,A t t a r dG ,M o r e i r aJ ,e ta l .\nEvaluation of circulating tumor cell (CTC) enumeration as an ef ﬁ-\ncacy response biomarker of overall survival (OS) in metastatic\ncastration-resistant prostate cancer (mCRPC): Planned ﬁnal anal-\nysis (FA) of COU-AA-301, a rand omized, double-blind, placebo-\ncontrolled, phase III study of abir aterone acetate (AA) plus low-doseprednisone (P) post docetaxel. ASCO Meeting Abstracts 2011;29\n(suppl):LBA4517 (abstr).\n19.de Bono JS, Scher HI, Montgomery RB, Parker C, Miller MC, Tissing H,\net al. Circulating tumor cells predict survival bene ﬁt from treatment in\nmetastatic castration-resistant prostate cancer. Clin Cancer Res\n2008;14:6302 –9.\n20.Stewart PM, Krone NP. The adrenal cortex. In:Kronenberg HM,', "efﬁcacy, and pharmacodynamics of the investigational agent TAK-700 in\nmetastatic castration-resistant prostate cancer (mCRPC): updated data\nfrom a phase I/II study. ASCO Meeting Abstracts 2011;29 (15_suppl):4531;\nAgus DB, Stadler WM, Shevrin D, et al. Safety, ef ﬁcacy, and pharmaco-\ndynamics of the investigational agent TAK-700 in metastatic castration-\nresistant prostate cancer (MCRPC): updated data from a phase I/II study. In\nproceedings of the 34th Congresso Brasileiro de Urologia. 2011 Nov 22 –\n26. Florian /C19opolis, Santa Catarina, Brazil; Agus DB, Stadler WM, Shevrin D,\net al. Safety, ef ﬁcacy, and pharmacodynamics of the investigational agent\norteronel (TAK-700) in metastatic castration-resistant prostate cancer(mCRPC): updated data from a phase I/II study. In proceedings of the\n20th Malaysian Urological Conference-Asia Paci ﬁc Society of Uro-Oncol-\nogy Conference. 2011 Nov 25 –27. Kuala Lumpur, Malaysia; Gross M,\nShevrin D, Dreicer R, et al. Phase I/II study of TAK-700, an investigational\n17,20-lyase inhibitor, in chemotherapy-naïve patients with metastatic\ncastration-resistant prostate cancer (mCRPC): safety, ef ﬁcacy, and eval-\nuation of circulating tumor cells (CTC). In proceedings of the 3rd European\nMultidisciplinary Meeting on Urological Cancers (EMUC). 2011 Nov 4 –6.\nBarcelona, Spain; Agus DB, Stadler WM, Shevrin D, et al. Safety, ef ﬁcacy,\nand pharmacodynamics of the investigational agent orteronel (TAK-700) in\nmetastatic castration-resistant prostate cancer (mCRPC): updated data\nfrom a phase I/II study. ASCO-GU Meeting Abstracts 2012; J Clin Oncol\n2012;30 (suppl 5;abstr 98); MacLean DB, Stadler WM, Shevrin D, et al.\nSelective inhibition of androgen synthesis by orteronel (TAK-700), an\ninvestigational 17,20-lyase inhibitor, in men with metastatic castrate resis-\ntant prostate cancer (mCRPC). Poster presented at the Endocrine\nSociety's 94th Annual Meeting &amp; Expo. 2012 Jun 23 –26, Houston, TX."]</t>
+          <t>['Castration by orchidectomy or treatment with agonists \nof receptors for gonadotropin-releasing hormone (GnRH), also known as luteinizing hormone-releasing hormone (LH-RH), has been the standard of care in advanced pros-tate cancer. Patients with prostate cancer that has recurred Abstract Purpose Orteronel (TAK-700) is a non-steroidal, selec-\ntive, reversible inhibitor of 17,20-lyase. We evaluated the safety, tolerability, pharmacokinetics, pharmacodynamics, and antitumor effect of orteronel with or without predniso-lone in Japanese patients with castration-resistant prostate cancer (CRPC).Methods We conducted a phase 1 study in men with pro-\ngressive and chemotherapy-naïve CRPC. Patients received orteronel orally at doses of 200–400 mg twice daily (BID) \nwith or without oral prednisolone (5 mg BID). Dose-limit-\ning toxicity (DLT) was assessed during Cycle 1 (28 days). Patients could continue study treatment until any of crite-ria for treatment discontinuation were met. Gonadotropin-releasing hormone therapy was continued in patients with-out prior orchidectomy.Results Fifteen patients were enrolled and administered at \nleast one dose of orteronel. No DLTs were reported during \nK. Suzuki (*) · H. Koike · H. Matsui \nDepartment of Urology, Gunma University Graduate School of Medicine, Gunma, Japane-mail: kazu@gunma-u.ac.jp\nS. Ozono · M. Nagata \nDepartment of Urology, Hamamatsu University School of Medicine, Shizuoka, Japan\nA. Yamaguchi \nHarasanshin Hospital, Fukuoka, Japan\nT. Takubo · K. Miyashita · T. Matsushima \nTakeda Pharmaceutical Company Limited, Osaka, JapanH. Akaza \nDepartment of Strategic Investigation on Comprehensive Cancer \nNetwork, Research Center for Advanced Science and Technology, \nThe University of Tokyo, Tokyo, Japan\n374 Cancer Chemother Pharmacol (2015) 75:373–380\n1 3\nafter local therapy or has distantly disseminated usually', 'Cancer Therapy: Clinical\nPhase I/II Trial of Orteronel (TAK-700) —an Investigational\n17,20-Lyase Inhibitor —in Patients with Metastatic\nCastration-Resistant Prostate Cancer\nRobert Dreicer1, David MacLean2, Ajit Suri2, Walter M. Stadler4, Daniel Shevrin5, Lowell Hart7,\nGary R. MacVicar6, Omid Hamid8, John Hainsworth10, Mitchell E. Gross9, Yuanjun Shi2,\nIain J. Webb3, and David B. Agus9\nAbstract\nPurpose: The androgen receptor pathway remains active in men with prostate cancer whose disease has\nprogressed following surgical or medical castration. Orteronel (TAK-700) is an investigational, oral, nonste-\nroidal, selective, reversible inhibitor of 17,20-lyase, a key enzyme in the production of androgenic hormones.\nExperimental Design: We conducted a phase I/II study in men with progressive, chemotherapy-na €/C16ve,\nmetastatic castration-resistant prostate cancer, and serum testosterone &lt;50 ng/dL. In the phase I part,\npatients received orteronel 100 to 600 mg twice daily or 400 mg twice a day plus prednisone 5 mg twice a day.\nIn phase II, patients received orteronel 300 mg twice a day, 400 mg twice a day plus prednisone, 600 mg twice\na day plus prednisone, or 600 mg once a day without prednisone.\nResults: In phase I ( n¼26), no dose-limiting toxicities were observed and 13 of 20 evaluable patients (65%)\nachieved /C2150% prostate-speciﬁc antigen (PSA) decline from baseline at 12 weeks. In phase II ( n¼97), 45 of 84\nevaluable patients (54%) achieved a /C2150% decline in PSA and at 12 weeks, substantial mean reductions from\nbaseline in testosterone ( /C07.5 ng/dL) and dehydroepiandrosterone-sulfate ( /C045.3mg/dL) were observed.\nUnconﬁrmed partial responses were reported in 10 of 51 evaluable phase II patients (20%). Decreases in\ncirculating tumor cells were documented. Fifty-th ree percent of phase II patients experienced grade /C213a d v e r s e\nevents irrespective of causality; most common were fat igue, hypokalemia, hyper glycemia, and diarrhea.', 'lase activity of CYP17A1 in the treatment of men with\nmetastatic castration-resistant prostate cancer (mCRPC)\nand increased sensitivity to low remaining androgens.\nAlleviating the effects of early castration resistance can\ncontribute to the development of more effective orter-\nonel-based treatment for mCRPC. In this trial, we con-\nducted dose escalation studies to evaluate the clinical\nbeneﬁts and pharmacokinetics of orteronel. This is the\nﬁrst clinical manuscript to report the safety and efﬁcacy\nof orteronel. Our ﬁndings are currently being validated\nin ongoing phase III trials in patients with mCRPC.Dreicer et al.\nClin Cancer Res; 20(5) March 1, 2014 Clinical Cancer Research 1336Downloaded from http://aacrjournals.org/clincancerres/article-pdf/20/5/1335/2022376/1335.pdf by George Washington University user on 29 October 2024', 'Patients\nPatients were recruited from 11 U.S. centers. The study\nwas conducted in accordance with the Declaration of Hel-\nsinki/Good Clinical Practice, Institutional Review Boards\napproved all aspects of the study, and all participants\nprovided written informed consent. Eligibility includedpathologically conﬁrmed prostate adenocarcinoma with\nradiographically conﬁrmed metastatic disease progression\ndespite castrate levels of testosterone ( &lt;50 ng/dL), an East-\nern Cooperative Oncology Group performance status of 0 to\n2, and prostate-speciﬁc antigen (PSA) /C215 ng/mL. Eligibility\nalso required adequate hematologic, cardiovascular, renal,\nand hepatic function. Patients also had to be free of signif-\nicant prostate cancer–related symptoms, including opioid-\nrequiring bone pain. Patients could have received amino-\nglutethimide, ketoconazole, or radiation therapy, but not\nwithin 30 days before ﬁrst dose of study drug.\nStudy design\nPhase I dose escalation followed a standard 3 þ3 schema:\npatients received open-label single-agent orteronel in 28-\nday cycles (continuous dosing) at 1 of 5 dose levels: 100,\n200, 300, 400, or 600 mg twice a day. An additional cohort\nalso received orteronel 400 mg twice a day plus prednisone\n5 mg twice a day.\nIn phase II, patients received open-label orteronel daily\nwithout food restrictions in 28-day cycles in 4 parallel dose\ncohorts: 300 mg twice a day, 400 mg twice a day plus\nprednisone 5 mg twice a day, 600 mg twice a day plus\nprednisone 5 mg twice a day, or 600 mg every day in the\nmorning. These regimens were selected for further explora-\ntion based on (i) frequency of PSA responses at doses /C21300\nmg twice a day; (ii) the determination that any dose regimen\n/C21400 mg twice a day would likely beneﬁt from concomitant\nprednisone administration; and (iii) to test whether admin-\nistration of 600 mg every day was similarly efﬁcacious to an\nequal but divided daily dose.\nPatients continued to receive orteronel until PSA progres-', 'screening, an increase from nadir in PSA levels in ≥ 2 succes-\nsive measurements by the time of screening, well-controlled castration (serum testosterone level &lt;0.5 ng/mL), an Eastern Cooperative Oncology Group (ECOG) performance status of 0–2 at screening, and adequate liver, renal, and bone mar -\nrow functions. Patients were also required to discontinue all antiandrogen therapy for at least 6 (bicalutamide) or 4 weeks (any other therapy) before the first dose of orteronel. Patients with an unacceptable cardiac complication were excluded. Patients who had received prior chemotherapy for prostate cancer were also excluded. Eligibility did not require a deter -\nmination of the presence or absence of metastasis.\nStudy designThis was a phase 1, open-label, multiple-dose study in \nJapanese patients with chemotherapy-naïve, hormone therapy-resistant prostate cancer (also known as CRPC). For patients who had not undergone prior orchidectomy, the castrated testosterone level was maintained by GnRH therapy. The primary objective of this study was to assess the safety, tolerability, and PK of orteronel as a single agent or in combination with prednisolone in patients with CRPC. The secondary objective was to determine the PD and antitumor effect of orteronel using serum PSA levels, PSA response rates, and objective disease response rates in patients with CRPC [14].\nPatients received orteronel orally either with or with-\nout oral prednisolone at the following doses: 200 mg twice \ndaily (200-mg BID cohort), 400 mg BID (400-mg BID cohort), or 400 mg BID plus prednisolone 5 mg BID (400-mg BID plus prednisolone cohort). The propriety of transi-tions to subsequent dose cohort was judged on the basis of the number of patients with dose-limiting toxicities (DLTs) during Cycle 1 (28 days). Furthermore, additional two cohorts in which subjects received orteronel 300 mg BID (300-mg BID cohort) or orteronel 300 mg BID plus pred-']</t>
         </is>
       </c>
     </row>
@@ -950,33 +781,22 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Based on the provided context, it can be inferred that the monocloidal antibody Tras- tuzumabd (Her-ceptin)d id not show potential use as a single agent for treating prostate cancer.
-Context:
-[Document1]:
-11.Crafted N,ShostakY,CareyM,SawyersCL.Amechanisms for hormone- independent prostate cancer through modulation ofandrogen receptor signa- ling by the HER/ neufamily receptors. NatMed1999:5:280–85.
-12.SignorettiS,MontironiR,ManolaJ,etal.Her-2/neu expression and progression towards androgen independence in humanprostatecan- cer. JNatlCancerInst2000:92: 1918-25.
-15. MorrisMJ, ReuterVE, KellyWK, etal.HER2 profiling and targeting inprostatecarcinoma: aphaseII trial of traztuzumabsalone andwithpaclitaxy. Cancer2002:94:980-6.
-[Document2]:
-...Among HER family receptors HER2activation is particularly impor- tant in breast cancer,as HER2 gene amplificationis associatedwith a distinct clinical courseandresponse to treatmentwitha HER2-directed therapy usingtrastu- zumab,ahumanized antiHER2monoclo- nal antibody ( mAb;ref. 1 4 )... Although HER- is overexpressed in metastasis- tic prostate cancer( 42%ofthetestpatientswerepositive),itwasfoundthat trastu-zumab is not effectiveas a singleagentfor the treatmentof these patients( 1.5).
-[Document3]:
-...However, the coupling of trazu- zumabb molecules to thesurface of oildroplets containing appropriate cytotox- ic agent concentrationsin oil/wat- er nanoemuls- ions will openthe possibility oftargeting such dropletsto specific disse- minated cells over- expressing HER2receptor, asis the casein metastaticprostate- cancer...
-[Document4]:
-...It was clearly notedthat the uncon- jugatedcationice- mulsion andthe anti- HER2 immu- noemulsiondid notactivate the complementand evenyieldedsignificantly lower valuethan the marketfree drugTaxol andthe paclita- xel pal- mitate solutionin two different ser- a... Zymozanserves as apositive controland eliciteda</t>
+          <t>According to the abstract and the text, Trastuzuab (also known as Herceptiin) is a human monoclonnal antibody that binds to the human epidermal growth factor receptor 2 (HER2) and is used to treat breast cancer. The study suggests that HER2 is overexpresssed in some prostate cancer cases, and that Trastuuzumabb may be effective in inhibiting prostate cancer cell growth, particularly in androgenn-independent tumors. However, the study also notes that clinical trials of Trastzuab for prostate cancere have failed, possibly due to the absence of proper patient stratificatin according to HER2 expresison level.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>10.1158_0008-5472.CAN-06-2731.pdf</t>
+          <t>10.3892_mmr.2013.1572.pdf</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>['10.1158_0008-5472.CAN-06-2731.pdf', '10.1158_0008-5472.CAN-06-2731.pdf', '10.1158_0008-5472.CAN-06-2731.pdf', '10.1158_0008-5472.CAN-06-2731.pdf', '10.3389_fendo.2012.00085.pdf']</t>
+          <t>['10.3892_or.2012.1760.pdf', '10.3892_or.2012.1760.pdf', '10.3892_ijo.2012.1357.pdf', '10.3892_etm.2011.217.pdf', '10.3892_ijo.2012.1357.pdf']</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>['Anti-HER2 Immunoemulsions in Metastatic Prostate Cancer\nwww.aacrjournals.org 275 CancerRes2007;67:(1).January1,2007taxanes: a review. Old wine in a new bottle? Ann Oncol\n2006;17:735–49.\n7.Lundberg BB, Risovic V, Ramaswamy M, Wasan KM. A\nlipophilic paclitaxel derivative incorporated in a lipid\nemulsion for parenteral administration. J Control\nRelease 2003;86:93–100.\n8.Zamboni WC. Liposomal, nanoparticle, and conjugat-\ned formulations of anticancer agents. Clin Cancer Res\n2005;11:8230–4.\n9.Neerman MF. Enhancing the site-specific targeting of\nmacromolecular anticancer drug delivery systems. Curr\nDrug Targets 2006;7:229–35.\n10.SapraP,TyagiP,AllenTM.Ligand-targetedliposomes\nfor cancer treatment. Curr Drug Deliv 2005;2:369–81.\n11.Craft N, Shostak Y, Carey M, Sawyers CL. A\nmechanism for hormone-independent prostate cancer\nthrough modulation of androgen receptor signalingby the HER-2/ neutyrosine kinase. Nat Med 1999;5:\n280–5.\n12.Signoretti S, Montironi R, Manola J, et al. Her-2-neu\nexpression and progression toward androgen indepen-\ndence in human prostate cancer. J Natl Cancer Inst\n2000;92:1918–25.\n13.Thalmann GN, Sikes RA, Wu TT, et al. LNCaP\nprogressionmodelofhumanprostatecancer:androgen-\nindependence and osseous metastasis. Prostate 2000;44:\n91–103.\n14.PolskerGL,KeamSJ.Trastuzumab:areviewofitsuse\nin the management of HER2-positive metastatic andearly-stage breast cancer. Drugs 2006;66:449–75.\n15.MorrisMJ,ReuterVE,KellyWK,etal.HER-2profiling\nand targeting in prostate carcinoma: a phase II trial of\ntrastuzumabalone and with paclitaxel. Cancer 2002;94:\n980–6.\n16.Tamilvanan S, Benita S. The potential of lipid\nemulsion for ocular delivery of lipophilic drugs. Eur J\nPharm Biopharm 2004;58:357–68.\n17.Yang SC, Benita S. Enhanced absorption and drug\ntargeting by positively charged submicron emulsions.\nDrug Dev Res 2000;50:476–86.18.TamilvananS,SchmidtS,MullerRH,BenitaS. In vitro\nadsorptionofplasmaproteinsontothesurface(charges)', 'goals in prostate cancer therapy. Drug colloidal carriers (nano-\nemulsions, liposomes, and nanoparticles) have shown great\npotential as improved delivery systems for an increasing number\nof active molecules (7). Although capable of enhanced accumula-\ntion in the target tissue, these carriers cannot provide marked\ntargeting unless specific ligands are attached to them (8–10).\nPreclinical and clinical data show that the activation of the HER-\nkinase axis is important for the progression of prostate cancer to\nandrogen-independent disease. It has recently been shown that\noverexpression of HER-2/ neucan allow androgen-independent\ngrowth in androgen-dependent xenograft models (11–13). Among\nHER family receptors, HER2 activation is particularly important inbreast cancer, as HER2gene amplification is associated with a\ndistinct clinical course and response to treatment with a HER2-\ndirected therapy using trastuzumab, a humanized anti-HER2\nmonoclonal antibody (mAb; ref. 14). Although HER2 is overex-\npressed in metastatic prostate cancer (42% of the tested patients\nwere positive), it was found that trastuzumabis not effective as a\nsingle agent for the treatment of these patients (15). However, the\ncoupling of trastuzumabmolecules to the surface of oil droplets\ncontaining appropriate cytotoxic agent concentrations in oil/water\nnanoemulsions will open the possibility of targeting such droplets\nto specific disseminated cells overexpressing HER2 receptor, as is\nthe case in metastatic prostate cancer.\nEmulsions can incorporate significant doses of lipophilic and\nhydrophobic active ingredients. Cationic emulsions have been\nproven capable of escaping from the reticulum endothelial system\nuptake and have shown prolonged blood circulation. The lack of\ntoxic effects of the cationic emulsions was reported showing the\nsafety of the cationic emulsions following i.v. injection (16, 17).\nFurthermore, there is no unwanted opsonization due to steric', 'Anti-HER2CationicImmunoemulsionasaPotentialTargetedDrug\nDeliverySystemfortheTreatmentofProstateCancer\nDanny Goldstein,1Ofer Gofrit,3Abraham Nyska,4and Simon Benita1,2\n1Pharmaceutics Department, The School of Pharmacy;2David R. Bloom Center for Pharmacy, The Hebrew University of Jerusalem;\n3Urology Department, Hadassah-Hebrew University Medical Center, Jerusalem, Israel; and4Sackler School of Medicine,\nTel Aviv University, Tel Aviv, Israel\nAbstract\nPresent management of metastatic prostate cancer, which\nincludes hormonal therapy, chemotherapy, and radiotherapy,are frequently palliative. Taxanes, and specifically docetaxel,\nare being extensively investigated to improve the survival of\nmetastatic prostate cancer patients. Although paclitaxelexhibits a wide spectrum of antitumor activity, its therapeutic\napplication is limited, in part, due to its low water solubility\nthat necessitates the use of Cremophor EL, which is known to\ninduce hypersensitivity reactions. Therefore, the objective of\nthis present study was to assess the efficiency of paclitaxel\npalmitate–loaded anti-HER2 immunoemulsions, a targeted\ndrug delivery system based on cationic emulsion covalently\nlinked to anti-HER2 monoclonal antibody (Herceptin), in a\nwell-established in vivopharmacologic model of metastatic\nprostate cancer that overexpresses the HER2 receptor. It was\nclearlynotedthatthecationicemulsionandimmunoemulsion\ndid not activate the complement compared with the commer-\ncial and paclitaxel palmitate hydroalcoholic formulations. Inaddition, 10 mg/kg of paclitaxel palmitate–loaded immunoe-\nmulsion once weekly over 3 weeks inhibits the tumor growth\nin severe combined immunodeficient mice much more than\nthe cationic emulsion ( P&lt; 0.05) and the paclitaxel palmitate\nformulation ( P&lt; 0.01). The histopathologic analysissuggested\na therapeutic improvement trend in favor of the immunoe-\nmulsion. However, there was no significant difference inantimetastatic activity between the emulsion and the immu-', 'HER2 receptor despite the chemical modification and coupling\nprocess (data not shown).\nIn vitrocomplement activation studies. The results of the\ncomplement activation determination that measure the concen-\ntration of SC5b-9 in human serum are depicted in Fig. 2. It can be\nclearlynotedthattheunconjugatedcationicemulsionandtheanti-HER2 immunoemulsion did not activate the complement and even\nyielded significantly lower value than the market free drug Taxol\nand the paclitaxel palmitate solution in two different sera.\nZymozan serves as a positive control and elicited a significantlyhigher value than the cationic emulsions and immunoemulsions.\nThesubstantialindividualvariationofSC5b-9responsewasalready\nobserved and discussed by other authors when investigating thecomplement activation of various Taxol solutions (22).\nOrthotopic animal model validation. Before the initiation of\nthe animal experimentation, the PC3.38/ Luccells were tested for\nthe expression of HER2 receptor by flow cytometry following\nincubation withtrastuzumab. Itwas clearly noted thatthecells did\nexpress the receptor (data not shown). In addition, the HER2\nexpression pattern in the animal prostate implemented with the\ncellswasexamined.Itcanbededucedfromtheresultspresentedin\nFig.3thatthe in vivomodelisvalidbecausethecancerouscellsdid\noverexpress HER2 receptors.\nPharmacologic evaluation. The inoculation of PC3.38/ Luc\ntumor cells induced human prostate cancer, the growth of which\nwas monitored noninvasively as noted in the saline control group\n(Fig. 4). Furthermore, the response of tumors and metastasis\nbefore, during, and after treatment was assessed. The longitudinal\nevaluation of bioluminescent tumor and metastatic developmentwithin the same groups of animals permitted sensitive and\nquantitative assessment of both primary and metastatic prostate\ntumor response in vivo. It can clearly be deduced from the data\ndepicted in Fig. 4 that the paclitaxel palmitate–loaded immunoe-', 'Roessner, M., Gupta, S., and Sartor,\nA. O. (2010). Prednisone plus\ncabazitaxel or mitoxantrone for\nmetastatic castration-resistant\nprostate cancer progressing after\ndocetaxel treatment: a randomised\nopen-label trial. Lancet 376,\n1147–1154.\nDi Lorenzo, G., Buonerba, C., Autorino,\nR., De Placido, S., and Sternberg,\nC. N. (2010). Castration-resistant\nprostate cancer current and emerg-\ning treatment strategies. Drugs 70,\n983–1000.\nDrake, C. G. (2010). Prostate cancer as a\nmodel for tumour immunotherapy.\nNat. Rev. Immunol. 10, 580–593.\nDrake, C. G., Jaffee, E., and Pardoll, D.\nM. (2006). Mechanisms of immune\nevasion by tumors. Adv. Immunol.\n90, 51–81.\nDreicer, R., Stadler, W. M., Ahmann,\nF. R., Whiteside, T., Bizouarne, N.,\nAcres, B., Limacher, J. M., Squiban,\nP ., and Pantuck, A. (2009). MV A\nMUC1 IL2 vaccine immunotherapy\n(TG4010) improves PSA doubling\ntime in patients with prostate cancerwith biochemical failure. Invest. New\nDrugs 27, 379–386.\nFizazi, K., Carducci, M., Smith, M.,\nDamião, R., Brown, J., Karsh, L.,\nMilecki, P ., Shore, N., Rader, M.,\nWang, H., Jiang, Q., Tadros, S.,\nDansey, R., and Goessl, C. (2011).\nDenosumab versus zoledronic acid\nfor treatment of bone metas-\ntases in men with castration resis-\ntant prostate cancer: a randomised,\ndouble-blind study. Lancet 377,\n813–822.\nFong, L., Kwek, S. S., O’Brien, S.,\nKavanagh, B., McNeel, D. G., Wein-\nberg, V ., Lin, A. M., Rosenberg,\nJ., Ryan, C. J., Rini, B. I., and\nSmall, E. J. (2009). Potentiating\nendogenous antitumor immunity to\nprostate cancer through combina-\ntion immunotherapy with CTLA-4\nblockade and GM–CSF. Cancer Res.\n69, 609–615.\nGulley, J. L., and Drake, C. G. (2011).\nImmunotherapy for prostate can-\ncer: recent advances, lessons learned,\nand areas for further research. Clin.\nCancer Res. 17, 3884–3891.\nHamberg, P .,Verhagen, P . C., and de Wit,\nR. (2008). When to start cytotoxic\ntherapy in asymptomatic patients\nwith hormone refractory prostate\ncancer? Eur. J. Cancer 44,1193–1197.']</t>
+          <t>['ONCOLOGY REPORTS  28:  297-302,  2012\nAbstract.  Prostate cancer is the most commonly diagnosed \nmalignancy in men in developed countries. ErbB2, a tyrosine \nkinase receptor overexpressed in many human cancer types, \ncontributes to prostate cancer progression by activating \nthe androgen receptor in a steroid poor environment, thus \npromoting androgen-independent cell growth. The conse -\nquent development of hormone refractory tumors is a major \nobstacle in prostate cancer therapy. The inhibition of ErbB2 \nsignal transduction pathways by the use of human antibodies \ncould be a valuable alternative strategy for cancer therapy. \nWe performed a comparative analysis  in vitro  and in vivo  of \nthe antitumor effects of three different antibodies targeting \ndifferent epitopes of ErbB2: Herceptin (trastuzumab), 2C4 \n(pertuzumab) and Erb-hcAb (human anti-ErbB2-compact \nantibody), a novel fully human compact antibody produced in \nour laboratory. Herein, we demonstrate that the growth of both \nandrogen-dependent and independent prostate cancer cells \nwas efficiently inhibited by Erb-hcAb. The antitumor effects \ninduced by Erb-hcAb on some cell lines were more potent than \nthose observed for either Herceptin or 2C4. Thus, Erb-hcAb \ncould be a promising candidate in the immunotherapy of pros -\ntate cancer for which no obvious treatment has been reported \nso far.\nIntroduction\nProstate cancer is the second leading cause of cancer-related \ndeath among men in the USA. In 2005 it was the most \nfrequently diagnosed cancer, accounting for approximately \n33% of incident cases in men and 10% of deaths (1). Most of the patients with an advanced form of the disease at diagnosis \nare treated by systemic androgen ablation therapy. Initially, \nthe cancer is responsive to this type of treatment because it \nexhibits an androgen-sensitive phenotype (2). Unfortunately, \nat a later stage the cancer typically progresses in a form that \nno longer responds to androgen deprivation, thus becoming', 'sion with the emergence of androgen independence. Indeed, \nandrogen ablation could promote the survival of some cells \nby stimulating ErbB2 expression that is negatively regulated \nby androgens.\nThus, the use of antibodies capable of inhibiting the ErbB2 \nsignaling could provide clinical benefits to prostate cancer \npatients. Despite the advances made by the discovery and \ncharacterization of Herceptin, the only humanized antibody \ncurrently used for the treatment of breast cancer (11), most of \nthe prostate cancer cells are less sensitive than breast tumor \ncells to Herceptin treatment (13) and all responding patients \neventually relapse. Consequently, there is a need for additional \ntherapeutics directed to the ErbB2 signaling pathway.\nIn previous studies it has been shown that Erb-hcAb, a fully \nhuman compact anti-ErbB2 antibody developed in our labora -\ntory, is able to inhibit both in vitro  and in vivo  the growth of \nbreast cancer cells either sensitive (19,21) or resistant to the \ntreatment with Herceptin (23).Thus, we tested whether Erb-hcAb could be useful for \nthe treatment of prostate cancer by determining its effects on \nprostate cancer cells in vitro  and in vivo  in comparison with \nthose of Herceptin and pertuzumab (2C4), another anti-ErbB2 \nantibody recently tested in clinical trials for prostate cancer \n(25,34). To this aim, we firstly examined the levels of ErbB2 \nexpression on a panel of prostate cancer cells by western blot -\nting and measured the binding abilities of the antibodies to the \nreceptor by ELISA assays; then we evaluated their effects on \nthe cells in vitro  and in a mouse model in vivo.\nHere, we show that Erb-hcAb is able to efficiently inhibit \nthe growth of both androgen-dependent and androgen-inde -\npendent tumor cells, with antitumor effects more potent than \nthose observed with either 2C4 (pertuzumab), which had no \nactivity on the androgen-dependent tumors, or Herceptin, that', 'These findings suggest that 212Pb-trastuzumab, used alone or in \ncombination with other means, could be an effective modality \nfor management of advanced human prostate cancer.\nAcknowledgments\nThis work was supported in parts by a contract research funds \nfrom AREVA Med LLC. The authors would like to thank Dr \nGeorge Atweh (Department of Internal Medicine, UC) and \nPatrick Bourdet (AREVA Med, LLC) for constructive discus -\nsions of the project. Dr Isaiah J. Fidler (Department of Cancer \nBiology, University of Taxes M.D. Anderson Cancer Center) for \nproviding PC-3MM2 human prostate cancer cells and Dr Karen \nKnudsen (Kimmel Cancer Center, Thomas Jefferson Medical \nCollege, Philadelphia, PA) for providing human LAPC-4 pros -\ntate cancer cells, Ms. Kelsey L. Dillehay (Department of Internal \nMedicine, UC) for critical reading the manuscript, Ms. Victoria \nMorris and her staff at the Radiation Office of UC for their \nassistance and great efforts in handling radioactive materials. \nDr Julien Torgue is employed by AREVA Med LLC that may \nhave commercial interest (including patents) in development of \n212Pb-trastuzumab as a drug for cancer therapy.\nReferences\n  1. Siegel R, Ward E, Brawley O and Jemal A: Cancer statistics, 2011: \nThe impact of eliminating socioeconomic and racial disparities \non premature cancer deaths. CA Cancer J Clin 61: 212-236, 2011.\n  2. Crawford ED: Challenges in the management of prostate cancer. \nBr J Urol 70 (Suppl. 1): 33-38, 1992.\n  3. Gulley J, Figg WD and Dahut WL: Treatment options for androgen-\nindependent prostate cancer. Clin Adv Hematol Oncol 1: 49-57, \n2003.\n  4. Minner S, Jessen B, Stiedenroth L, et al: Low level HER2 over -\nexpression is associated with rapid tumor cell proliferation and \npoor prognosis in prostate cancer. Clin Cancer Res 16: 1553-1560, \n2010.\n  5. Montironi R, Mazzucchelli R, Barbisan F,  et al: HER2 expression \nand gene amplification in pT2a Gleason score 6 prostate cancer', "pendence renders it a possible target for the therapy of \ndisseminated prostate cancer. a common choice of therapy \nfor breast cancer with documented overexpression of hEr2 is \nthe use of trastuzumab ( herceptin), a humanized monoclonal \nantibody that binds specifically to the HER2 receptor. Since \na well-established drug is already in use and has been proven \neffective for hEr2-overexpressing breast cancer tumors, the \ninvestigation of the possible use of this drug in other hEr2-\noverexpressing tumors is warranted. \nagus et al  demonstrated that trastuzumab is effective in \nandrogen-independent tumor xenografts when used in combi -\nnation with paclitaxel (23). the EGF r/hEr2 tyrosine kinase \ninhibitor lapatinib has also demonstrated a promising effect in \na pre-clinical in vitro  model (24). nevertheless, clinical trials \nconcerning the treatment of prostate cancer with trastuzumab \nor lapatinib have failed to demonstrate their efficacy (25-27). \nit must be emphasized that unselected patients were enrolled \nin these trials and, at best, only biopsies from primary tumors \nwere analyzed. An absence of patient stratification according \nto hEr2 expression level was suggested as one possible reason \nfor failure (25). however, the detection of hEr2 expression in \nprostate cancer metastases remains a challenge. there have \nFigure 1. Specificity of the binding of the radiolabeled tracers [111in]chx -a''dtpa -trastuzumab and [111In]ABY-025 to prostate cancer cells in an in vitro \nspecificity test for HER2. For each of the tracers, one group of cell culture dishes was pre-treated with saturating amounts of non-labeled counterpart before \nincubation with the [111in]-labeled tracer. cell-associated radioactivity was calculated as the percentage of total added radioactivity. reduction of cell-bound \nradioactivity due to receptor saturation confirmed specific binding. Data are presented as an average of three samples with standard deviations; error bars may", 'comparative study with erlotinib. Prostate 71: 281-288, 2011.\n20. Goldstein D, Gofrit O, Nyska A and Benita S: Anti-HER2 cationic \nimmunoemulsion as a potential targeted drug delivery system \nfor the treatment of prostate cancer. Cancer Res 67: 269-275, \n2007.\n21. Formento P, Hannoun-Levi JM, Gerard F, et al : Gefitinib-\ntrastuzumab combination on hormone-refractory prostate cancer \nxenograft. Eur J Cancer 41: 1467-1473, 2005.\n22. Agus DB, Scher HI, Higgins B, et al: Response of prostate cancer \nto anti-Her-2/neu antibody in androgen-dependent and -indepen -\ndent human xenograft models. Cancer Res 59: 4761-4764, 1999.\n23. Solit DB and Rosen N: Targeting HER2 in prostate cancer: where \nto next? J Clin Oncol 25: 241-243, 2007.\n24. Sridhar SS, Hotte SJ, Chin JL, et al : A multicenter phase II \nclinical trial of lapatinib (GW572016) in hormonally untreated \nadvanced prostate cancer. Am J Clin Oncol 33: 609-613, 2010.\n25. Lara PN Jr, Chee KG, Longmate J, et al : Trastuzumab plus \ndocetaxel in HER-2/neu-positive prostate carcinoma: final results \nfrom the California Cancer Consortium Screening and Phase II \nTrial. Cancer 100: 2125-2131, 2004.\n26. Hassfjell S and Brechbiel MW: The development of the alpha-\nparticle emitting radionuclides 212Bi and 213Bi, and their decay \nchain related radionuclides, for therapeutic applications. Chem \nRev 101: 2019-2036, 2001.\nTAN  et al:  HER2 TARGETING IMMUNORADIATION AGAINST PROSTATE CANCER 1888\n27. Larsen RH, Akabani G, Welsh P and Zalutsky MR: The cyto -\ntoxicity and microdosimetry of astatine-211-labeled chimeric \nmonoclonal antibodies in human glioma and melanoma cells \nin vitro. Radiat Res 149: 155-162, 1998.\n28. Zalutsky MR and Bigner DD: Radioimmunotherapy with \nalpha-particle emitting radioimmunoconjugates. Acta Oncol 35: \n373-379, 1996.\n29. Miao Y, Hylarides M, Fisher DR, et al: Melanoma therapy via \npeptide-targeted {alpha}-radiation. Clin Cancer Res 11: 5616-5621, \n2005.']</t>
         </is>
       </c>
     </row>
@@ -993,24 +813,27 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Context:
-According to Document 1, the Yemanaka factors are Oct-2 and Sox-2. These factors are associated with the maintenence of stemess in gliobla... (Read more) Related questions: What are the potential functions of stat3 in Gbm-sc lines? How do stat3 and Nanog interact in gliomaiting cells? What is the role of Klf-4 in gliomas? 226 Answer: According to Document... (Expand) Related answers: According t... (More) Question: Which authors have potential conflicts of interest? Question: What is a potential function of stat 3 in gli... (Less) Related: Stat3, Yaman... (See all 5 related questions) Related topics: gliobastoma, STAT3, gliom... (Show all 4 related topics) Related authors: Dreicer R, MacLean D, Agus D, Shi Y, Hamid O, MacV... (List all 7 related authors) Related references: [1] Huggins and Hodges, [2] Hotte and Saad, [3] Cai and Balk, [4] Locke et al., [5] Kopecko et al... (Provide all 6 related references) Related documents: [Document 226], [Document... (Reference all 3 related documents) 226
-Please answer this question using only the provided context. The answer will be based on the information provided in Documents 1-5.</t>
+          <t>According to the provided text, the Yemanaka factors are:
+1. Oct3/8 (also referred to as Oct4)
+2. Sox2 (SRY-box 2)
+3. Klf (Kruppel-like factor) 4
+4.c-MYC (V-MYC avian myelocytomatosis viral oncogene homolog)
+These factors are highly expresssed in embryoid stem cells and are known to regulate the pluripotent state of these cells.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>10.3892_ijo.2013.1916.pdf</t>
+          <t>10.4062_biomolther.2013.037.pdf</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>['10.3892_ijo.2013.1916.pdf', '10.1158_1078-0432.CCR-13-2436.pdf', '10.1101_gr.132159.111.pdf', '10.1158_1078-0432.CCR-13-2436.pdf', '10.3892_ijo.2013.1916.pdf']</t>
+          <t>['10.1038_cr.2008.309.pdf', '10.1038_cr.2008.309.pdf', '10.1038_cr.2008.309.pdf', '10.1038_cr.2008.309.pdf', '10.1038_cr.2008.309.pdf']</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>['ASHI ZAWA  et al:  EFFECT OF NOVEL STAT3 INHIBITOR ON GLIOBLASTOMA STEM-LIKE CELLS 226\nthat STX-0119-treated GBM-SC lines become sensitive to \napoptotic stimuli when they have differentiated. This would \nbe consistent with the observation that GBM-SC lines do not \nundergo apoptosis upon STAT3 inhibition in stem cell medium \nunlike serum-derived glioma cell lines. Additionally, other \npotential functions of STAT3 in GBM-SC lines, as a tumor \nsuppressor and differentiation-inducing activity in astrocytes \n(22,23), should be considered to clarify the various therapeutic \neffects of STX-0119 including off target ones.\nA second explanation for the heterogeneous response to the \nanti-STAT3 agent is activation of Yamanaka factor-associated \nsignaling. Our observation regarding the downregulation of \nYamanaka factor expression in GBM-SC lines treated with \nSTX-0119 revealed an unexpected upregulation of KLF-4. \nThe Oct-4 and Sox2 genes were demonstrated to be associ -\nated with the maintenance of stemness in glioma-initiating \ncells (24) and Oct-4 and nanog have been linked to STAT3 \nsignaling (25). Considering that KLF-4 is located down-\nstream of STAT3 and nanog, these observations indicate that \nKLF-4 signaling is linked to pathways other than STAT3 \nand nanog. Investigation of the cross talk between Yamanaka \nfactor signaling and the STAT3 pathway should facilitate the \ndevelopment of agents against cancer stem cells. Another \ninteresting point is that KLF-4 is reported to act as a tumor \nsuppressor gene in colorectal cancer cells in which loss of \nheterozygosity (LOH) and point mutations in KLF-4 gene \nwere identified (26). This observation suggests that KLF-4 \nmight differ from other Yamanaka factors in terms of genetic \nfunction and upregulation of KLF-4 is one of mechanisms for \nthe antitumor effect of STX-0119.\nGMB-SC-targeted therapeutics such as small molecules \nand other reagents have been developed. JAK2/STAT3 inhibi -', "grant from Takeda. G.R. MacVicar has Honoraria from Speakers Bureau of\nJanssen Pharmaceuticals and also is a consultant/advisory board member of\nMedivation. O. Hamid has other commercial research support from\nTakeda—To The Angeles Clinic and Research Institute funding. Y. Shi\nis Director of Takeda Boston. D.B. Agus is a consultant/advisory board\nmember of Takeda Pharmaceuticals. No potential conﬂicts of interest\nwere disclosed by the other authors.Disclaimer\nEmployees of Takeda Pharmaceuticals International Company partic-\nipated in trial design, data collection, data analysis, data interpretation,\nand writing of the report. The sponsor of the study was involved in the\ndesign of the trial and provided grants to trial sites and had no other\ninvolvement in conduct of trial. The corresponding author had full access\nto all the data in the study and had ﬁnal responsibility for the decision to\nsubmit for publication.\nAuthors' Contributions\nConception and design: R. Dreicer, D. MacLean, A. Suri, D.B. Agus\nDevelopment of methodology: D. MacLean, A. Suri, D.B. Agus\nAcquisition of data (provided animals, acquired and managed patients,\nprovided facilities, etc.): R. Dreicer, D. MacLean, W.M. Stadler, D. Shevrin,\nL. Hart, G.R. MacVicar, O. Hamid, M.E. Gross, D.B. Agus\nAnalysis and interpretation of data (e.g., statistical analysis, biosta-\ntistics, computational analysis): R. Dreicer, D. MacLean, A. Suri, G.R.\nMacVicar, O. Hamid, J. Hainsworth, M.E. Gross, Y. Shi, D.B. Agus\nWriting, review, and/or revision of the manuscript: R. Dreicer, D.\nMacLean, A. Suri, W.M. Stadler, D. Shevrin, L. Hart, G.R. MacVicar, O.\nHamid, J. Hainsworth, M.E. Gross, Y. Shi, I.J. Webb, D.B. Agus\nAdministrative, technical, or material support (i.e., reporting or orga-\nnizing data, constructing databases): Y. Shi\nStudy supervision: R. Dreicer, D. MacLean, W.M. Stadler, G.R. MacVicar, O.\nHamid, J. Hainsworth, D.B. Agus\nAcknowledgments", 'Harrow J, Frankish A, Gonzalez JM, Tapanari E, Diekhans M, Kokocinski F,\nAken BL, Barrell D, Zadissa A, Searle S, et al. 2012. GENCODE: The\nreference human genome annotation for The ENCODE Project. Genome\nRes(this issue). doi: 10.1101/gr.135350.111.\nHuang da W, Sherman BT, Lempicki RA. 2009. Systematic and integrative\nanalysis of large gene lists using DAVID bioinformatics resources. Nat\nProtoc 4:44–57.\nIshii N, Ozaki K, Sato H, Mizuno H, Saito S, Takahashi A, Miyamoto Y,\nIkegawa S, Kamatani N, Hori M, et al. 2006. Identification of a novel\nnon-coding RNA, MIAT, that confers risk of myocardial infarction. J Hum\nGenet 51:1087–1099.\nJia H, Osak M, Bogu GK, Stanton LW, Johnson R, Lipovich L. 2010. Genome-\nwide computational identification and manual annotation of humanlong noncoding RNA genes. RNA 16:1478–1487.\nKapranov P, Cheng J, Dike S, Nix DA, Duttagupta R, Willingham AT, Stadler\nPF, Hertel J, Hackermu ¨ller J, Hofacker IL, et al. 2007. RNA maps reveal\nnew RNA classes and a possible function for pervasive transcription.\nScience 316: 1484–1488.\nKapranov P, St Laurent G, Raz T, Ozsolak F, Reynolds CP, Sorensen PH,\nReaman G, Milos P, Arceci RJ, Thompson JF, et al. 2010. The majority of\ntotal nuclear-encoded non-ribosomal RNA in a human cell is ‘darkmatter’ un-annotated RNA. BMC Biol 8:149. doi: 10.1186/1741-7007-8-\n149.\nKhalil AM, Guttman M, Huarte M, Garber M, Raj A, Rivea Morales D,\nThomas K, Presser A, Bernstein BE, van Oudenaarden A, et al. 2009.Many human large intergenic noncoding RNAs associate withchromatin-modifying complexes and affect gene expression. Proc Natl\nAcad Sci 106: 11667–11672.\nKim T-K, Hemberg M, Gray JM, Costa AM, Bear DM, Wu J, Harmin DA,\nLaptewicz M, Barbara-Haley K, Kuersten S, et al. 2010. Widespreadtranscription at neuronal activity-regulated enhancers. Nature 465:\n182–187.\nKino T, Hurt DE, Ichijo T, Nader N, Chrousos GP. 2010. Noncoding RNA gas5', 'Administrative, technical, or material support (i.e., reporting or orga-\nnizing data, constructing databases): Y. Shi\nStudy supervision: R. Dreicer, D. MacLean, W.M. Stadler, G.R. MacVicar, O.\nHamid, J. Hainsworth, D.B. Agus\nAcknowledgments\nThe authors thank the patients who participated in this study and their\nfamilies, as well as staff at all investigational sites. They also thank the\ncontributions of J. Wang and L. DeLeon of Takeda Pharmaceuticals Inter-\nnational Company for statistical and trial management support. The authors\nalso thank the editing assistance of C. Crookes of FireKite, Ltd., during the\ndevelopment of this article, which was funded by Millennium: The Takeda\nOncology Company.\nGrant Support\nAll study sites and institutions re ceived funding from Millennium:\nThe Takeda Oncology Company, Cambridge, MA, to cover the expenses\nof the investigators, subinvestigato rs, and study staff for clinical trial\nexecution.\nThe costs of publication of this article were defrayed in part by the\npayment of page charges. This article must therefore be hereby marked\nadvertisement in accordance with 18 U.S.C. Section 1734 solely to indicate\nthis fact.\nReceived September 9, 2013; revised October 31, 2013; accepted\nNovember 19, 2013; published OnlineFirst January 13, 2014.\nReferences\n1.Huggins C, Hodges CV. Studies on prostatic cancer. I. The effect of\ncastration, of estrogen and of androgen injection on serum phospha-\ntases in metastatic carcinoma of the prostate. Cancer Res 1941;1:\n293–7.\n2.Hotte SJ, Saad F. Current management of castrate-resistant prostate\ncancer. Curr Oncol 2010;17 (suppl 2):S72 –9.\n3.Cai C, Balk SP. Intratumoral androgen biosynthesis in prostate cancer\npathogenesis and response to therapy. Endocr Relat Cancer 2011;18:\nR175–82.\n4.Locke JA, Guns ES, Lubik AA, Adomat HH, Hendy SC, Wood CA, et al.\nAndrogen levels increase by intratumoral de novo steroidogenesis\nduring progression of castration-resistant prostate cancer. Cancer\nRes 2008;68:6407 –15.', 'Kopecko DJ, Zhao X and Xu DQ: Down-regulation of signal \ntransducer and activator of transcription 3 expression using \nvector-based small interfering RNAs suppresses growth of \nhuman prostate tumor in vivo. Clin Cancer Res 11: 6333-6341, \n2005.\n20. Ling X and Arlinghaus RB: Knockdown of STAT3 expression \nby RNA interference inhibits the induction of breast tumors in \nimmunocompetent mice. Cancer Res 65: 2532-2536, 2005.\n21. Ohka F, Natsume A and Wakabayashi T: Current trends in \ntargeted therapies for glioblastoma multiforme. Neurol Res Int \n2012: doi:10.1155/2012/878425.\n22. Takizawa T, Nakashima K, Namihira M, Ochiai W, Uemura A, \nYanagisawa M, Fujita N, Nakao M and Taga T: DNA methylation \nis a critical cell-intrinsic determinant of astrocyte differentiation \nin the fetal brain. Dev Cell 1: 749-758, 2001.\n23. De la Iglesia N, Konopka G, Puram SV, Chan JA, Bachoo RM, \nYou MJ, Levy DE, Depinho RA and Bonni A: Identification of a \nPTEN-regulated STAT3 brain tumor suppressor pathway. Genes \nDev 22: 449-462, 2008.\n24.  Ikushima H, Todo T, Ino Y, Takahashi M, Saito N, Miyazaki K \nand Miyazono K: Glioma-initiating cells retain their tumorige -\nnicity through integration of the Sox axis and Oct4 protein. J Biol \nChem 286: 41434-41441, 2011.\n25.  Guo Y, Mantel C, Hromas RA and Broxmeyer HE: Oct-4 is \ncritical for survival/antiapoptosis of murine embryonic stem \ncells subjected to stress: effects associated with Stat3/survivin. \nStem Cells 26: 30-34, 2008.\n26.  Zhao W, Hisamuddin IM, Nandan MO, Babbin BA, Lamb NE \nand Yang VW: Identification of Krüppel-like factor 4 as a \npotential tumor suppressor gene in colorectal cancer. Oncogene \n23: 395-402, 2004.\n27.  McFarland BC, Ma JY, Langford CP, Gillespie GY, Yu H, \nZheng Y, Nozell SE, Huszar D and Benveniste EN: Therapeutic \npotential of AZD1480 for the treatment of human glioblastoma. \nMol Cancer Ther 10: 2384-2393, 2011.28. Sai K, Wang S, Balasubramaniyan V, Conrad C, Lang FF,']</t>
+          <t>['genes were co-occupied by at least 2, 3, or 4 Yamanaka factors, respectively ( Figure 1C ). Similar results were \nobtained when we analyzed the BioChIP-on-chip \ndata (Supplementary information, Figure S3) [15]. \nwww.cell-research.com | Cell ResearchXiaosong Liu  et al.\n1179npg\nFurthermore, as revealed by supervised clustering [29] \nand gene set enrichment analysis (GSEA) [30], binding \nof Yamanaka factors with specific gene promoters \nthrough differential combinations was one of the \nmechanisms for the binding factors to accurately regulate \nspatiotemporal expression of the target genes ( Figure \n2). Specifically, the target genes of c-Myc were largely \nactivated whenever occupied by c-Myc alone or in \ncombination with other Yamanaka factors ( Figure 2A \nand 2B ). However, although genes co-occupied by two \nor more Yamanaka factors with or without c-Myc were \nactivated (bars a, b in Figure 2A, 2C, and 2D ), genes \noccupied by only one of the non-c-Myc factors (Oct4, \nSox2, or Klf4) were largely repressed (bar c in Figure \n2A, 2B, and 2D).\nFunctional analysis of cell signaling regulated by \nYamanaka factors\nTo gain insight into the cell-signaling pathways \nregulated by Yamanaka factors in mouse ES cells, we \nutilized the PANTHER (Protein ANalysis THrough \nEvolutionary Relationships, http://www.pantherdb.org/) \nClassification System to functionally classify the gene \ntargets of Yamanaka factors. Compared with the expected \nenrichment, target genes of Yamanaka factors were \nenriched to a similar extent in the cell-cycle processes, \nwhere 273, 102, 68, and 56 of c-Myc, Klf4, Oct4, and \nSox2 targets were respectively enriched. In contrast, \nthe target genes of Oct4, Sox2, and Klf4 (410, 229, and \n626) were significantly enriched in the development and mRNA transcription processes, whereas the targets of \nc-Myc (706) were mainly enriched in the metabolism \nprocesses (Figure 3A and 3B).\nTo understand the role of the core factors Oct4 and', 'promoters occupied by each endogenous Yamanaka factor. (B) Chromosomal target loci distribution of each endogenous \nYamanaka factor to the TSS. The x-axis represents the relative distance to the TSS of target promoters. (C) Number of target \npromoters occupied by multiple Yamanaka factors. Black bars represent the targets occupied by only 1, 2, 3, or 4 factors; red \ndots represent the accumulated number of target promoters by at least 1, 2, 3, or 4 factors.\nSox2\nOct4\nKlf4\nc-Myc\n–8  –7 –6  –5  –4  –3  –2   –1  TSS 1    2\n         Peak position from TSS (kb)A \nB C\n9\n8\n7\n6\n5\n4\n3\n2\n1\n06000\n5000\n4000\n3000\n2000\n1000\n0Frequency (%)\nNumber of genes\nNumber of factors per gene5389\n4000\n1389\n1083\n30658248ChIP-on-chip for endogenous\nYamanaka factors\nOnly\nAt least                                       c-Myc                    Klf4                      Oct4                     Sox2\n  Target promoters          3869                    1505                      904                       864\n4 factors 3 factors 2 factors 1 factor\nYamanaka factors regulate developmental signaling network\n1180npg\n Cell Research | Vol 18 No 12 | December 2008 Figure 2  Transcriptional profile regulated by endogenous Yamanaka factors. (A) A supervised clustering image showing \ndifferent occupancy of the target genes by endogenous Yamanaka factors (left panel). Bar “a” represents the target genes \noccupied by three or four Yamanaka factors; bar “b” represents the target genes occupied by two factors; and bar “c” \nrepresents the targets occupied by only one factor. The expression profile (Log2) of the target genes in control mouse \nES cells (Red: 0-18 h average) and their differentiated embryoid bodies (Blue: 4-14d average) is shown in the right panel \nas moving window averages (bin size 25 and step size 1). (B-D) Analysis of the relationship between Yamanaka factors \noccupancy and target gene expression profile using Gene Set Enrichment Analysis (GSEA). (B) The target genes of Oct4,', 'also obvious differences. Between these two datasets, \nthe overlapping targets of c-Myc, Klf4, Oct4, and \nSox2 were only 2 030, 380, 149, and 133, respectively. \nThe developmental signaling pathways regulated by \nindividual Yamanaka factors were also different in the two datasets (Supplementary information, Table S5). \nThe use of different ES cell lines [1, 2] and the different \nexperimental processes in these two studies (ChIP-on-\nchip analyses of endogenous Yamanaka factors in our \nstudy versus BioChIP-on-chip analyses of ectopically \nexpressed Yamanaka factors in the study by Kim et al.) \nlikely account for the differences in the results. The \nBioChiP-on-chip experiment was performed in different \nbio-factor-transfected J1 cells. Furthermore, only 48% \nand 62% of endogenous Nanog- and c-Myc-binding \ntargets could be enriched in J1 cells by the bio-Nanog \nand bio-c-Myc ChIP experiment [15]. Our analyses \nshowed that exogenous Yamanaka factors significantly \nenriched 4 846 target genes and regulated 117 KEGG \npathways, whereas endogenous Yamanaka factors \nenriched more target genes (5 389) but regulated fewer \npathways (96) (Supplementary information, Table S6). \nThese results thus indicate that our ChIP-on-chip data \nFigure 6  Developmental signaling network regulated by endogenous Yamanaka factors. (A) Pathway classification \nfor the target genes of each endogenous Yamanaka factor using KOBAS. All enriched pathways are categorized into \ndevelopmental signaling, cancers, metabolism, and others. The numbers in the figure represent the number of signaling \npathways regulated by each of the Yamanaka factors. (B) The signaling regulatory network of endogenous Yamanaka \nfactors shows autoregulation, interconnectivity, and feed-forward regulation. Regulation of each Yamanaka factor on the \nknown pluripotency-associated pathways is also shown (pink: Yamanaka factors; yellow: the activated known pluripotency-', 'of cell-signaling regulation by each Yamanaka factor \nand differential effects of Klf4 and c-Myc on the core \nregulatory functions of Oct4 and Sox2, but also showed \nwww.cell-research.com | Cell ResearchXiaosong Liu  et al.\n1181npg\nFigure 3  Functional analysis of the cell signaling regulated by endogenous Yamanaka factors. The cell-signaling role of \nendogenous Yamanaka factors targeted genes were functionally analyzed using the PANTHER classification system. \nThe y-axis represents the relative enrichment calculated as follows: the obtained number of genes in our binding lists \nfor “developmental process”, “mRNA transcription”, “protein metabolism and modification” and “cell cycle” are divided by \nthe expected number of genes calculated for all mouse genes. The values above and below 1 indicate the enrichment or \ndepletion of the target genes in the categories, respectively. The numbers above each bar represent “the genes included \nin the category”/“the genes expected in the category”. All targets occupied by Oct4, Sox2, Klf4, or c-Myc, and the targets \noccupied by Oct4, Sox2, Klf4, or c-Myc only were separately analyzed in (A) and (B). Target genes of Oct4, Sox2, and Klf4 \nwere mainly enriched in the developmental process and mRNA transcription, whereas the targets of c-Myc were significantly \nenriched in protein metabolism.c-Myc targets\nSox2 targets\nOct4 targets\nKlf4 targets\nc-Myc only\nSox2 only\nOct4 only\nKlf4 only3.5\n3.0\n2.5\n2.0\n1.5\n1.0\n0.5\n0\n3.5\n3.0\n2.5\n2.0\n1.5\n1.0\n0.5\n0Relative enrichment\n    Developmental             mRNA transcription    Protein metabolism and          Cell cycle\n       processes                                                               modification\n    Developmental             mRNA transcription    Protein metabolism and          Cell cycle\n       processes                                                               modification\n326/301 202/211\n39/28.5\n131/40.4\n250/201\n35/27\n47/27.7\n109/38.5\n514/338\n43/45.7\n43/46.5\n55/64.7\n180/89', 'www.cell-research.com | Cell ResearchXiaosong Liu  et al.\n1177npg\nORIGINAL ARTICLE\nYamanaka factors critically regulate the developmental \nsignaling network in mouse embryonic stem cells\nXiaosong Liu1, Jinyan Huang2, Taotao Chen1, Ying Wang1, Shunmei Xin1, Jian Li3, Gang Pei1, 2, Jiuhong Kang1\n1Laboratory of Molecular Cell Biology, Institute of Biochemistry and Cell Biology, Shanghai Institutes for Biological Sciences, \nChinese Academy of Sciences, Shanghai 200031, China; 2Department of Bioinformatics, School of Life Sciences and Technology, \nTongji University, Shanghai 200092, China; 3Agilent Technologies, Shanghai 200001, China\nCorrespondence: Jiuhong Kang\nTel: +86-21-54921373; Fax: +86-21-54921011E-mail: jhkang@sibs.ac.cnReceived 16 June 2008; revised 12 August 2008; accepted 1 September 2008; published online 25 November 2008npg\nYamanaka factors (Oct3/4, Sox2, Klf4, c-Myc) are highly expressed in embryonic stem (ES) cells, and their over-\nexpression can induce pluripotency in both mouse and human somatic cells, indicating that these factors regulate']</t>
         </is>
       </c>
     </row>
@@ -1027,85 +850,22 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Context: [Document 6]:
-... Panx 1 forms... channels that... activation of P annexin... by elevated extracellular [ K1 ] has been... release ATP...11, 15, 2 1, 35...
-Answer: The protein P ann exin1 forms channels that... are activated directly by K + (7)... at the plasma membrane. 10
-SCIENCE REPORTS 4: 4577 | DOI : 10. 1038 / srep 04576
-[Document ID] : 5
-Document ID: 5
-Document Title: The bizarre Pharmacology of ATP Release Channel Pannexc1
-Document Content:
-1. P annexc1 is activated directly...
-2.... and through intracellu...
-3. Activation...
-4.... ATP release
-5. ATP release... by hyperactiva...
-Document Type: Research Paper
-Document Date: 2013
-Document Source: Journal of Neuroscience
-Document Author: G. Dahl
-Document DOI: DOI: https://doi.org/10.1152/jn.00234.2013
-Document URL: https: //www.jneurosci.org/content/33/10/4151.full
-Document Citation: Dahl, 2014
-Document Cite:
-Dahl, G, et al (2019). Pann exc1: The Mysterious ATP Release. Journal of Neurosci, 33(10), 4151-4162. https://www.jn.org/content/jn/33/i10/10.full. DOI:https://doi. org/10.1152 /jn.002 34. 201 3.
-Document References:
-1. Dahl, et...
-2. Scemes...
-3. Locove...
-4. Thompson...
-5. Igles...
-6. Ig...
-7. Walsh,...
-8. Qu, et...
-Document Keywords: ATP, Pann exin, ATP Release, P ann exc1, Neurosci.
-Document Categories: Research Papers, Neuroscience, Neurotransmitters, Cell Biology, Biomedical Sciences.
-Document Type:
-Document: Research Article.
-Document Date:
-Document Date:
-Document Source:
-Document Source:
-Document Author:
-Document Author:
-Document DOI:
-Document DOI:
-Document URL:
-Document URL:
-Document Citation:
-Document Citation:
-Document References:
-Document Keywords:
-Document Categories:
-Document Type:
-Document: Document.
-Document:
-Document:
-1
-2
-3
-4
-5
-6
-7
-8
-9
-10</t>
+          <t>According to the text, PannEXIN1 channels traffic to the Plasma Membrane, whereas PannExIN2 oligmers localize in intracellar vesicles, specifically early endosomes.</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>10.1038_srep04576.pdf</t>
+          <t>10.1186_1757-2215-6-82.pdf</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>['10.1038_srep04576.pdf', '10.1038_srep04576.pdf', '10.1038_srep04576.pdf', '10.1038_srep04576.pdf', '10.1038_srep04576.pdf']</t>
+          <t>['10.3389_fncel.2014.00468.pdf', '10.1371_journal.pone.0077722.pdf', '10.3389_fphys.2014.00139.pdf', '10.3389_fncel.2014.00468.pdf', '10.3389_fncel.2014.00468.pdf']</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>['through P2Y receptors and by cytoplasmic calcium. FEBS Letters 580, 239–244\n(2006).\n14. Locovei, S., Scemes, E., Qiu, F., Spray, D. C. &amp; Dahl, G. Pannexin1 is part of the\npore forming unit of the P2X(7) receptor death complex. FEBS Lett 581, 483–488\n(2007).\n15. Bao, L., Locovei, S. &amp; Dahl, G. Pannexin membrane channels are\nmechanosensitive conduits for ATP. FEBS Lett 572, 65–68 (2004).\n16. Qiu, F. &amp; Dahl, G. A permeant regulating its permeation pore: inhibition of\npannexin 1 channels by ATP. Am J Physiol Cell Physiol 296, C250–255 (2009).17. Ma, W. H., Hui, H., Pelegrin, P. &amp; Surprenant, A. Pharmacological\nCharacterization of Pannexin-1 Currents Expressed in Mammalian Cells. JPET\n328, 409–418 (2009).\n18. Qiu, F., Wang, J. &amp; Dahl, G. Alanine substitution scanning of pannexin1 reveals\namino acid residues mediating ATP sensitivity. Purinergic Signal 8, 81–90 (2012).\n19. Thompson, R. J., Zhou, N. &amp; MacVicar, B. A. Ischemia opens neuronal gap\njunction hemichannels. Science 312, 924–927 (2006).\n20. Thompson, R. J. et al. Activation of pannexin-1 hemichannels augments aberrant\nbursting in the hippocampus. Science 322, 1555–1559 (2008).\n21. Locovei, S., Bao, L. &amp; Dahl, G. Pannexin 1 in erythrocytes: Function without a gap.\nProc Natl Acad Sci U S A 103, 7655–7659 (2006).\n22. Sridharan, M. et al. Pannexin 1 is the conduit for low oxygen tension-induced ATP\nrelease from human erythrocytes. Am J Physiol Heart Circ Physiol 299,\nH1146–1152 (2010).\n23. Silverman, W., Locovei, S. &amp; Dahl, G. Probenecid, a gout remedy, inhibits\npannexin 1 channels. Am J Physiol Cell Physiol 295, C761–767 (2008).\n24. Bruzzone, R., Barbe, M. T., Jakob, N. J. &amp; Monyer, H. Pharmacological properties\nof homomeric and heteromeric pannexin hemichannels expressed in Xenopus\noocytes. J Neurochem 92, 1033–1043 (2005).\n25. Wang, J., Jackson, D. G. &amp; Dahl, G. The food dye FD&amp;C Blue No. 1 is a selective\ninhibitor of the ATP release channel Panx1. J Gen Physiol 141, 649–656 (2013).', 'oocytes. J Neurochem 92, 1033–1043 (2005).\n25. Wang, J., Jackson, D. G. &amp; Dahl, G. The food dye FD&amp;C Blue No. 1 is a selective\ninhibitor of the ATP release channel Panx1. J Gen Physiol 141, 649–656 (2013).\n26. Dahl, G., Qiu, F. &amp; Wang, J. The bizarre pharmacology of the ATP release channel\npannexin1. Neuropharmacology 75, 583–593 (2013).\n27. Chekeni, F. B. et al. Pannexin 1 channels mediate ‘find-me’ signal release and\nmembrane permeability during apoptosis. Nature 467, 863–867 (2010).\n28. Wang, J. &amp; Dahl, G. SCAM analysis of Panx1 suggests a peculiar pore structure.\nJ Gen Physiol 136, 515–527 (2010).\n29. Bunse, S. et al. Single cysteines in the extracellular and transmembrane regions\nmodulate pannexin 1 channel function. J Membr Biol 244, 21–33 (2011).\n30. Porter, A. G. &amp; Janicke, R. U. Emerging roles of caspase-3 in apoptosis. Cell Death\nDiffer 6, 99–104 (1999).\n31. Santiago, M. F. V. J., Patel, N. K., Lutz, S. E., Caille, D., Charollais, A., Meda, P. &amp;\nScemes, E. Targeting Pannexin1 improves seizure outcome. Plos One 6, e25178\n(2011).\n32. Borgens, R. B. &amp; Liu-Snyder, P. Understanding secondary injury. QR e vB i o l 87,\n89–127 (2012).\n33. Locovei, S., Wang, J. &amp; Dahl, G. Activation of pannexin 1 channels by ATP\nthrough P2Y receptors and by cytoplasmic calcium. FEBS Lett 580, 239–244\n(2006).\n34. Iglesias, R. et al. P2X7 receptor-Pannexin1 complex: pharmacology and signaling.\nAm J Physiol Cell Physiol 295, C752–760 (2008).\n35. Ransford, G. A. et al. Pannexin 1 contributes to ATP release in airway epithelia.\nAm J Respir Cell Mol Biol 41, 525–534 (2009).\n36. Iglesias, R., Dahl, G., Qiu, F., Spray, D. C. &amp; Scemes, E. Pannexin 1: the molecular\nsubstrate of astrocyte ‘‘hemichannels’’ J Neurosci 29, 7092–7097 (2009).\n37. Walsh, J. G., Muruve, D. A. &amp; Power, C. Inflammasomes in the CNS. Nat Rev\nNeurosci (2014).\n38. Qu, Y. et al. Pannexin-1 Is Required for ATP Release during Apoptosis but Not for\nInflammasome Activation. J Immunol 186, 6553–6561 (2011).', 'Here we provide evidence that Pannexin1 is a key molecule that\norchestrates caspase-dependent cell death in response to elevation of\nextracellular K1and ATP concentrations. Athough we have\nrestricted our investigation to the combined effects of ATP and\n[K1]oon Panx1 channels, it is clear that other molecules are also\ninvolved in Panx1-mediated cell death. For instance, glutamate\nreleased from damaged cells stimulates Panx1 through the NMDA\nreceptors (Thompson et al., 2006), and the low oxygen environment\nresulting from obstructed/severed blood vessels and from edema is a\nknown condition that activates Panx1 channels19,21,22.\nPanx1 forms plasma membrane channels that are activated\ndirectly by K1(7) and, through intracellular signaling cascades, by\nATP-sensitive P2 receptors33,34. Activation of Pannexin1 by elevated\nextracellular [K1] has been reported to induce caspase-1 activation\nand IL-1 brelease7and to release ATP11,15,21,35. The potentially dele-\nterious consequences of ATP-mediated cell death by hyperactivation\nof the innate immune response via such a Panx1 positive feedback\nFigure 7 |AnnexinV staining in astrocytes. (Top) Examples of epifluorescence images of cultured WT astrocytes treated for 1–2 hr with 2.5 and 10 mM\nK1- ACSF showing staining for Annexin V (green) and Dapi (red). (Bottom) Mean 6s.e.m. values of Annexin V fluorescence per total number of nuclei\n(left) and the mean 6s.e.m. fold changes in Annexin V (right) obtained for WT and Panx1 KO exposed to 2.5 mM K1-ACSF and to 10 mM K1-ACSF in\nthe absence and presence of 300 mM BzATP. In parentheses are the number of images used for measurements that were obtained from 2 Panx1KO and 3\nWT mice. Note that although not significant, there was a slight increase in Annexin V as measured in WT astrocytes exposed to 10 mM K1-ACSF. To\navoid any bias, we measured total fluorescence and divided by cell number. This procedure results in an underestimation of K 1-induced cell death', '37. Walsh, J. G., Muruve, D. A. &amp; Power, C. Inflammasomes in the CNS. Nat Rev\nNeurosci (2014).\n38. Qu, Y. et al. Pannexin-1 Is Required for ATP Release during Apoptosis but Not for\nInflammasome Activation. J Immunol 186, 6553–6561 (2011).\n39. Dahl, G. The Xenopus oocyte cell-cell channel assay for functional analysis of gap\njunction proteins., in Cell-cell interactions. A practical approach. (eds. Stevenson,\nB., Gallin, W. &amp; Paul, D.) 143–165 (IRL, Oxford; 1992).\n40. Dahl, G. &amp; Pfahnl, A. Mutagenesis to study channel structure. Methods Mol Biol\n154, 251–268 (2001).\n41. Dahl, G. &amp; Keane, R. W. Pannexin: From discovery to bedside in 11 1/24 years?\nBrain Res 1487 , 150–159 (2012).\nAcknowledgments\nWe thank Naman K. Patel for animal care and astrocyte cell culture. Work reported here\nwas supported by a grant from the Craig Nielsen Foundation. We also thank our home\ninstitutions for additional support.\nAuthor contributions\nG.D., E.S. and R.W.K. designed research; D.G.J., J.W.and E.S. performed research; E.S.,\nD.G.J., J.W. and G.D. analyzed data; and G.D., E.S. and R.W.K. wrote the paper.\nAdditional information\nCompeting financial interests : The authors declare no competing financial interests.\nHow to cite this article: Jackson, D.G., Wang, J.J., Keane, R.W., Scemes, E. &amp; Dahl, G. ATP\nand potassium ions: a deadly combination for astrocytes. Sci. Rep. 4, 4576; DOI:10.1038/\nsrep04576 (2014).\nThis work is licensed under a Creative Commons Attribution-NonCommercial-\nShareAlike 3.0 Unported License. The images in this article are included in the\narticle’s Creative Commons license, unless indicated otherwise in the image credit;\nif the image is not included under the Creative Commons license, users will need to\nobtain permission from the license holder in order to reproduce the image. To view a\ncopy of this license, visit http://creativecommons.org/licenses/by-nc-sa/3.0/\nwww.nature.com/ scientificreports\nSCIENTIFIC REPORTS | 4 : 4576 | DOI: 10.1038/srep04576 9', 'inhibitor25, was attenuated in a [K1]odose-dependent manner\n(Figure 3). Considering, that the putative binding sites for ATP\nand BB FCF overlap25, it seems plausible that the putative binding\nsites of K1and BzATP on Panx1 channels overlap as well. However,\nit cannot be excluded that K1affects the ATP binding site\nallosterically.\nPanx1 activation, a path to cell death? The Panx1 membrane\nprotein exhibits a long stretch of amino acids at the carboxytermi-\nnus that is located at the cytoplasmic surface of the plasma\nmembrane. Truncation of carboxy-terminal sequences was typi-\ncally tolerated, basic channel functions remained preserved, as\nobserved for Panx1 359stop or Panx1 408stop, for example. When\nexpressed in oocytes, both mutants yielded currents similar in\namplitude as wtPanx1 and sensitivity to Panx1 inhibitors, such as\ncarbenoxolone, was preserved (Figure 4a). Only when Panx1 was\ntruncated at position 378 to mimic cleavage of the protein by\ncaspase-327were the gating properties altered. The channel became\nconstitutively active and the rectification prominently seen with\nwtPanx1 was absent (Figure 4b). As a consequence, the cells\nexpressing this truncation mutant died when incubated for\n.12 hours. Although the Panx1 inhibitors carbenoxolone (CBX)\nor Probenecid efficiently inhibited currents mediated by Panx1\nFigure 2 |Quantitative analysis of inhibition of Panx1 currents by ATP\nor BzATP at different K1concentrations. (a) In normal Ringer solution\n(1 mM K1), 500 mM ATP inhibited voltage-induced currents. With the\nsame ATP concentration, currents induced by K1were minimally affected\n(10 mM [K1]o) or not at all (42.5 mM [K1]o). BzATP (300 mM) was\neffectively inhibiting at 40 mM [K1]o, but not at 75 mM. (b) Competition\nbetween BzATP and K1.A t4 0m M[ K1]o, increasing the BzATP\nconcentration restored the inhibitory capacity of this compound.\nIncreasing the [K1]oto 75 mM eliminated the inhibitory effect of even\n300mM BzATP.']</t>
+          <t>['ORIGINAL RESEARCH ARTICLE\npublished: 02 February 2015\ndoi: 10.3389/fncel.2014.00468\nPannexin2 oligomers localize in the membranes of\nendosomal vesicles in mammalian cells while Pannexin1channels trafﬁc to the plasma membrane\nDaniela Boassa1*, Phuong Nguyen1, Junru Hu1, Mark H. Ellisman1,2and Gina E. Sosinsky1,2*\n1National Center for Microscopy and Imaging Research, Center for Research in Biological Systems, University of California, San Diego, La Jolla, CA, U SA\n2Department of Neurosciences, University of California, San Diego, La Jolla, CA, USA\nEdited by:\nJuan Andrés Orellana, Pontiﬁcia\nUniversidad Católica de Chile, Chile\nReviewed by:\nLilian Irene Plotkin, Indiana\nUniversity School of Medicine, USA\nManuel Antonio Riquelme,\nUniversity of Texas Health ScienceCenter at San Antonio, USA\nVeronica Abudara, Universidad de la\nRepública, Uruguay\n*Correspondence:\nDaniela Boassa and Gina E.\nSosinsky, National Center for\nMicroscopy and Imaging Research,\nSchool of Medicine, University ofCalifornia, San Diego, BSB 1000,\n9500 Gilman Drive, MC 0608,\nLa Jolla, CA 92093-0608, USAe-mail: dboassa@ucsd.edu;\ngsosinsky@ucsd.eduPannexin2 (Panx2) is the largest of three members of the pannexin proteins. Pannexins\nare topologically related to connexins and innexins, but serve different functional roles than\nforming gap junctions. We previously showed that pannexins form oligomeric channels butunlike connexins and innexins, they form only single membrane channels. High levels of\nPanx2 mRNA and protein in the Central Nervous System (CNS) have been documented.\nWhereas Pannexin1 (Panx1) is fairly ubiquitous and Pannexin3 (Panx3) is found in skinand connective tissue, both are fully glycosylated, trafﬁc to the plasma membrane and\nhave functions correlated with extracellular ATP release. Here, we describe trafﬁcking\nand subcellular localizations of exogenous Panx2 and Panx1 protein expression in MDCK,HeLa, and HEK 293T cells as well as endogenous Panx1 and Panx2 patterns in the', 'vivo.\nUnique glycosylation of drPanx1b affects localization in\nvitro\nThe subcellular localization of Panx1 proteins was analyzed\nin transiently transfected mouse Neuroblastoma 2a (N2a) cells\nexpressing C-terminally EYFP-tagged Panx1 fusion proteins,\ncontaining the full coding regions of either drPanx1b\n(aa 1-422), drPanx1a (aa 1-417) or mPanx1 (aa 1-426).\nmPanx1 is the best characterized pannexin protein and served\nas reference protein for subsequent experiments. In N2a cells,\ndrPanx1b, mPanx1, and especially drPanx1a are prominently\nlocalized in the plasma membrane 48 h post transfection\n(Figure 3A ). drPanx1b and mPanx1 were located in the plasma\nmembrane and perinuclear region, whereas drPanx1a was\nmainly found in the cell membrane. Fluorescent aggregates,\nmost pronounced for drPanx1b, potentially reflected rate\nlimiting steps and/or local accumulation during the life cycle of\nthese proteins. Similar to drPanx1a [ 10], drPanx1b does not\nshow gap junction-like assemblies in the plasma membrane,\nsuggesting that drPanx1b, like mPanx1 and drPanx1a,\npreferentially forms unopposed membrane channels. The\ndistributions of the three constructs by confocal imaging are\nconsistent with previous reports demonstrating a plasma\nmembrane expression for Panx1 [10,11,24,25].\nSince the anti-drPanx1b antibody was unsuitable for western\nblot, EYFP tagged Panx1 protein expression was used to\nreveal post-translational modifications using an antibody\nspecific for EYFP detection. Consistent with previous studies\nreporting N-glycosylation sites in EL2 at N254 for mPanx1 orN246 for drPanx1a [ 10,11,25–27 ], we confirmed the Panx1-\nspecific band pattern corresponding to the unmodified Gly0\ncore proteins, high mannose Gly1 species and complex\nglycosylated Gly2 species (Figure 3B). The pattern for\ndrPanx1b was more complex, showing motilities different from\nthe calculated MW of 76.6 kDa for the fusion protein, indicating\nmore extensive post-translational modifications.', 'Cea et al. Panx1 in skeletal muscles\nkidney, prostate, and small intestine, and low to almost unde-\ntectable levels are found in lung, liver, pancreas, spleen, colon,and peripheral blood ( Baranova et al., 2004 ). The pattern of\nexpression of the other two Panxs is completely different; Panx2is preferentially expressed in brain ( Baranova et al., 2004 )a n d\nPanx3, mostly expressed in bone and skin ( Sandilos and Bayliss,\n2012 ). Panx1 channels are oligomeric structures formed by 6\nsubunits of Panx1 protein ( Boassa et al., 2007 ). Panx1 shows\nsimilar membrane topology than Cxs and is characterized byfour transmembrane (TM) segments, two extracellular loops, andcytoplasmic localization of both amino and C-termini. Panxs 1and 3 are glycoproteins, unlike Cxs that are not glycosylated. Ithas been proposed that glycosylation of Panxs prevents forma-tion of gap junction channels ( Boassa et al., 2008 ). Panx1 and\nPanx3 suffer N-linked glycosylation at Asp254 present in the sec-ond extracellular loop and Asp71 found at the ﬁrst extracellularloop, respectively. However, a fraction of Panx1 mutant that is notglycosylated still trafﬁcs to the cell surface, suggesting that Panx1glycosylated protein could interact and form channels with ung-lycosylated forms and/or that the unglycosylated Panx1 fractionforms gap junction channel-like structures ( Penuela et al., 2009 ).\nStructural analyses of the lining residues of the Panx1 pore\nusing the substituted cysteine accessibility method (SCAM) haverevealed that the TM1 region and domains of the ﬁrst extracellu-lar loop (E1) are exposed to the channel lumen. Also, C-terminalamino acids substitution and reagent perturbation suggest thecontribution of this segment to the permeation pathway ( Wang\nand Dahl, 2010 ). Panx1 channels activated by positive membrane\npotentials show several substates. The full open state presents acharacteristically high conductan ce in different cell types includ-', 'and subcellular localizations of exogenous Panx2 and Panx1 protein expression in MDCK,HeLa, and HEK 293T cells as well as endogenous Panx1 and Panx2 patterns in the\nCNS. Panx2 was found in intracellular localizations, was partially N-glycosylated, and\nlocalizations were non-overlapping with Panx1 . Confocal images of hippocampal sectionsimmunolabeled for the astrocytic protein GFAP , Panx1 and Panx2 demonstrated that the\ntwo isoforms, Panx1 and Panx2, localized at different subcellular compartments in both\nastrocytes and neurons. Using recombinant fusions of Panx2 with appended genetic tags\ndeveloped for correlated light and electron microscopy and then expressed in different cell\nlines, we determined that Panx2 is localized in the membrane of intracellular vesiclesand not in the endoplasmic reticulum as initially indicated by calnexin colocalization\nexperiments. Dual immunoﬂuorescence imaging with protein markers for speciﬁc vesicle\ncompartments showed that Panx2 vesicles are early endosomal in origin. In electrontomographic volumes, cross-sections of these vesicles displayed ﬁne structural details\nand close proximity to actin ﬁlaments. Thus, pannexins expressed at different subcellular\ncompartments likely exert distinct functional roles, particularly in the nervous system.\nKeywords: pannexin channels, ATP signaling, tetracysteine tag, miniSOG, correlated light and electron\nmicroscopy, electron tomography, intercellular communication, connexin\nINTRODUCTION\nThe pannexins (Panx1, Panx2, and Panx3) are unique entities in\nthe “connexin-like” family of proteins. These three membraneproteins are topologically similar to innexins (invertebrate gapjunction proteins) (Panchin et al., 2000; Locovei et al., 2006a )\nwith some sequence similarities, but function as single membranechannels (pannexons) in mammals ( Locovei et al., 2006a ). As\nshown in Figure 1A , the hallmarks of this folding topology are', 'analysis in light microscopy. J. Microsc. 224, 213–232. doi: 10.1111/j.1365-\n2818.2006.01706.x\nBoyce, A. K., Prager, R. T., Wicki-Stordeur, L. E., and Swayne, L. A. (2014).\nPore positioning: current concepts in Pannexin channel trafﬁcking. Channels\n(Austin). 8, 110–117. doi: 10.4161/chan.27287\nBruzzone, R., Hormuzdi, S. G., Barbe, M. T., Herb, A., and Monyer, H. (2003).\nPannexins, a family of gap junction proteins expressed in brain. Proc. Natl. Acad.\nSci. U.S.A. 100, 13644–13649. doi: 10.1073/pnas.2233464100\nBurns, A. R., Phillips, S. C., and Sokoya, E. M. (2012). Pannexin protein\nexpression in the rat middle cerebral artery. J. Vasc. Res. 49, 101–110. doi:\n10.1159/000332329\nBushong, E. A., Martone, M. E., Jones, Y. Z., and Ellisman, M. H. (2002).\nProtoplasmic astrocytes in CA1 stratum radiatum occupy separate anatomical\ndomains. J. Neurosci. 22, 183–192.\nChekeni, F. B., Elliott, M. R., Sandilos, J. K., Walk, S. F., Kinchen, J. M., Lazarowski,\nE. R., et al. (2010). Pannexin 1 channels mediate ‘ﬁnd-me’ signal release\nand membrane permeability during apoptosis. Nature 467, 863–867. doi:\n10.1038/nature09413\nCone, A. C., Ambrosi, C., Scemes, E., Martone, M. E., and Sosinsky, G. E. (2013).\nA comparative antibody analysis of pannexin1 expression in four rat brain\nregions reveals varying subcellular localizations. Front. Pharmacol. 4:6. doi:\n10.3389/fphar.2013.00006\nDell’Angelica, E. C., Ohno, H., Ooi, C. E., Rabinovich, E., Roche, K. W., and\nBonifacino, J. S. (1997). AP-3: an adaptor-like protein complex with ubiquitousexpression. EMBO J. 16, 917–928. doi: 10.1093/emboj/16.5.917\nDe Matteis, M. A., and Luini, A. (2008). Exiting the Golgi complex. Nat. Rev. Mol.\nCell Biol. 9, 273–284. doi: 10.1038/nrm2378\nD’Hondt, C., Ponsaerts, R., De Smedt, H., Vinken, M., De Vuyst, E., De Bock, M.,\net al. (2011). Pannexin channels in ATP release and beyond: an unexpected\nFrontiers in Cellular Neuroscience www.frontiersin.org February 2015 | Volume 8 | Article 468 |13']</t>
         </is>
       </c>
     </row>
@@ -1122,59 +882,15 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Context: [Document 7], [Document...
-#### Context:
-[...]
-#### Answer:
-Based on the provided context, the currently known
-mito- chondrial diseases attributed to
-POL G mutations are:
-1. Autosomal recessi ve progressive external opthalmopleg ia
-2. Mitochon-
-drial neuro-gastrointestinal enc ephalo-myopathy ( MNG I E)
-#### Explanation:
-The documents provided describe the association of POL G
-mutations with progressive extern al ophthalmoplegi a and MNGI E.
-Document 8 reports that POL G mutations have been found in
-patients with MNG IE, while Document 2 and Document 4
-describe the association with autosomal domin ant or recessi-
-ve progressive external opphthalmople gi a. The clinical
-features described in these documents, including PEO, axonal
-sensory neuropathy,
-sens ory ataxi a, cardiomyopathy,
-retinopathy,
-sensorineural heari ng loss,
-thalam ic lesions,
-mus cle dystrophy,
-facial diplegi a,
-dysartri a,
-and dysphagi a, are consistent with the clinical presentation
-of both diseases. Therefore, it can be concluded that POLG
-mutations are associated with both autosomal rec essive
-progressi ve extern al opthalmop le gi a and mito chond rial
-neur o-gast ro-intest in al enc e phalo-my op athy ( M NG I E).
-[Document
-[...]
-#### References:
-[1] Zevian i, Servid e i, G ellera, B ertini, DiM aur o, DiDo nat o
-S : An autosom al domin ant disorder with mult i ple delet ions
-of mitochond rial DNA starting a t the D-lo o p region. Nat ure
-1989;339:309–3 11.
-[2] Kauk o n e n, J usel i us JK, T iranti V
-et al: R ole of aden in e nucleotide transloca tor 1
-in mtDNA main t enance. Sci ence 200 0;289:782– 785.
-[...]. (more) (less)
-#### Relevant
-References:
-1 Z evian i M, S ervid e
-S, G elle ra C, B er tini E
-D iMa ur o S,
-D</t>
+          <t>Based on the context, POLG (mitochondial DNA polymerases gamma) mutations have been associated with the following mitochondrial diseases:
+1. Progressive external ophyhalmoplegic (PEo) with multiple mitochondrial DNA (mtDNA) deletions.
+2. Mitochndrial neuro-gastrointestinal-encephalomopathy (MNIE), which is an autosomally recessive disease characterized by PEO, multiple mt DNA deletitions, and gastrointestinal manifestations.
+These findings indicate that POLG sequence analysis should be considered in patients presenting with features of MNIE but without thymidne phosphorylases (TP) mutations.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>10.1038_sj.ejhg.5201002.pdf</t>
+          <t>10.3892_or.2012.1625.pdf</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">

</xml_diff>